<commit_message>
ur user profile are updated
</commit_message>
<xml_diff>
--- a/Form SpecificationsV0.1_DRAFT.xlsx
+++ b/Form SpecificationsV0.1_DRAFT.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="110">
   <si>
     <t xml:space="preserve"> Specifications Author:</t>
   </si>
@@ -365,6 +365,15 @@
   </si>
   <si>
     <t xml:space="preserve">Date of Birth </t>
+  </si>
+  <si>
+    <t xml:space="preserve">settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sign out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Help</t>
   </si>
   <si>
     <t xml:space="preserve">demographic page</t>
@@ -2039,10 +2048,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2289,10 +2298,10 @@
     </row>
     <row r="11" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="34" t="s">
         <v>89</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>90</v>
       </c>
       <c r="C11" s="45"/>
       <c r="D11" s="28"/>
@@ -2308,10 +2317,10 @@
     </row>
     <row r="12" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="44" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C12" s="45"/>
       <c r="D12" s="28"/>
@@ -2327,10 +2336,10 @@
     </row>
     <row r="13" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="44" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C13" s="45"/>
       <c r="D13" s="28"/>
@@ -2346,7 +2355,7 @@
     </row>
     <row r="14" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="44" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B14" s="34" t="s">
         <v>93</v>
@@ -2365,7 +2374,7 @@
     </row>
     <row r="15" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="44" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B15" s="34" t="s">
         <v>94</v>
@@ -2383,11 +2392,11 @@
       <c r="M15" s="18"/>
     </row>
     <row r="16" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="34" t="s">
         <v>95</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>96</v>
       </c>
       <c r="C16" s="45"/>
       <c r="D16" s="28"/>
@@ -2402,11 +2411,11 @@
       <c r="M16" s="18"/>
     </row>
     <row r="17" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="34" t="s">
-        <v>97</v>
+      <c r="A17" s="44" t="s">
+        <v>92</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C17" s="45"/>
       <c r="D17" s="28"/>
@@ -2421,11 +2430,11 @@
       <c r="M17" s="18"/>
     </row>
     <row r="18" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="34" t="s">
         <v>97</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>99</v>
       </c>
       <c r="C18" s="45"/>
       <c r="D18" s="28"/>
@@ -2441,10 +2450,10 @@
     </row>
     <row r="19" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C19" s="45"/>
       <c r="D19" s="28"/>
@@ -2463,7 +2472,7 @@
         <v>100</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C20" s="45"/>
       <c r="D20" s="28"/>
@@ -2479,10 +2488,10 @@
     </row>
     <row r="21" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="34" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C21" s="45"/>
       <c r="D21" s="28"/>
@@ -2501,7 +2510,7 @@
         <v>103</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C22" s="45"/>
       <c r="D22" s="28"/>
@@ -2520,7 +2529,7 @@
         <v>103</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23" s="45"/>
       <c r="D23" s="28"/>
@@ -2535,8 +2544,12 @@
       <c r="M23" s="18"/>
     </row>
     <row r="24" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
+      <c r="A24" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>107</v>
+      </c>
       <c r="C24" s="45"/>
       <c r="D24" s="28"/>
       <c r="E24" s="28"/>
@@ -2548,6 +2561,59 @@
       <c r="K24" s="34"/>
       <c r="L24" s="19"/>
       <c r="M24" s="18"/>
+    </row>
+    <row r="25" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="45"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="18"/>
+    </row>
+    <row r="26" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="45"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="34"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="18"/>
+    </row>
+    <row r="27" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="34"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="18"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>

</xml_diff>

<commit_message>
receive ur user profile updted
</commit_message>
<xml_diff>
--- a/Form SpecificationsV0.1_DRAFT.xlsx
+++ b/Form SpecificationsV0.1_DRAFT.xlsx
@@ -1,44 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/FabstechTZ/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="0" windowWidth="21820" windowHeight="13440" tabRatio="500" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Approval" sheetId="1" r:id="rId1"/>
-    <sheet name="Example" sheetId="2" r:id="rId2"/>
-    <sheet name="Example 2" sheetId="3" r:id="rId3"/>
-    <sheet name="Functional Specs" sheetId="4" r:id="rId4"/>
+    <sheet name="Approval" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Example" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Example 2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Functional Specs" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Example!$A$1:$M$6</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Example 2'!$A$1:$M$10</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Functional Specs'!$A$1:$M$5</definedName>
-    <definedName name="Print_Area_0" localSheetId="1">Example!$A$1:$M$6</definedName>
-    <definedName name="Print_Area_0" localSheetId="2">'Example 2'!$A$1:$M$10</definedName>
-    <definedName name="Print_Area_0" localSheetId="3">'Functional Specs'!$A$1:$M$5</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">Example!$A:$B,Example!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Example 2'!$A:$B,'Example 2'!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="3">'Functional Specs'!$A:$B,'Functional Specs'!$1:$1</definedName>
-    <definedName name="Print_Titles_0" localSheetId="1">Example!$A:$B,Example!$1:$1</definedName>
-    <definedName name="Print_Titles_0" localSheetId="2">'Example 2'!$A:$B,'Example 2'!$1:$1</definedName>
-    <definedName name="Print_Titles_0" localSheetId="3">'Functional Specs'!$A:$B,'Functional Specs'!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Example!$A$1:$M$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">Example!$A:$B,Example!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'Example 2'!$A$1:$M$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles" vbProcedure="false">'Example 2'!$A:$B,'Example 2'!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Functional Specs'!$A$1:$M$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Titles" vbProcedure="false">'Functional Specs'!$A:$B,'Functional Specs'!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="Print_Area_0" vbProcedure="false">Example!$A$1:$M$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="Print_Titles_0" vbProcedure="false">Example!$A:$B,Example!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Example!$A$1:$M$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">Example!$A:$B,Example!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="Print_Area_0" vbProcedure="false">'Example 2'!$A$1:$M$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="Print_Titles_0" vbProcedure="false">'Example 2'!$A:$B,'Example 2'!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'Example 2'!$A$1:$M$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles" vbProcedure="false">'Example 2'!$A:$B,'Example 2'!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="Print_Area_0" vbProcedure="false">'Functional Specs'!$A$1:$M$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="Print_Titles_0" vbProcedure="false">'Functional Specs'!$A:$B,'Functional Specs'!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Functional Specs'!$A$1:$M$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Titles" vbProcedure="false">'Functional Specs'!$A:$B,'Functional Specs'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -47,15 +43,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="113">
   <si>
     <t xml:space="preserve"> Specifications Author:</t>
   </si>
   <si>
-    <t>Mwombeki Fabian</t>
-  </si>
-  <si>
-    <t>Project Manager</t>
+    <t xml:space="preserve">Mwombeki Fabian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Manager</t>
   </si>
   <si>
     <t xml:space="preserve">                                                </t>
@@ -64,74 +60,74 @@
     <t xml:space="preserve">                                          </t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Signature</t>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signature</t>
   </si>
   <si>
     <t xml:space="preserve">Date </t>
   </si>
   <si>
-    <t>(DD-MMM-YYYY)</t>
-  </si>
-  <si>
-    <t>Reviewer:</t>
-  </si>
-  <si>
-    <t>Savannah Informatics Form Designer</t>
-  </si>
-  <si>
-    <t>Savannah Informatics Form Designer, Programmer</t>
-  </si>
-  <si>
-    <t>Form/Page</t>
-  </si>
-  <si>
-    <t>Question</t>
-  </si>
-  <si>
-    <t>Field Name (form designer to complete)</t>
-  </si>
-  <si>
-    <t>Response on PDF</t>
-  </si>
-  <si>
-    <t>Database Value</t>
-  </si>
-  <si>
-    <t>Field Type
+    <t xml:space="preserve">(DD-MMM-YYYY)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reviewer:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Savannah Informatics Form Designer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Savannah Informatics Form Designer, Programmer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Form/Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field Name (form designer to complete)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response on PDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field Type
 (Check Box, Radio Button, Text Field, Scale, Dropdown, etc.)</t>
   </si>
   <si>
-    <t>Field Validation</t>
-  </si>
-  <si>
-    <t>Format
+    <t xml:space="preserve">Field Validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Format
 (Text, Numeric, Date)</t>
   </si>
   <si>
-    <t>Required
+    <t xml:space="preserve">Required
 (Y/N)</t>
   </si>
   <si>
-    <t>Condition(s)</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>Display in Site Console
+    <t xml:space="preserve">Condition(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display in Site Console
 (Max 40 of Characters)</t>
   </si>
   <si>
-    <t>Other (Calculation, hidden fields)</t>
-  </si>
-  <si>
-    <t>Cover page</t>
+    <t xml:space="preserve">Other (Calculation, hidden fields)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cover page</t>
   </si>
   <si>
     <t xml:space="preserve">Cover page will display after authentication to form before first assessment at each Visit (Cycle).
@@ -147,13 +143,13 @@
 </t>
   </si>
   <si>
-    <t>NA, not enterable</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Prepopulated</t>
+    <t xml:space="preserve">NA, not enterable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prepopulated</t>
   </si>
   <si>
     <t xml:space="preserve">Study ID
@@ -168,77 +164,77 @@
     <t xml:space="preserve">Training </t>
   </si>
   <si>
-    <t>I prefer the colour</t>
-  </si>
-  <si>
-    <t>Training_Q1</t>
-  </si>
-  <si>
-    <t>Red, Blue</t>
-  </si>
-  <si>
-    <t>1
+    <t xml:space="preserve">I prefer the colour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training_Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red, Blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1
 2</t>
   </si>
   <si>
-    <t>Radio Button</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>One must be selected</t>
-  </si>
-  <si>
-    <t>Page Navigation Arrows</t>
+    <t xml:space="preserve">Radio Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One must be selected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page Navigation Arrows</t>
   </si>
   <si>
     <t xml:space="preserve">Previous </t>
   </si>
   <si>
-    <t>Previous + page #</t>
-  </si>
-  <si>
-    <t>Button</t>
-  </si>
-  <si>
-    <t>If tapped</t>
-  </si>
-  <si>
-    <t>Prior page will display</t>
-  </si>
-  <si>
-    <t>Next</t>
-  </si>
-  <si>
-    <t>Next + page #</t>
-  </si>
-  <si>
-    <t>Next page will display</t>
-  </si>
-  <si>
-    <t>Pagination</t>
-  </si>
-  <si>
-    <t>ALL</t>
-  </si>
-  <si>
-    <t>Pages in a Cycle will be paginated as page x of y from the first page in the cycle to the last so patients have a concept of how far they've completed a cycle.</t>
-  </si>
-  <si>
-    <t>Response on Site</t>
-  </si>
-  <si>
-    <t>PAISs</t>
-  </si>
-  <si>
-    <t>PAISS Instruction Set 1</t>
-  </si>
-  <si>
-    <t>PAISs Instruction Set 2</t>
-  </si>
-  <si>
-    <t>Q1a
+    <t xml:space="preserve">Previous + page #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If tapped</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prior page will display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Next</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Next + page #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Next page will display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pagination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pages in a Cycle will be paginated as page x of y from the first page in the cycle to the last so patients have a concept of how far they've completed a cycle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response on Site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAISs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAISS Instruction Set 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAISs Instruction Set 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1a
 Q1b
 Q2a
 Q2b
@@ -254,7 +250,7 @@
 Q5d</t>
   </si>
   <si>
-    <t>PAISs_UBS_Gripping
+    <t xml:space="preserve">PAISs_UBS_Gripping
 PAISs_UBS_Lifting
 PAISs_LBS_Standing
 PAISs_LBS_Climbing
@@ -270,10 +266,10 @@
 PAISs_END_WlkIncline</t>
   </si>
   <si>
-    <t>0-No Difficulty, 1, 2, 3, 4, 5, 6, 7, 8, 0, 10-Unable to do</t>
-  </si>
-  <si>
-    <t>1
+    <t xml:space="preserve">0-No Difficulty, 1, 2, 3, 4, 5, 6, 7, 8, 0, 10-Unable to do</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1
 2
 3
 4
@@ -286,159 +282,172 @@
 11</t>
   </si>
   <si>
-    <t>All Questions on Form</t>
-  </si>
-  <si>
-    <t>I see the question but choose not to answer it</t>
-  </si>
-  <si>
-    <t>Fieldname + "NA"</t>
-  </si>
-  <si>
-    <t>Checked or unchecked</t>
-  </si>
-  <si>
-    <t>If checked, value is 1
+    <t xml:space="preserve">All Questions on Form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I see the question but choose not to answer it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fieldname + "NA"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checked or unchecked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If checked, value is 1
 If unchecked, value if "Off"</t>
   </si>
   <si>
-    <t>Y, if none of the other answers are selected</t>
-  </si>
-  <si>
-    <t>If checked</t>
-  </si>
-  <si>
-    <t>Satisfies required response</t>
-  </si>
-  <si>
-    <t>Refused</t>
-  </si>
-  <si>
-    <t>Field is hidden unless question is left blank upon submit.</t>
-  </si>
-  <si>
-    <t>Last Page of Form</t>
-  </si>
-  <si>
-    <t>By checking the box below I confirm that the answers I have provided are accurate</t>
-  </si>
-  <si>
-    <t>Form_Confirm</t>
-  </si>
-  <si>
-    <t>Check Box</t>
-  </si>
-  <si>
-    <t>Upon Submit, all required questions left blank will display “I see the question but choose not to answer it”</t>
-  </si>
-  <si>
-    <t>Confirmed</t>
+    <t xml:space="preserve">Y, if none of the other answers are selected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If checked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Satisfies required response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refused</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field is hidden unless question is left blank upon submit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Page of Form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">By checking the box below I confirm that the answers I have provided are accurate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Form_Confirm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upon Submit, all required questions left blank will display “I see the question but choose not to answer it”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirmed</t>
   </si>
   <si>
     <t xml:space="preserve">Response on portal </t>
   </si>
   <si>
-    <t>log in page</t>
+    <t xml:space="preserve">log in page</t>
   </si>
   <si>
     <t xml:space="preserve">sign in </t>
   </si>
   <si>
-    <t>Password tab</t>
-  </si>
-  <si>
-    <t>Linked in Sign in addnon</t>
-  </si>
-  <si>
-    <t>Facebook sign in addon</t>
+    <t xml:space="preserve">Password tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linked in Sign in addnon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facebook sign in addon</t>
   </si>
   <si>
     <t xml:space="preserve">user profile </t>
   </si>
   <si>
-    <t>user name</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last name</t>
-  </si>
-  <si>
-    <t>Email address</t>
+    <t xml:space="preserve">user name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email address</t>
   </si>
   <si>
     <t xml:space="preserve">Date of Birth </t>
   </si>
   <si>
-    <t>demographic page</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>Company name</t>
-  </si>
-  <si>
-    <t>Employers/post job</t>
-  </si>
-  <si>
-    <t>post job</t>
-  </si>
-  <si>
-    <t>registration</t>
-  </si>
-  <si>
-    <t>learn about posting a job</t>
-  </si>
-  <si>
-    <t>Sir name</t>
-  </si>
-  <si>
-    <t>photo</t>
-  </si>
-  <si>
-    <t>First name</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Education Page</t>
-  </si>
-  <si>
-    <t>Find jobs- which job</t>
-  </si>
-  <si>
-    <t>Search Page</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Find Salaries - job title</t>
-  </si>
-  <si>
-    <t>Name of school</t>
+    <t xml:space="preserve">Help</t>
+  </si>
+  <si>
+    <t xml:space="preserve">settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sign out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demographic page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sir name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Education Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of school</t>
   </si>
   <si>
     <t xml:space="preserve">Course taken </t>
   </si>
   <si>
-    <t>Year Graduated</t>
-  </si>
-  <si>
-    <t>Award given</t>
+    <t xml:space="preserve">Year Graduated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Award given</t>
+  </si>
+  <si>
+    <t xml:space="preserve">level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find jobs- which job</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find Salaries - job title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employers/post job</t>
+  </si>
+  <si>
+    <t xml:space="preserve">post job</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">learn about posting a job</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="D\-MMM"/>
+  </numFmts>
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -447,9 +456,97 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -461,28 +558,28 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="18"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -502,7 +599,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Times New Roman"/>
@@ -531,7 +628,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -539,12 +636,48 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -571,208 +704,341 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
-    <border>
+  <borders count="6">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF808080"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF808080"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF808080"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+  <cellStyleXfs count="36">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+  <cellXfs count="46">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="22">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -831,311 +1097,40 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" customWidth="1"/>
-    <col min="6" max="1025" width="8.83203125" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.83"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23" x14ac:dyDescent="0.25">
+    <row r="1" customFormat="false" ht="23" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="1"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" customFormat="false" ht="30.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1152,7 +1147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
         <v>5</v>
@@ -1167,7 +1162,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -1176,42 +1171,42 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" customFormat="false" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1226,7 +1221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6"/>
       <c r="B11" s="7" t="s">
         <v>5</v>
@@ -1241,7 +1236,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1250,28 +1245,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="13"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>10</v>
       </c>
@@ -1286,7 +1281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6"/>
       <c r="B19" s="7" t="s">
         <v>5</v>
@@ -1301,7 +1296,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1310,7 +1305,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -1318,9 +1313,10 @@
       <c r="E21" s="13"/>
     </row>
   </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="1" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Bold"&amp;12Novartis_BYM338E2202_Global Phase II
 WR myPROpad Setup Specifications
 &amp;A&amp;R&amp;"Times New Roman,Bold"&amp;10Version DRAFT 1.0</oddHeader>
@@ -1330,34 +1326,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <pageSetUpPr fitToPage="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="17" customWidth="1"/>
-    <col min="4" max="5" width="20.33203125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="18" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="18" customWidth="1"/>
-    <col min="10" max="10" width="14" style="19" customWidth="1"/>
-    <col min="11" max="11" width="24.1640625" style="20" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" style="20" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="13" style="18" hidden="1" customWidth="1"/>
-    <col min="14" max="1025" width="21.6640625" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="16" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="17" width="23.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="18" width="20.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="16" width="13.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="16" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="18" width="12.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="18" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="19" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="20" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="20" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="18" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="21.67"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="24" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" s="24" customFormat="true" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
         <v>13</v>
       </c>
@@ -1398,7 +1394,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="32" customFormat="1" ht="91" x14ac:dyDescent="0.2">
+    <row r="2" s="32" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
         <v>26</v>
       </c>
@@ -1439,7 +1435,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="32" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" s="32" customFormat="true" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
         <v>33</v>
       </c>
@@ -1476,8 +1472,8 @@
       <c r="L3" s="30"/>
       <c r="M3" s="31"/>
     </row>
-    <row r="4" spans="1:13" s="35" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="46" t="s">
+    <row r="4" s="35" customFormat="true" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="28" t="s">
         <v>41</v>
       </c>
       <c r="B4" s="33" t="s">
@@ -1517,8 +1513,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="35" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="46"/>
+    <row r="5" s="35" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="28"/>
       <c r="B5" s="33" t="s">
         <v>47</v>
       </c>
@@ -1556,7 +1552,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="37" customFormat="1" ht="65" x14ac:dyDescent="0.2">
+    <row r="6" s="37" customFormat="true" ht="65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="28" t="s">
         <v>50</v>
       </c>
@@ -1597,10 +1593,10 @@
   <mergeCells count="1">
     <mergeCell ref="A4:A5"/>
   </mergeCells>
-  <printOptions horizontalCentered="1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="1" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="0" pageOrder="overThenDown" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Bold"&amp;12Novartis_BYM338E2202_Global Phase II
 WR myPROpad Setup Specifications
 &amp;A&amp;R&amp;"Times New Roman,Bold"&amp;10Version DRAFT 1.0</oddHeader>
@@ -1611,34 +1607,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <pageSetUpPr fitToPage="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="17" customWidth="1"/>
-    <col min="4" max="5" width="20.33203125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="18" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="18" customWidth="1"/>
-    <col min="10" max="10" width="14" style="19" customWidth="1"/>
-    <col min="11" max="11" width="24.1640625" style="20" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" style="20" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="13" style="18" hidden="1" customWidth="1"/>
-    <col min="14" max="1025" width="21.6640625" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="16" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="17" width="23.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="18" width="20.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="16" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="16" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="18" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="18" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="19" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="20" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="20" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="18" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="21.67"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="24" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+    <row r="1" s="24" customFormat="true" ht="52" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
         <v>13</v>
       </c>
@@ -1679,7 +1675,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="32" customFormat="1" ht="91" x14ac:dyDescent="0.2">
+    <row r="2" s="32" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
         <v>26</v>
       </c>
@@ -1720,8 +1716,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="35" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46" t="s">
+    <row r="3" s="35" customFormat="true" ht="22" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="28" t="s">
         <v>54</v>
       </c>
       <c r="B3" s="38" t="s">
@@ -1761,8 +1757,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="35" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
+    <row r="4" s="35" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="28"/>
       <c r="B4" s="33" t="s">
         <v>56</v>
       </c>
@@ -1800,8 +1796,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="35" customFormat="1" ht="182" x14ac:dyDescent="0.2">
-      <c r="A5" s="46"/>
+    <row r="5" s="35" customFormat="true" ht="182" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="28"/>
       <c r="B5" s="38" t="s">
         <v>57</v>
       </c>
@@ -1839,7 +1835,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="35" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+    <row r="6" s="35" customFormat="true" ht="52" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="28" t="s">
         <v>61</v>
       </c>
@@ -1880,7 +1876,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="35" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+    <row r="7" s="35" customFormat="true" ht="52" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="28" t="s">
         <v>71</v>
       </c>
@@ -1921,8 +1917,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="35" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="46" t="s">
+    <row r="8" s="35" customFormat="true" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="28" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="33" t="s">
@@ -1962,8 +1958,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="35" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="46"/>
+    <row r="9" s="35" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="28"/>
       <c r="B9" s="33" t="s">
         <v>47</v>
       </c>
@@ -2001,7 +1997,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="37" customFormat="1" ht="65" x14ac:dyDescent="0.2">
+    <row r="10" s="37" customFormat="true" ht="65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="28" t="s">
         <v>50</v>
       </c>
@@ -2043,10 +2039,10 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A8:A9"/>
   </mergeCells>
-  <printOptions horizontalCentered="1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="1" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="0" pageOrder="overThenDown" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Bold"&amp;12Novartis_BYM338E2202_Global Phase II
 WR myPROpad Setup Specifications
 &amp;A&amp;R&amp;"Times New Roman,Bold"&amp;10Version DRAFT 1.0</oddHeader>
@@ -2057,34 +2053,34 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <pageSetUpPr fitToPage="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="33" style="19" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="40" customWidth="1"/>
-    <col min="4" max="5" width="20.33203125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="18" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="18" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="18" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="18" customWidth="1"/>
-    <col min="10" max="10" width="14" style="19" customWidth="1"/>
-    <col min="11" max="11" width="24.1640625" style="19" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" style="19" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="13" style="18" hidden="1" customWidth="1"/>
-    <col min="14" max="1025" width="21.6640625" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="19" width="33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="40" width="23.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="18" width="20.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="18" width="13.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="18" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="18" width="12.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="18" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="19" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="19" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="19" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="18" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="21.67"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="24" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" s="24" customFormat="true" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
         <v>13</v>
       </c>
@@ -2125,7 +2121,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="43" t="s">
         <v>78</v>
       </c>
@@ -2148,7 +2144,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="43" t="s">
         <v>78</v>
       </c>
@@ -2164,15 +2160,15 @@
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
       <c r="K3" s="28"/>
-      <c r="L3" s="35">
-        <f>D3</f>
+      <c r="L3" s="35" t="n">
+        <f aca="false">D3</f>
         <v>0</v>
       </c>
       <c r="M3" s="35" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="43" t="s">
         <v>78</v>
       </c>
@@ -2195,7 +2191,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="43" t="s">
         <v>78</v>
       </c>
@@ -2218,7 +2214,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="43" t="s">
         <v>83</v>
       </c>
@@ -2235,7 +2231,7 @@
       <c r="J6" s="28"/>
       <c r="K6" s="28"/>
     </row>
-    <row r="7" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="43" t="s">
         <v>83</v>
       </c>
@@ -2252,7 +2248,7 @@
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
     </row>
-    <row r="8" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="44" t="s">
         <v>83</v>
       </c>
@@ -2271,7 +2267,7 @@
       <c r="L8" s="19"/>
       <c r="M8" s="18"/>
     </row>
-    <row r="9" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="44" t="s">
         <v>83</v>
       </c>
@@ -2290,7 +2286,7 @@
       <c r="L9" s="19"/>
       <c r="M9" s="18"/>
     </row>
-    <row r="10" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="44" t="s">
         <v>83</v>
       </c>
@@ -2309,12 +2305,12 @@
       <c r="L10" s="19"/>
       <c r="M10" s="18"/>
     </row>
-    <row r="11" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="34" t="s">
         <v>89</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>98</v>
       </c>
       <c r="C11" s="45"/>
       <c r="D11" s="28"/>
@@ -2328,12 +2324,12 @@
       <c r="L11" s="19"/>
       <c r="M11" s="18"/>
     </row>
-    <row r="12" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="44" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C12" s="45"/>
       <c r="D12" s="28"/>
@@ -2347,12 +2343,12 @@
       <c r="L12" s="19"/>
       <c r="M12" s="18"/>
     </row>
-    <row r="13" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="44" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C13" s="45"/>
       <c r="D13" s="28"/>
@@ -2366,12 +2362,12 @@
       <c r="L13" s="19"/>
       <c r="M13" s="18"/>
     </row>
-    <row r="14" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="44" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C14" s="45"/>
       <c r="D14" s="28"/>
@@ -2385,12 +2381,12 @@
       <c r="L14" s="19"/>
       <c r="M14" s="18"/>
     </row>
-    <row r="15" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="44" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C15" s="45"/>
       <c r="D15" s="28"/>
@@ -2404,12 +2400,12 @@
       <c r="L15" s="19"/>
       <c r="M15" s="18"/>
     </row>
-    <row r="16" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="34" t="s">
-        <v>101</v>
+    <row r="16" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="44" t="s">
+        <v>92</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C16" s="45"/>
       <c r="D16" s="28"/>
@@ -2423,12 +2419,12 @@
       <c r="L16" s="19"/>
       <c r="M16" s="18"/>
     </row>
-    <row r="17" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="34" t="s">
-        <v>101</v>
+    <row r="17" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="44" t="s">
+        <v>92</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C17" s="45"/>
       <c r="D17" s="28"/>
@@ -2442,12 +2438,12 @@
       <c r="L17" s="19"/>
       <c r="M17" s="18"/>
     </row>
-    <row r="18" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="34" t="s">
-        <v>101</v>
+    <row r="18" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="44" t="s">
+        <v>92</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C18" s="45"/>
       <c r="D18" s="28"/>
@@ -2461,12 +2457,12 @@
       <c r="L18" s="19"/>
       <c r="M18" s="18"/>
     </row>
-    <row r="19" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="34" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C19" s="45"/>
       <c r="D19" s="28"/>
@@ -2480,12 +2476,12 @@
       <c r="L19" s="19"/>
       <c r="M19" s="18"/>
     </row>
-    <row r="20" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="34" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C20" s="45"/>
       <c r="D20" s="28"/>
@@ -2499,12 +2495,12 @@
       <c r="L20" s="19"/>
       <c r="M20" s="18"/>
     </row>
-    <row r="21" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="34" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" s="45"/>
       <c r="D21" s="28"/>
@@ -2518,12 +2514,12 @@
       <c r="L21" s="19"/>
       <c r="M21" s="18"/>
     </row>
-    <row r="22" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="34" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C22" s="45"/>
       <c r="D22" s="28"/>
@@ -2537,12 +2533,12 @@
       <c r="L22" s="19"/>
       <c r="M22" s="18"/>
     </row>
-    <row r="23" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="34" t="s">
         <v>103</v>
-      </c>
-      <c r="B23" s="34" t="s">
-        <v>91</v>
       </c>
       <c r="C23" s="45"/>
       <c r="D23" s="28"/>
@@ -2556,9 +2552,9 @@
       <c r="L23" s="19"/>
       <c r="M23" s="18"/>
     </row>
-    <row r="24" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="34" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B24" s="34" t="s">
         <v>105</v>
@@ -2575,12 +2571,12 @@
       <c r="L24" s="19"/>
       <c r="M24" s="18"/>
     </row>
-    <row r="25" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="34" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C25" s="45"/>
       <c r="D25" s="28"/>
@@ -2594,12 +2590,12 @@
       <c r="L25" s="19"/>
       <c r="M25" s="18"/>
     </row>
-    <row r="26" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="34" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="C26" s="45"/>
       <c r="D26" s="28"/>
@@ -2613,12 +2609,12 @@
       <c r="L26" s="19"/>
       <c r="M26" s="18"/>
     </row>
-    <row r="27" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="34" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C27" s="45"/>
       <c r="D27" s="28"/>
@@ -2632,9 +2628,13 @@
       <c r="L27" s="19"/>
       <c r="M27" s="18"/>
     </row>
-    <row r="28" spans="1:13" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="34"/>
-      <c r="B28" s="34"/>
+    <row r="28" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>110</v>
+      </c>
       <c r="C28" s="45"/>
       <c r="D28" s="28"/>
       <c r="E28" s="28"/>
@@ -2647,11 +2647,64 @@
       <c r="L28" s="19"/>
       <c r="M28" s="18"/>
     </row>
+    <row r="29" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="45"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="18"/>
+    </row>
+    <row r="30" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="45"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="34"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="18"/>
+    </row>
+    <row r="31" s="35" customFormat="true" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="18"/>
+    </row>
   </sheetData>
-  <printOptions horizontalCentered="1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="1" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="0" pageOrder="overThenDown" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Bold"&amp;12Novartis_BYM338E2202_Global Phase II
 WR myPROpad Setup Specifications
 &amp;A&amp;R&amp;"Times New Roman,Bold"&amp;10Version DRAFT 1.0</oddHeader>

</xml_diff>

<commit_message>
Added some information about employee page
</commit_message>
<xml_diff>
--- a/Form SpecificationsV0.1_DRAFT.xlsx
+++ b/Form SpecificationsV0.1_DRAFT.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/FabstechTZ/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="80" yWindow="0" windowWidth="24580" windowHeight="16900" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Approval" sheetId="1" r:id="rId1"/>
@@ -26,7 +31,7 @@
     <definedName name="Print_Titles_0" localSheetId="2">'Example 2'!$A:$B,'Example 2'!$1:$1</definedName>
     <definedName name="Print_Titles_0" localSheetId="3">'Functional Specs'!$B:$C,'Functional Specs'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -42,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="123">
   <si>
     <t xml:space="preserve"> Specifications Author:</t>
   </si>
@@ -464,12 +469,15 @@
   <si>
     <t>Text Field</t>
   </si>
+  <si>
+    <t>Empoloyee Page</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="14">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -680,7 +688,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -801,9 +809,21 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -822,19 +842,10 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1173,38 +1184,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
-    <col min="6" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" customWidth="1"/>
+    <col min="6" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5">
+    <row r="1" spans="1:5" ht="23" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="1"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="30.6" customHeight="1">
+    <row r="2" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1221,7 +1232,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1">
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
         <v>5</v>
@@ -1236,7 +1247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -1245,42 +1256,42 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="22.35" customHeight="1">
+    <row r="10" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1295,7 +1306,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="8" customFormat="1">
+    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="7" t="s">
         <v>5</v>
@@ -1310,7 +1321,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="8" customFormat="1">
+    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1319,28 +1330,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="13"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>10</v>
       </c>
@@ -1355,7 +1366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="7" t="s">
         <v>5</v>
@@ -1370,7 +1381,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1379,7 +1390,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -1399,34 +1410,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="16" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="17" customWidth="1"/>
-    <col min="4" max="5" width="20.28515625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="16" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="18" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="18" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="17" customWidth="1"/>
+    <col min="4" max="5" width="20.33203125" style="18" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="16" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="18" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="18" customWidth="1"/>
     <col min="10" max="10" width="14" style="19" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" style="20" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" style="20" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="24.1640625" style="20" customWidth="1"/>
+    <col min="12" max="12" width="21.6640625" style="20" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="18" hidden="1" customWidth="1"/>
-    <col min="14" max="1025" width="21.7109375" customWidth="1"/>
+    <col min="14" max="1025" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="24" customFormat="1" ht="84.75" customHeight="1">
+    <row r="1" spans="1:13" s="24" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>13</v>
       </c>
@@ -1467,7 +1478,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="32" customFormat="1" ht="89.25">
+    <row r="2" spans="1:13" s="32" customFormat="1" ht="91" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>26</v>
       </c>
@@ -1508,7 +1519,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="32" customFormat="1" ht="27.95" customHeight="1">
+    <row r="3" spans="1:13" s="32" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>33</v>
       </c>
@@ -1545,8 +1556,8 @@
       <c r="L3" s="30"/>
       <c r="M3" s="31"/>
     </row>
-    <row r="4" spans="1:13" s="35" customFormat="1" ht="23.1" customHeight="1">
-      <c r="A4" s="44" t="s">
+    <row r="4" spans="1:13" s="35" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="46" t="s">
         <v>41</v>
       </c>
       <c r="B4" s="33" t="s">
@@ -1586,8 +1597,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="35" customFormat="1" ht="24" customHeight="1">
-      <c r="A5" s="44"/>
+    <row r="5" spans="1:13" s="35" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="46"/>
       <c r="B5" s="33" t="s">
         <v>47</v>
       </c>
@@ -1625,7 +1636,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="37" customFormat="1" ht="76.5">
+    <row r="6" spans="1:13" s="37" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
         <v>50</v>
       </c>
@@ -1680,34 +1691,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B2" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="16" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="17" customWidth="1"/>
-    <col min="4" max="5" width="20.28515625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="16" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="16" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="18" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="18" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="17" customWidth="1"/>
+    <col min="4" max="5" width="20.33203125" style="18" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="16" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="18" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="18" customWidth="1"/>
     <col min="10" max="10" width="14" style="19" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" style="20" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" style="20" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="24.1640625" style="20" customWidth="1"/>
+    <col min="12" max="12" width="21.6640625" style="20" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="18" hidden="1" customWidth="1"/>
-    <col min="14" max="1025" width="21.7109375" customWidth="1"/>
+    <col min="14" max="1025" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="24" customFormat="1" ht="63.75">
+    <row r="1" spans="1:13" s="24" customFormat="1" ht="52" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>13</v>
       </c>
@@ -1748,7 +1759,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="32" customFormat="1" ht="89.25">
+    <row r="2" spans="1:13" s="32" customFormat="1" ht="91" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>26</v>
       </c>
@@ -1789,8 +1800,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="35" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A3" s="44" t="s">
+    <row r="3" spans="1:13" s="35" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="46" t="s">
         <v>54</v>
       </c>
       <c r="B3" s="38" t="s">
@@ -1830,8 +1841,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="35" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="44"/>
+    <row r="4" spans="1:13" s="35" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="46"/>
       <c r="B4" s="33" t="s">
         <v>56</v>
       </c>
@@ -1869,8 +1880,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="35" customFormat="1" ht="178.5">
-      <c r="A5" s="44"/>
+    <row r="5" spans="1:13" s="35" customFormat="1" ht="182" x14ac:dyDescent="0.2">
+      <c r="A5" s="46"/>
       <c r="B5" s="38" t="s">
         <v>57</v>
       </c>
@@ -1908,7 +1919,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="35" customFormat="1" ht="63.75">
+    <row r="6" spans="1:13" s="35" customFormat="1" ht="52" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
         <v>61</v>
       </c>
@@ -1949,7 +1960,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="35" customFormat="1" ht="51">
+    <row r="7" spans="1:13" s="35" customFormat="1" ht="52" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
         <v>71</v>
       </c>
@@ -1990,8 +2001,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="35" customFormat="1" ht="23.1" customHeight="1">
-      <c r="A8" s="44" t="s">
+    <row r="8" spans="1:13" s="35" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="46" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="33" t="s">
@@ -2031,8 +2042,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="35" customFormat="1" ht="24" customHeight="1">
-      <c r="A9" s="44"/>
+    <row r="9" spans="1:13" s="35" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="46"/>
       <c r="B9" s="33" t="s">
         <v>47</v>
       </c>
@@ -2070,7 +2081,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="37" customFormat="1" ht="76.5">
+    <row r="10" spans="1:13" s="37" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="A10" s="28" t="s">
         <v>50</v>
       </c>
@@ -2126,35 +2137,35 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView showGridLines="0" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="19" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="19" customWidth="1"/>
     <col min="3" max="3" width="33" style="19" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" style="40" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="18" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="18" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="18" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="18" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="40" customWidth="1"/>
+    <col min="5" max="6" width="20.33203125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="18" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" style="18" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="18" customWidth="1"/>
     <col min="11" max="11" width="14" style="19" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" style="19" customWidth="1"/>
-    <col min="13" max="13" width="21.7109375" style="19" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="24.1640625" style="19" customWidth="1"/>
+    <col min="13" max="13" width="21.6640625" style="19" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="13" style="18" hidden="1" customWidth="1"/>
-    <col min="15" max="1026" width="21.7109375" customWidth="1"/>
+    <col min="15" max="1026" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="24" customFormat="1" ht="76.5">
+    <row r="1" spans="1:14" s="24" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="B1" s="41" t="s">
         <v>13</v>
       </c>
@@ -2195,11 +2206,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="2" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="35">
         <v>1</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="49" t="s">
         <v>95</v>
       </c>
       <c r="C2" s="34" t="s">
@@ -2223,11 +2234,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="3" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="35">
         <v>2</v>
       </c>
-      <c r="B3" s="46"/>
+      <c r="B3" s="50"/>
       <c r="C3" s="34" t="s">
         <v>86</v>
       </c>
@@ -2250,11 +2261,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="4" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="35">
         <v>3</v>
       </c>
-      <c r="B4" s="46"/>
+      <c r="B4" s="50"/>
       <c r="C4" s="34" t="s">
         <v>87</v>
       </c>
@@ -2276,8 +2287,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B5" s="46"/>
+    <row r="5" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="50"/>
       <c r="C5" s="34" t="s">
         <v>88</v>
       </c>
@@ -2293,8 +2304,8 @@
       <c r="K5" s="28"/>
       <c r="L5" s="28"/>
     </row>
-    <row r="6" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B6" s="46"/>
+    <row r="6" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="50"/>
       <c r="C6" s="34" t="s">
         <v>96</v>
       </c>
@@ -2310,8 +2321,8 @@
       <c r="K6" s="28"/>
       <c r="L6" s="28"/>
     </row>
-    <row r="7" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B7" s="46"/>
+    <row r="7" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="50"/>
       <c r="C7" s="34" t="s">
         <v>89</v>
       </c>
@@ -2327,8 +2338,8 @@
       <c r="K7" s="28"/>
       <c r="L7" s="28"/>
     </row>
-    <row r="8" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B8" s="46"/>
+    <row r="8" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="50"/>
       <c r="C8" s="34" t="s">
         <v>90</v>
       </c>
@@ -2344,11 +2355,11 @@
       <c r="K8" s="28"/>
       <c r="L8" s="28"/>
     </row>
-    <row r="9" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="9" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="35">
         <v>4</v>
       </c>
-      <c r="B9" s="47"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="34" t="s">
         <v>91</v>
       </c>
@@ -2370,11 +2381,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="10" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="35">
         <v>5</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="49" t="s">
         <v>107</v>
       </c>
       <c r="C10" s="34" t="s">
@@ -2392,11 +2403,11 @@
       <c r="K10" s="28"/>
       <c r="L10" s="28"/>
     </row>
-    <row r="11" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="11" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="35">
         <v>6</v>
       </c>
-      <c r="B11" s="46"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="34" t="s">
         <v>98</v>
       </c>
@@ -2412,11 +2423,11 @@
       <c r="K11" s="28"/>
       <c r="L11" s="28"/>
     </row>
-    <row r="12" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="12" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="35">
         <v>7</v>
       </c>
-      <c r="B12" s="46"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="34" t="s">
         <v>80</v>
       </c>
@@ -2434,11 +2445,11 @@
       <c r="M12" s="19"/>
       <c r="N12" s="18"/>
     </row>
-    <row r="13" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="13" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="35">
         <v>8</v>
       </c>
-      <c r="B13" s="46"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="34" t="s">
         <v>78</v>
       </c>
@@ -2456,11 +2467,11 @@
       <c r="M13" s="19"/>
       <c r="N13" s="18"/>
     </row>
-    <row r="14" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="14" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="35">
         <v>9</v>
       </c>
-      <c r="B14" s="46"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="34" t="s">
         <v>99</v>
       </c>
@@ -2478,11 +2489,11 @@
       <c r="M14" s="19"/>
       <c r="N14" s="18"/>
     </row>
-    <row r="15" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="15" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="35">
         <v>10</v>
       </c>
-      <c r="B15" s="46"/>
+      <c r="B15" s="50"/>
       <c r="C15" s="34" t="s">
         <v>79</v>
       </c>
@@ -2500,11 +2511,11 @@
       <c r="M15" s="19"/>
       <c r="N15" s="18"/>
     </row>
-    <row r="16" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="16" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="35">
         <v>11</v>
       </c>
-      <c r="B16" s="46"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="34" t="s">
         <v>100</v>
       </c>
@@ -2522,8 +2533,8 @@
       <c r="M16" s="19"/>
       <c r="N16" s="18"/>
     </row>
-    <row r="17" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B17" s="46"/>
+    <row r="17" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="50"/>
       <c r="C17" s="34" t="s">
         <v>102</v>
       </c>
@@ -2541,11 +2552,11 @@
       <c r="M17" s="19"/>
       <c r="N17" s="18"/>
     </row>
-    <row r="18" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="18" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="35">
         <v>12</v>
       </c>
-      <c r="B18" s="47"/>
+      <c r="B18" s="51"/>
       <c r="C18" s="34" t="s">
         <v>101</v>
       </c>
@@ -2563,11 +2574,11 @@
       <c r="M18" s="19"/>
       <c r="N18" s="18"/>
     </row>
-    <row r="19" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="19" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="35">
         <v>13</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="52" t="s">
         <v>108</v>
       </c>
       <c r="C19" s="34" t="s">
@@ -2585,11 +2596,11 @@
       <c r="M19" s="19"/>
       <c r="N19" s="18"/>
     </row>
-    <row r="20" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="20" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="35">
         <v>14</v>
       </c>
-      <c r="B20" s="49"/>
+      <c r="B20" s="53"/>
       <c r="C20" s="34" t="s">
         <v>104</v>
       </c>
@@ -2605,8 +2616,8 @@
       <c r="M20" s="19"/>
       <c r="N20" s="18"/>
     </row>
-    <row r="21" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B21" s="49"/>
+    <row r="21" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="53"/>
       <c r="C21" s="34" t="s">
         <v>99</v>
       </c>
@@ -2622,11 +2633,11 @@
       <c r="M21" s="19"/>
       <c r="N21" s="18"/>
     </row>
-    <row r="22" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="22" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="35">
         <v>15</v>
       </c>
-      <c r="B22" s="49"/>
+      <c r="B22" s="53"/>
       <c r="C22" s="34" t="s">
         <v>81</v>
       </c>
@@ -2642,11 +2653,11 @@
       <c r="M22" s="19"/>
       <c r="N22" s="18"/>
     </row>
-    <row r="23" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="23" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="35">
         <v>16</v>
       </c>
-      <c r="B23" s="49"/>
+      <c r="B23" s="53"/>
       <c r="C23" s="34" t="s">
         <v>105</v>
       </c>
@@ -2662,11 +2673,11 @@
       <c r="M23" s="19"/>
       <c r="N23" s="18"/>
     </row>
-    <row r="24" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="24" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="35">
         <v>17</v>
       </c>
-      <c r="B24" s="50"/>
+      <c r="B24" s="54"/>
       <c r="C24" s="34" t="s">
         <v>106</v>
       </c>
@@ -2682,11 +2693,11 @@
       <c r="M24" s="19"/>
       <c r="N24" s="18"/>
     </row>
-    <row r="25" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="25" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="35">
         <v>18</v>
       </c>
-      <c r="B25" s="51" t="s">
+      <c r="B25" s="47" t="s">
         <v>114</v>
       </c>
       <c r="C25" s="34" t="s">
@@ -2704,11 +2715,11 @@
       <c r="M25" s="19"/>
       <c r="N25" s="18"/>
     </row>
-    <row r="26" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="26" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="35">
         <v>19</v>
       </c>
-      <c r="B26" s="52"/>
+      <c r="B26" s="55"/>
       <c r="C26" s="34" t="s">
         <v>82</v>
       </c>
@@ -2724,11 +2735,11 @@
       <c r="M26" s="19"/>
       <c r="N26" s="18"/>
     </row>
-    <row r="27" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="27" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="35">
         <v>20</v>
       </c>
-      <c r="B27" s="52"/>
+      <c r="B27" s="55"/>
       <c r="C27" s="34" t="s">
         <v>109</v>
       </c>
@@ -2744,11 +2755,11 @@
       <c r="M27" s="19"/>
       <c r="N27" s="18"/>
     </row>
-    <row r="28" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="28" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="35">
         <v>21</v>
       </c>
-      <c r="B28" s="52"/>
+      <c r="B28" s="55"/>
       <c r="C28" s="34" t="s">
         <v>84</v>
       </c>
@@ -2764,8 +2775,8 @@
       <c r="M28" s="19"/>
       <c r="N28" s="18"/>
     </row>
-    <row r="29" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B29" s="52"/>
+    <row r="29" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="55"/>
       <c r="C29" s="34" t="s">
         <v>110</v>
       </c>
@@ -2781,8 +2792,8 @@
       <c r="M29" s="19"/>
       <c r="N29" s="18"/>
     </row>
-    <row r="30" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B30" s="52"/>
+    <row r="30" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="55"/>
       <c r="C30" s="34" t="s">
         <v>112</v>
       </c>
@@ -2798,8 +2809,8 @@
       <c r="M30" s="19"/>
       <c r="N30" s="18"/>
     </row>
-    <row r="31" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B31" s="52"/>
+    <row r="31" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="55"/>
       <c r="C31" s="34" t="s">
         <v>113</v>
       </c>
@@ -2815,11 +2826,11 @@
       <c r="M31" s="19"/>
       <c r="N31" s="18"/>
     </row>
-    <row r="32" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="32" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="35">
         <v>22</v>
       </c>
-      <c r="B32" s="53"/>
+      <c r="B32" s="48"/>
       <c r="C32" s="34" t="s">
         <v>111</v>
       </c>
@@ -2835,11 +2846,11 @@
       <c r="M32" s="19"/>
       <c r="N32" s="18"/>
     </row>
-    <row r="33" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="33" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="35">
         <v>23</v>
       </c>
-      <c r="B33" s="51" t="s">
+      <c r="B33" s="47" t="s">
         <v>119</v>
       </c>
       <c r="C33" s="34" t="s">
@@ -2859,11 +2870,11 @@
       <c r="M33" s="19"/>
       <c r="N33" s="18"/>
     </row>
-    <row r="34" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="34" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="35">
         <v>24</v>
       </c>
-      <c r="B34" s="54"/>
+      <c r="B34" s="56"/>
       <c r="C34" s="34" t="s">
         <v>116</v>
       </c>
@@ -2881,11 +2892,11 @@
       <c r="M34" s="19"/>
       <c r="N34" s="18"/>
     </row>
-    <row r="35" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="35" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="35">
         <v>25</v>
       </c>
-      <c r="B35" s="54"/>
+      <c r="B35" s="56"/>
       <c r="C35" s="34" t="s">
         <v>117</v>
       </c>
@@ -2903,14 +2914,14 @@
       <c r="M35" s="19"/>
       <c r="N35" s="18"/>
     </row>
-    <row r="36" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="36" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="35">
         <v>27</v>
       </c>
-      <c r="B36" s="51" t="s">
+      <c r="B36" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="C36" s="55" t="s">
+      <c r="C36" s="44" t="s">
         <v>120</v>
       </c>
       <c r="D36" s="43"/>
@@ -2927,12 +2938,12 @@
       <c r="M36" s="19"/>
       <c r="N36" s="18"/>
     </row>
-    <row r="37" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+    <row r="37" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="35">
         <v>28</v>
       </c>
-      <c r="B37" s="53"/>
-      <c r="C37" s="55" t="s">
+      <c r="B37" s="48"/>
+      <c r="C37" s="44" t="s">
         <v>117</v>
       </c>
       <c r="D37" s="43"/>
@@ -2949,14 +2960,83 @@
       <c r="M37" s="19"/>
       <c r="N37" s="18"/>
     </row>
+    <row r="38" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="35">
+        <v>29</v>
+      </c>
+      <c r="B38" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="43"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="34"/>
+      <c r="L38" s="34"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="18"/>
+    </row>
+    <row r="39" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="48"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="45"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="34"/>
+      <c r="L39" s="34"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="18"/>
+    </row>
+    <row r="40" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="47"/>
+      <c r="C40" s="44"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="45"/>
+      <c r="J40" s="45"/>
+      <c r="K40" s="34"/>
+      <c r="L40" s="34"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="18"/>
+    </row>
+    <row r="41" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="48"/>
+      <c r="C41" s="44"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="45"/>
+      <c r="J41" s="45"/>
+      <c r="K41" s="34"/>
+      <c r="L41" s="34"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B36:B37"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="B10:B18"/>
     <mergeCell ref="B19:B24"/>
     <mergeCell ref="B25:B32"/>
     <mergeCell ref="B33:B35"/>
-    <mergeCell ref="B36:B37"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="1" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Employee and Employer front end
</commit_message>
<xml_diff>
--- a/Form SpecificationsV0.1_DRAFT.xlsx
+++ b/Form SpecificationsV0.1_DRAFT.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/FabstechTZ/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="0" windowWidth="24580" windowHeight="16900" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="75" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Approval" sheetId="1" r:id="rId1"/>
@@ -31,7 +26,7 @@
     <definedName name="Print_Titles_0" localSheetId="2">'Example 2'!$A:$B,'Example 2'!$1:$1</definedName>
     <definedName name="Print_Titles_0" localSheetId="3">'Functional Specs'!$B:$C,'Functional Specs'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -46,8 +41,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>ABDULKARIM</author>
+  </authors>
+  <commentList>
+    <comment ref="B64" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ABDULKARIM:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+z</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="152">
   <si>
     <t xml:space="preserve"> Specifications Author:</t>
   </si>
@@ -470,14 +499,101 @@
     <t>Text Field</t>
   </si>
   <si>
-    <t>Empoloyee Page</t>
+    <t>Company Review Page</t>
+  </si>
+  <si>
+    <t>Company name</t>
+  </si>
+  <si>
+    <t>Employers/post job</t>
+  </si>
+  <si>
+    <t>Account information</t>
+  </si>
+  <si>
+    <t>Getting started</t>
+  </si>
+  <si>
+    <t>Job details</t>
+  </si>
+  <si>
+    <t>Application settings</t>
+  </si>
+  <si>
+    <t>Job description</t>
+  </si>
+  <si>
+    <t>Account information page</t>
+  </si>
+  <si>
+    <t>Company size</t>
+  </si>
+  <si>
+    <t>Person name</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Dropdown</t>
+  </si>
+  <si>
+    <t>Getting started page</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Continue</t>
+  </si>
+  <si>
+    <t>Job details page</t>
+  </si>
+  <si>
+    <t>Type of job (full-time, part-time, etc)</t>
+  </si>
+  <si>
+    <t>How did you here about us (radio, TV, etc)</t>
+  </si>
+  <si>
+    <t>Salary for this job (optional)</t>
+  </si>
+  <si>
+    <t>Salary per? (monrh, week, etc)</t>
+  </si>
+  <si>
+    <t>how do you want to receive application? (email, in-person)</t>
+  </si>
+  <si>
+    <t>Appilication for this job will be sent to which email?</t>
+  </si>
+  <si>
+    <t>Required experience</t>
+  </si>
+  <si>
+    <t>Required skills</t>
+  </si>
+  <si>
+    <t>Required education</t>
+  </si>
+  <si>
+    <t>Post Job</t>
+  </si>
+  <si>
+    <t>Text Area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -576,6 +692,41 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -688,7 +839,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -809,21 +960,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -842,10 +987,28 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1184,38 +1347,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" customWidth="1"/>
-    <col min="6" max="1025" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" customWidth="1"/>
+    <col min="6" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="22.5">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="1"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="30.6" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1232,7 +1395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" s="8" customFormat="1">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
         <v>5</v>
@@ -1247,7 +1410,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -1256,42 +1419,42 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="22.35" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1306,7 +1469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" s="8" customFormat="1">
       <c r="A11" s="6"/>
       <c r="B11" s="7" t="s">
         <v>5</v>
@@ -1321,7 +1484,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" s="8" customFormat="1">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1330,28 +1493,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="13"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
         <v>10</v>
       </c>
@@ -1366,7 +1529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" s="6"/>
       <c r="B19" s="7" t="s">
         <v>5</v>
@@ -1381,7 +1544,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1390,7 +1553,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -1410,34 +1573,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="17" customWidth="1"/>
-    <col min="4" max="5" width="20.33203125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="18" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="16" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="17" customWidth="1"/>
+    <col min="4" max="5" width="20.28515625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="16" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="18" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="18" customWidth="1"/>
     <col min="10" max="10" width="14" style="19" customWidth="1"/>
-    <col min="11" max="11" width="24.1640625" style="20" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" style="20" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" style="20" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" style="20" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="18" hidden="1" customWidth="1"/>
-    <col min="14" max="1025" width="21.6640625" customWidth="1"/>
+    <col min="14" max="1025" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="24" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="24" customFormat="1" ht="84.75" customHeight="1">
       <c r="A1" s="21" t="s">
         <v>13</v>
       </c>
@@ -1478,7 +1641,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="32" customFormat="1" ht="91" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="32" customFormat="1" ht="89.25">
       <c r="A2" s="25" t="s">
         <v>26</v>
       </c>
@@ -1519,7 +1682,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="32" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" s="32" customFormat="1" ht="27.95" customHeight="1">
       <c r="A3" s="25" t="s">
         <v>33</v>
       </c>
@@ -1556,7 +1719,7 @@
       <c r="L3" s="30"/>
       <c r="M3" s="31"/>
     </row>
-    <row r="4" spans="1:13" s="35" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="35" customFormat="1" ht="23.1" customHeight="1">
       <c r="A4" s="46" t="s">
         <v>41</v>
       </c>
@@ -1597,7 +1760,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="35" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="35" customFormat="1" ht="24" customHeight="1">
       <c r="A5" s="46"/>
       <c r="B5" s="33" t="s">
         <v>47</v>
@@ -1636,7 +1799,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="37" customFormat="1" ht="65" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="37" customFormat="1" ht="76.5">
       <c r="A6" s="28" t="s">
         <v>50</v>
       </c>
@@ -1691,34 +1854,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B2" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="17" customWidth="1"/>
-    <col min="4" max="5" width="20.33203125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="18" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="16" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="17" customWidth="1"/>
+    <col min="4" max="5" width="20.28515625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="16" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="16" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="18" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="18" customWidth="1"/>
     <col min="10" max="10" width="14" style="19" customWidth="1"/>
-    <col min="11" max="11" width="24.1640625" style="20" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" style="20" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" style="20" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" style="20" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="18" hidden="1" customWidth="1"/>
-    <col min="14" max="1025" width="21.6640625" customWidth="1"/>
+    <col min="14" max="1025" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="24" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="24" customFormat="1" ht="63.75">
       <c r="A1" s="21" t="s">
         <v>13</v>
       </c>
@@ -1759,7 +1922,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="32" customFormat="1" ht="91" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="32" customFormat="1" ht="89.25">
       <c r="A2" s="25" t="s">
         <v>26</v>
       </c>
@@ -1800,7 +1963,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="35" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" s="35" customFormat="1" ht="21.95" customHeight="1">
       <c r="A3" s="46" t="s">
         <v>54</v>
       </c>
@@ -1841,7 +2004,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="35" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="35" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="46"/>
       <c r="B4" s="33" t="s">
         <v>56</v>
@@ -1880,7 +2043,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="35" customFormat="1" ht="182" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="35" customFormat="1" ht="178.5">
       <c r="A5" s="46"/>
       <c r="B5" s="38" t="s">
         <v>57</v>
@@ -1919,7 +2082,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="35" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="35" customFormat="1" ht="63.75">
       <c r="A6" s="28" t="s">
         <v>61</v>
       </c>
@@ -1960,7 +2123,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="35" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="35" customFormat="1" ht="51">
       <c r="A7" s="28" t="s">
         <v>71</v>
       </c>
@@ -2001,7 +2164,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="35" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="35" customFormat="1" ht="23.1" customHeight="1">
       <c r="A8" s="46" t="s">
         <v>41</v>
       </c>
@@ -2042,7 +2205,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="35" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" s="35" customFormat="1" ht="24" customHeight="1">
       <c r="A9" s="46"/>
       <c r="B9" s="33" t="s">
         <v>47</v>
@@ -2081,7 +2244,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="37" customFormat="1" ht="65" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" s="37" customFormat="1" ht="76.5">
       <c r="A10" s="28" t="s">
         <v>50</v>
       </c>
@@ -2137,35 +2300,35 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="19" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="19" customWidth="1"/>
     <col min="3" max="3" width="33" style="19" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" style="40" customWidth="1"/>
-    <col min="5" max="6" width="20.33203125" style="18" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="18" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="18" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="18" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" style="40" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="18" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="18" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="18" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="18" customWidth="1"/>
     <col min="11" max="11" width="14" style="19" customWidth="1"/>
-    <col min="12" max="12" width="24.1640625" style="19" customWidth="1"/>
-    <col min="13" max="13" width="21.6640625" style="19" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" style="19" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" style="19" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="13" style="18" hidden="1" customWidth="1"/>
-    <col min="15" max="1026" width="21.6640625" customWidth="1"/>
+    <col min="15" max="1026" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="24" customFormat="1" ht="65" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="24" customFormat="1" ht="76.5">
       <c r="B1" s="41" t="s">
         <v>13</v>
       </c>
@@ -2206,11 +2369,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A2" s="35">
         <v>1</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="47" t="s">
         <v>95</v>
       </c>
       <c r="C2" s="34" t="s">
@@ -2234,11 +2397,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A3" s="35">
         <v>2</v>
       </c>
-      <c r="B3" s="50"/>
+      <c r="B3" s="48"/>
       <c r="C3" s="34" t="s">
         <v>86</v>
       </c>
@@ -2261,11 +2424,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A4" s="35">
         <v>3</v>
       </c>
-      <c r="B4" s="50"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="34" t="s">
         <v>87</v>
       </c>
@@ -2287,8 +2450,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="50"/>
+    <row r="5" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B5" s="48"/>
       <c r="C5" s="34" t="s">
         <v>88</v>
       </c>
@@ -2304,8 +2467,8 @@
       <c r="K5" s="28"/>
       <c r="L5" s="28"/>
     </row>
-    <row r="6" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="50"/>
+    <row r="6" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B6" s="48"/>
       <c r="C6" s="34" t="s">
         <v>96</v>
       </c>
@@ -2321,8 +2484,8 @@
       <c r="K6" s="28"/>
       <c r="L6" s="28"/>
     </row>
-    <row r="7" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="50"/>
+    <row r="7" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B7" s="48"/>
       <c r="C7" s="34" t="s">
         <v>89</v>
       </c>
@@ -2338,8 +2501,8 @@
       <c r="K7" s="28"/>
       <c r="L7" s="28"/>
     </row>
-    <row r="8" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="50"/>
+    <row r="8" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B8" s="48"/>
       <c r="C8" s="34" t="s">
         <v>90</v>
       </c>
@@ -2355,11 +2518,11 @@
       <c r="K8" s="28"/>
       <c r="L8" s="28"/>
     </row>
-    <row r="9" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A9" s="35">
         <v>4</v>
       </c>
-      <c r="B9" s="51"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="34" t="s">
         <v>91</v>
       </c>
@@ -2381,11 +2544,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A10" s="35">
         <v>5</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="47" t="s">
         <v>107</v>
       </c>
       <c r="C10" s="34" t="s">
@@ -2403,11 +2566,11 @@
       <c r="K10" s="28"/>
       <c r="L10" s="28"/>
     </row>
-    <row r="11" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A11" s="35">
         <v>6</v>
       </c>
-      <c r="B11" s="50"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="34" t="s">
         <v>98</v>
       </c>
@@ -2423,11 +2586,11 @@
       <c r="K11" s="28"/>
       <c r="L11" s="28"/>
     </row>
-    <row r="12" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A12" s="35">
         <v>7</v>
       </c>
-      <c r="B12" s="50"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="34" t="s">
         <v>80</v>
       </c>
@@ -2445,11 +2608,11 @@
       <c r="M12" s="19"/>
       <c r="N12" s="18"/>
     </row>
-    <row r="13" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A13" s="35">
         <v>8</v>
       </c>
-      <c r="B13" s="50"/>
+      <c r="B13" s="48"/>
       <c r="C13" s="34" t="s">
         <v>78</v>
       </c>
@@ -2467,11 +2630,11 @@
       <c r="M13" s="19"/>
       <c r="N13" s="18"/>
     </row>
-    <row r="14" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A14" s="35">
         <v>9</v>
       </c>
-      <c r="B14" s="50"/>
+      <c r="B14" s="48"/>
       <c r="C14" s="34" t="s">
         <v>99</v>
       </c>
@@ -2489,11 +2652,11 @@
       <c r="M14" s="19"/>
       <c r="N14" s="18"/>
     </row>
-    <row r="15" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A15" s="35">
         <v>10</v>
       </c>
-      <c r="B15" s="50"/>
+      <c r="B15" s="48"/>
       <c r="C15" s="34" t="s">
         <v>79</v>
       </c>
@@ -2511,11 +2674,11 @@
       <c r="M15" s="19"/>
       <c r="N15" s="18"/>
     </row>
-    <row r="16" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A16" s="35">
         <v>11</v>
       </c>
-      <c r="B16" s="50"/>
+      <c r="B16" s="48"/>
       <c r="C16" s="34" t="s">
         <v>100</v>
       </c>
@@ -2533,8 +2696,8 @@
       <c r="M16" s="19"/>
       <c r="N16" s="18"/>
     </row>
-    <row r="17" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="50"/>
+    <row r="17" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B17" s="48"/>
       <c r="C17" s="34" t="s">
         <v>102</v>
       </c>
@@ -2552,11 +2715,11 @@
       <c r="M17" s="19"/>
       <c r="N17" s="18"/>
     </row>
-    <row r="18" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A18" s="35">
         <v>12</v>
       </c>
-      <c r="B18" s="51"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="34" t="s">
         <v>101</v>
       </c>
@@ -2574,11 +2737,11 @@
       <c r="M18" s="19"/>
       <c r="N18" s="18"/>
     </row>
-    <row r="19" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A19" s="35">
         <v>13</v>
       </c>
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="50" t="s">
         <v>108</v>
       </c>
       <c r="C19" s="34" t="s">
@@ -2596,11 +2759,11 @@
       <c r="M19" s="19"/>
       <c r="N19" s="18"/>
     </row>
-    <row r="20" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A20" s="35">
         <v>14</v>
       </c>
-      <c r="B20" s="53"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="34" t="s">
         <v>104</v>
       </c>
@@ -2616,8 +2779,8 @@
       <c r="M20" s="19"/>
       <c r="N20" s="18"/>
     </row>
-    <row r="21" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="53"/>
+    <row r="21" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B21" s="51"/>
       <c r="C21" s="34" t="s">
         <v>99</v>
       </c>
@@ -2633,11 +2796,11 @@
       <c r="M21" s="19"/>
       <c r="N21" s="18"/>
     </row>
-    <row r="22" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A22" s="35">
         <v>15</v>
       </c>
-      <c r="B22" s="53"/>
+      <c r="B22" s="51"/>
       <c r="C22" s="34" t="s">
         <v>81</v>
       </c>
@@ -2653,11 +2816,11 @@
       <c r="M22" s="19"/>
       <c r="N22" s="18"/>
     </row>
-    <row r="23" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A23" s="35">
         <v>16</v>
       </c>
-      <c r="B23" s="53"/>
+      <c r="B23" s="51"/>
       <c r="C23" s="34" t="s">
         <v>105</v>
       </c>
@@ -2673,11 +2836,11 @@
       <c r="M23" s="19"/>
       <c r="N23" s="18"/>
     </row>
-    <row r="24" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A24" s="35">
         <v>17</v>
       </c>
-      <c r="B24" s="54"/>
+      <c r="B24" s="52"/>
       <c r="C24" s="34" t="s">
         <v>106</v>
       </c>
@@ -2693,11 +2856,11 @@
       <c r="M24" s="19"/>
       <c r="N24" s="18"/>
     </row>
-    <row r="25" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A25" s="35">
         <v>18</v>
       </c>
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="53" t="s">
         <v>114</v>
       </c>
       <c r="C25" s="34" t="s">
@@ -2715,11 +2878,11 @@
       <c r="M25" s="19"/>
       <c r="N25" s="18"/>
     </row>
-    <row r="26" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A26" s="35">
         <v>19</v>
       </c>
-      <c r="B26" s="55"/>
+      <c r="B26" s="54"/>
       <c r="C26" s="34" t="s">
         <v>82</v>
       </c>
@@ -2735,11 +2898,11 @@
       <c r="M26" s="19"/>
       <c r="N26" s="18"/>
     </row>
-    <row r="27" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A27" s="35">
         <v>20</v>
       </c>
-      <c r="B27" s="55"/>
+      <c r="B27" s="54"/>
       <c r="C27" s="34" t="s">
         <v>109</v>
       </c>
@@ -2755,11 +2918,11 @@
       <c r="M27" s="19"/>
       <c r="N27" s="18"/>
     </row>
-    <row r="28" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A28" s="35">
         <v>21</v>
       </c>
-      <c r="B28" s="55"/>
+      <c r="B28" s="54"/>
       <c r="C28" s="34" t="s">
         <v>84</v>
       </c>
@@ -2775,8 +2938,8 @@
       <c r="M28" s="19"/>
       <c r="N28" s="18"/>
     </row>
-    <row r="29" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="55"/>
+    <row r="29" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B29" s="54"/>
       <c r="C29" s="34" t="s">
         <v>110</v>
       </c>
@@ -2792,8 +2955,8 @@
       <c r="M29" s="19"/>
       <c r="N29" s="18"/>
     </row>
-    <row r="30" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="55"/>
+    <row r="30" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B30" s="54"/>
       <c r="C30" s="34" t="s">
         <v>112</v>
       </c>
@@ -2809,8 +2972,8 @@
       <c r="M30" s="19"/>
       <c r="N30" s="18"/>
     </row>
-    <row r="31" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="55"/>
+    <row r="31" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B31" s="54"/>
       <c r="C31" s="34" t="s">
         <v>113</v>
       </c>
@@ -2826,11 +2989,11 @@
       <c r="M31" s="19"/>
       <c r="N31" s="18"/>
     </row>
-    <row r="32" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A32" s="35">
         <v>22</v>
       </c>
-      <c r="B32" s="48"/>
+      <c r="B32" s="55"/>
       <c r="C32" s="34" t="s">
         <v>111</v>
       </c>
@@ -2846,11 +3009,11 @@
       <c r="M32" s="19"/>
       <c r="N32" s="18"/>
     </row>
-    <row r="33" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A33" s="35">
         <v>23</v>
       </c>
-      <c r="B33" s="47" t="s">
+      <c r="B33" s="50" t="s">
         <v>119</v>
       </c>
       <c r="C33" s="34" t="s">
@@ -2870,7 +3033,7 @@
       <c r="M33" s="19"/>
       <c r="N33" s="18"/>
     </row>
-    <row r="34" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A34" s="35">
         <v>24</v>
       </c>
@@ -2892,7 +3055,7 @@
       <c r="M34" s="19"/>
       <c r="N34" s="18"/>
     </row>
-    <row r="35" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A35" s="35">
         <v>25</v>
       </c>
@@ -2914,14 +3077,14 @@
       <c r="M35" s="19"/>
       <c r="N35" s="18"/>
     </row>
-    <row r="36" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A36" s="35">
         <v>27</v>
       </c>
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="C36" s="44" t="s">
+      <c r="C36" s="45" t="s">
         <v>120</v>
       </c>
       <c r="D36" s="43"/>
@@ -2938,12 +3101,12 @@
       <c r="M36" s="19"/>
       <c r="N36" s="18"/>
     </row>
-    <row r="37" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="A37" s="35">
         <v>28</v>
       </c>
-      <c r="B37" s="48"/>
-      <c r="C37" s="44" t="s">
+      <c r="B37" s="52"/>
+      <c r="C37" s="45" t="s">
         <v>117</v>
       </c>
       <c r="D37" s="43"/>
@@ -2960,78 +3123,549 @@
       <c r="M37" s="19"/>
       <c r="N37" s="18"/>
     </row>
-    <row r="38" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="35">
-        <v>29</v>
-      </c>
-      <c r="B38" s="47" t="s">
+    <row r="38" spans="1:14">
+      <c r="B38" s="53" t="s">
         <v>122</v>
       </c>
-      <c r="C38" s="44" t="s">
-        <v>88</v>
+      <c r="C38" s="34" t="s">
+        <v>123</v>
       </c>
       <c r="D38" s="43"/>
-      <c r="E38" s="45"/>
-      <c r="F38" s="45"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="45"/>
-      <c r="I38" s="45"/>
-      <c r="J38" s="45"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H38" s="44"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="44"/>
       <c r="K38" s="34"/>
       <c r="L38" s="34"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="18"/>
-    </row>
-    <row r="39" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="48"/>
-      <c r="C39" s="44"/>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="B39" s="54"/>
+      <c r="C39" s="34" t="s">
+        <v>117</v>
+      </c>
       <c r="D39" s="43"/>
-      <c r="E39" s="45"/>
-      <c r="F39" s="45"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="45"/>
-      <c r="J39" s="45"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H39" s="44"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="44"/>
       <c r="K39" s="34"/>
       <c r="L39" s="34"/>
-      <c r="M39" s="19"/>
-      <c r="N39" s="18"/>
-    </row>
-    <row r="40" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="47"/>
-      <c r="C40" s="44"/>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="B40" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" s="57" t="s">
+        <v>125</v>
+      </c>
       <c r="D40" s="43"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="44"/>
       <c r="G40" s="33"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="45"/>
-      <c r="J40" s="45"/>
+      <c r="H40" s="44"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
       <c r="K40" s="34"/>
       <c r="L40" s="34"/>
-      <c r="M40" s="19"/>
-      <c r="N40" s="18"/>
-    </row>
-    <row r="41" spans="1:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="48"/>
-      <c r="C41" s="44"/>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="B41" s="54"/>
+      <c r="C41" s="57" t="s">
+        <v>126</v>
+      </c>
       <c r="D41" s="43"/>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
       <c r="G41" s="33"/>
-      <c r="H41" s="45"/>
-      <c r="I41" s="45"/>
-      <c r="J41" s="45"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="44"/>
       <c r="K41" s="34"/>
       <c r="L41" s="34"/>
-      <c r="M41" s="19"/>
-      <c r="N41" s="18"/>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="B42" s="54"/>
+      <c r="C42" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="D42" s="43"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="44"/>
+      <c r="K42" s="34"/>
+      <c r="L42" s="34"/>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="B43" s="54"/>
+      <c r="C43" s="57" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" s="43"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="34"/>
+      <c r="L43" s="34"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="B44" s="55"/>
+      <c r="C44" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" s="43"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="44"/>
+      <c r="I44" s="44"/>
+      <c r="J44" s="44"/>
+      <c r="K44" s="34"/>
+      <c r="L44" s="34"/>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="B45" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D45" s="43"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H45" s="44"/>
+      <c r="I45" s="44"/>
+      <c r="J45" s="44"/>
+      <c r="K45" s="34"/>
+      <c r="L45" s="34"/>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="B46" s="59"/>
+      <c r="C46" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="D46" s="43"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H46" s="44"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
+      <c r="K46" s="34"/>
+      <c r="L46" s="34"/>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="B47" s="59"/>
+      <c r="C47" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="D47" s="43"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H47" s="44"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
+      <c r="K47" s="34"/>
+      <c r="L47" s="34"/>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="B48" s="59"/>
+      <c r="C48" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" s="43"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H48" s="44"/>
+      <c r="I48" s="44"/>
+      <c r="J48" s="44"/>
+      <c r="K48" s="34"/>
+      <c r="L48" s="34"/>
+    </row>
+    <row r="49" spans="2:14" ht="25.5">
+      <c r="B49" s="59"/>
+      <c r="C49" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="D49" s="43"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="44"/>
+      <c r="G49" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="H49" s="44"/>
+      <c r="I49" s="44"/>
+      <c r="J49" s="44"/>
+      <c r="K49" s="34"/>
+      <c r="L49" s="34"/>
+      <c r="M49"/>
+      <c r="N49"/>
+    </row>
+    <row r="50" spans="2:14" ht="25.5" customHeight="1">
+      <c r="B50" s="58" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D50" s="43"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H50" s="44"/>
+      <c r="I50" s="44"/>
+      <c r="J50" s="44"/>
+      <c r="K50" s="34"/>
+      <c r="L50" s="34"/>
+    </row>
+    <row r="51" spans="2:14">
+      <c r="B51" s="59"/>
+      <c r="C51" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="D51" s="43"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H51" s="44"/>
+      <c r="I51" s="44"/>
+      <c r="J51" s="44"/>
+      <c r="K51" s="34"/>
+      <c r="L51" s="34"/>
+    </row>
+    <row r="52" spans="2:14">
+      <c r="B52" s="59"/>
+      <c r="C52" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="D52" s="43"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H52" s="44"/>
+      <c r="I52" s="44"/>
+      <c r="J52" s="44"/>
+      <c r="K52" s="34"/>
+      <c r="L52" s="34"/>
+    </row>
+    <row r="53" spans="2:14">
+      <c r="B53" s="59"/>
+      <c r="C53" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D53" s="43"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H53" s="44"/>
+      <c r="I53" s="44"/>
+      <c r="J53" s="44"/>
+      <c r="K53" s="34"/>
+      <c r="L53" s="34"/>
+    </row>
+    <row r="54" spans="2:14">
+      <c r="B54" s="60"/>
+      <c r="C54" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D54" s="43"/>
+      <c r="E54" s="44"/>
+      <c r="F54" s="44"/>
+      <c r="G54" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H54" s="44"/>
+      <c r="I54" s="44"/>
+      <c r="J54" s="44"/>
+      <c r="K54" s="34"/>
+      <c r="L54" s="34"/>
+    </row>
+    <row r="55" spans="2:14">
+      <c r="B55" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="C55" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="D55" s="43"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="44"/>
+      <c r="G55" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="H55" s="44"/>
+      <c r="I55" s="44"/>
+      <c r="J55" s="44"/>
+      <c r="K55" s="34"/>
+      <c r="L55" s="34"/>
+    </row>
+    <row r="56" spans="2:14">
+      <c r="B56" s="59"/>
+      <c r="C56" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="D56" s="43"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H56" s="44"/>
+      <c r="I56" s="44"/>
+      <c r="J56" s="44"/>
+      <c r="K56" s="34"/>
+      <c r="L56" s="34"/>
+    </row>
+    <row r="57" spans="2:14">
+      <c r="B57" s="59"/>
+      <c r="C57" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="D57" s="43"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
+      <c r="G57" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="H57" s="44"/>
+      <c r="I57" s="44"/>
+      <c r="J57" s="44"/>
+      <c r="K57" s="34"/>
+      <c r="L57" s="34"/>
+    </row>
+    <row r="58" spans="2:14">
+      <c r="B58" s="59"/>
+      <c r="C58" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D58" s="43"/>
+      <c r="E58" s="44"/>
+      <c r="F58" s="44"/>
+      <c r="G58" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H58" s="44"/>
+      <c r="I58" s="44"/>
+      <c r="J58" s="44"/>
+      <c r="K58" s="34"/>
+      <c r="L58" s="34"/>
+    </row>
+    <row r="59" spans="2:14">
+      <c r="B59" s="60"/>
+      <c r="C59" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D59" s="43"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="44"/>
+      <c r="G59" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H59" s="44"/>
+      <c r="I59" s="44"/>
+      <c r="J59" s="44"/>
+      <c r="K59" s="34"/>
+      <c r="L59" s="34"/>
+    </row>
+    <row r="60" spans="2:14" ht="25.5">
+      <c r="B60" s="58" t="s">
+        <v>128</v>
+      </c>
+      <c r="C60" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="D60" s="43"/>
+      <c r="E60" s="44"/>
+      <c r="F60" s="44"/>
+      <c r="G60" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H60" s="44"/>
+      <c r="I60" s="44"/>
+      <c r="J60" s="44"/>
+      <c r="K60" s="34"/>
+      <c r="L60" s="34"/>
+    </row>
+    <row r="61" spans="2:14" ht="25.5">
+      <c r="B61" s="59"/>
+      <c r="C61" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="D61" s="43"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="H61" s="44"/>
+      <c r="I61" s="44"/>
+      <c r="J61" s="44"/>
+      <c r="K61" s="34"/>
+      <c r="L61" s="34"/>
+    </row>
+    <row r="62" spans="2:14">
+      <c r="B62" s="59"/>
+      <c r="C62" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D62" s="43"/>
+      <c r="E62" s="44"/>
+      <c r="F62" s="44"/>
+      <c r="G62" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="H62" s="44"/>
+      <c r="I62" s="44"/>
+      <c r="J62" s="44"/>
+      <c r="K62" s="34"/>
+      <c r="L62" s="34"/>
+    </row>
+    <row r="63" spans="2:14">
+      <c r="B63" s="60"/>
+      <c r="C63" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D63" s="43"/>
+      <c r="E63" s="44"/>
+      <c r="F63" s="44"/>
+      <c r="G63" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H63" s="44"/>
+      <c r="I63" s="44"/>
+      <c r="J63" s="44"/>
+      <c r="K63" s="34"/>
+      <c r="L63" s="34"/>
+    </row>
+    <row r="64" spans="2:14">
+      <c r="B64" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="D64" s="43"/>
+      <c r="E64" s="44"/>
+      <c r="F64" s="44"/>
+      <c r="G64" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="H64" s="44"/>
+      <c r="I64" s="44"/>
+      <c r="J64" s="44"/>
+      <c r="K64" s="34"/>
+      <c r="L64" s="34"/>
+    </row>
+    <row r="65" spans="2:12">
+      <c r="B65" s="59"/>
+      <c r="C65" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="D65" s="43"/>
+      <c r="E65" s="44"/>
+      <c r="F65" s="44"/>
+      <c r="G65" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="H65" s="44"/>
+      <c r="I65" s="44"/>
+      <c r="J65" s="44"/>
+      <c r="K65" s="34"/>
+      <c r="L65" s="34"/>
+    </row>
+    <row r="66" spans="2:12">
+      <c r="B66" s="59"/>
+      <c r="C66" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="D66" s="43"/>
+      <c r="E66" s="44"/>
+      <c r="F66" s="44"/>
+      <c r="G66" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="H66" s="44"/>
+      <c r="I66" s="44"/>
+      <c r="J66" s="44"/>
+      <c r="K66" s="34"/>
+      <c r="L66" s="34"/>
+    </row>
+    <row r="67" spans="2:12">
+      <c r="B67" s="59"/>
+      <c r="C67" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="D67" s="43"/>
+      <c r="E67" s="44"/>
+      <c r="F67" s="44"/>
+      <c r="G67" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="H67" s="44"/>
+      <c r="I67" s="44"/>
+      <c r="J67" s="44"/>
+      <c r="K67" s="34"/>
+      <c r="L67" s="34"/>
+    </row>
+    <row r="68" spans="2:12">
+      <c r="B68" s="60"/>
+      <c r="C68" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="D68" s="43"/>
+      <c r="E68" s="44"/>
+      <c r="F68" s="44"/>
+      <c r="G68" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H68" s="44"/>
+      <c r="I68" s="44"/>
+      <c r="J68" s="44"/>
+      <c r="K68" s="34"/>
+      <c r="L68" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="13">
+    <mergeCell ref="B55:B59"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="B64:B68"/>
+    <mergeCell ref="B36:B37"/>
     <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B40:B44"/>
+    <mergeCell ref="B45:B49"/>
+    <mergeCell ref="B50:B54"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="B10:B18"/>
     <mergeCell ref="B19:B24"/>
@@ -3048,5 +3682,6 @@
     <oddFooter>&amp;L&amp;"Times New Roman,Regular"&amp;8&amp;F&amp;C&amp;"Times New Roman,Regular"&amp;8Page &amp;P of &amp;N
 &amp;"Times New Roman,Italic"writeresult Proprietary Confidential - For authorized use only&amp;R&amp;"Times New Roman,Regular"&amp;8Print Date/Time: &amp;D &amp;T</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Form field names added
</commit_message>
<xml_diff>
--- a/Form SpecificationsV0.1_DRAFT.xlsx
+++ b/Form SpecificationsV0.1_DRAFT.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/FabstechTZ/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="0" windowWidth="28540" windowHeight="17660" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="75" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Approval" sheetId="1" r:id="rId1"/>
@@ -20,10 +15,10 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Example!$A$1:$M$6</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Example 2'!$A$1:$M$10</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Functional Specs'!$B$1:$N$9</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Functional Specs'!$B$1:$N$27</definedName>
     <definedName name="Print_Area_0" localSheetId="1">Example!$A$1:$M$6</definedName>
     <definedName name="Print_Area_0" localSheetId="2">'Example 2'!$A$1:$M$10</definedName>
-    <definedName name="Print_Area_0" localSheetId="3">'Functional Specs'!$B$1:$N$9</definedName>
+    <definedName name="Print_Area_0" localSheetId="3">'Functional Specs'!$B$1:$N$27</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Example!$A:$B,Example!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Example 2'!$A:$B,'Example 2'!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'Functional Specs'!$B:$C,'Functional Specs'!$1:$1</definedName>
@@ -31,7 +26,7 @@
     <definedName name="Print_Titles_0" localSheetId="2">'Example 2'!$A:$B,'Example 2'!$1:$1</definedName>
     <definedName name="Print_Titles_0" localSheetId="3">'Functional Specs'!$B:$C,'Functional Specs'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -47,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="205">
   <si>
     <t xml:space="preserve"> Specifications Author:</t>
   </si>
@@ -497,9 +492,6 @@
     <t>Company size</t>
   </si>
   <si>
-    <t>Person name</t>
-  </si>
-  <si>
     <t>Phone</t>
   </si>
   <si>
@@ -569,14 +561,164 @@
     <t>link to Facebook addin Code</t>
   </si>
   <si>
-    <t>Log in</t>
+    <t>user_name</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>school_name</t>
+  </si>
+  <si>
+    <t>graduate_year</t>
+  </si>
+  <si>
+    <t>award</t>
+  </si>
+  <si>
+    <t>education_level</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>work_experience</t>
+  </si>
+  <si>
+    <t>resume</t>
+  </si>
+  <si>
+    <t>job_title</t>
+  </si>
+  <si>
+    <t>job_location</t>
+  </si>
+  <si>
+    <t>search_job</t>
+  </si>
+  <si>
+    <t>company_or_job</t>
+  </si>
+  <si>
+    <t>search-salary</t>
+  </si>
+  <si>
+    <t>company_name</t>
+  </si>
+  <si>
+    <t>search_company</t>
+  </si>
+  <si>
+    <t>company_size</t>
+  </si>
+  <si>
+    <t>Person full name</t>
+  </si>
+  <si>
+    <t>person_name</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>job_type</t>
+  </si>
+  <si>
+    <t>job_salry</t>
+  </si>
+  <si>
+    <t>salry_time_range</t>
+  </si>
+  <si>
+    <t>application_media</t>
+  </si>
+  <si>
+    <t>application_email</t>
+  </si>
+  <si>
+    <t>job_description</t>
+  </si>
+  <si>
+    <t>education</t>
+  </si>
+  <si>
+    <t>experience</t>
+  </si>
+  <si>
+    <t>post_job</t>
+  </si>
+  <si>
+    <t>aboutus_spread_way</t>
+  </si>
+  <si>
+    <t>Signup page</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>Repeat password</t>
+  </si>
+  <si>
+    <t>P.O.Box</t>
+  </si>
+  <si>
+    <t>Settlement</t>
+  </si>
+  <si>
+    <t>Physical  home address</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>birth_date</t>
+  </si>
+  <si>
+    <t>natonality</t>
+  </si>
+  <si>
+    <t>settlement</t>
+  </si>
+  <si>
+    <t>education-level</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>home_address</t>
+  </si>
+  <si>
+    <t>post_office_box</t>
+  </si>
+  <si>
+    <t>repeat_password</t>
+  </si>
+  <si>
+    <t>signup</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -698,6 +840,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -809,7 +957,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -927,9 +1075,6 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -942,6 +1087,33 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -951,33 +1123,21 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1317,38 +1477,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" customWidth="1"/>
-    <col min="6" max="1025" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" customWidth="1"/>
+    <col min="6" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="22.5">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="1"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="30.6" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1365,7 +1525,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" s="8" customFormat="1">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
         <v>5</v>
@@ -1380,7 +1540,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -1389,42 +1549,42 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="22.35" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1439,7 +1599,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" s="8" customFormat="1">
       <c r="A11" s="6"/>
       <c r="B11" s="7" t="s">
         <v>5</v>
@@ -1454,7 +1614,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" s="8" customFormat="1">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1463,28 +1623,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="13"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
         <v>10</v>
       </c>
@@ -1499,7 +1659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" s="6"/>
       <c r="B19" s="7" t="s">
         <v>5</v>
@@ -1514,7 +1674,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1523,7 +1683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -1543,7 +1703,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1553,24 +1713,24 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="17" customWidth="1"/>
-    <col min="4" max="5" width="20.33203125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="18" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="16" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="17" customWidth="1"/>
+    <col min="4" max="5" width="20.28515625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="16" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="18" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="18" customWidth="1"/>
     <col min="10" max="10" width="14" style="19" customWidth="1"/>
-    <col min="11" max="11" width="24.1640625" style="20" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" style="20" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" style="20" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" style="20" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="18" hidden="1" customWidth="1"/>
-    <col min="14" max="1025" width="21.6640625" customWidth="1"/>
+    <col min="14" max="1025" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="24" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="24" customFormat="1" ht="84.75" customHeight="1">
       <c r="A1" s="21" t="s">
         <v>13</v>
       </c>
@@ -1611,7 +1771,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="32" customFormat="1" ht="91" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="32" customFormat="1" ht="89.25">
       <c r="A2" s="25" t="s">
         <v>26</v>
       </c>
@@ -1652,7 +1812,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="32" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" s="32" customFormat="1" ht="27.95" customHeight="1">
       <c r="A3" s="25" t="s">
         <v>33</v>
       </c>
@@ -1689,7 +1849,7 @@
       <c r="L3" s="30"/>
       <c r="M3" s="31"/>
     </row>
-    <row r="4" spans="1:13" s="35" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="35" customFormat="1" ht="23.1" customHeight="1">
       <c r="A4" s="47" t="s">
         <v>41</v>
       </c>
@@ -1730,7 +1890,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="35" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="35" customFormat="1" ht="24" customHeight="1">
       <c r="A5" s="47"/>
       <c r="B5" s="33" t="s">
         <v>47</v>
@@ -1769,7 +1929,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="37" customFormat="1" ht="65" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="37" customFormat="1" ht="76.5">
       <c r="A6" s="28" t="s">
         <v>50</v>
       </c>
@@ -1824,7 +1984,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1834,24 +1994,24 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="17" customWidth="1"/>
-    <col min="4" max="5" width="20.33203125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="18" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="16" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="17" customWidth="1"/>
+    <col min="4" max="5" width="20.28515625" style="18" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="16" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="16" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="18" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="18" customWidth="1"/>
     <col min="10" max="10" width="14" style="19" customWidth="1"/>
-    <col min="11" max="11" width="24.1640625" style="20" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" style="20" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" style="20" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" style="20" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="18" hidden="1" customWidth="1"/>
-    <col min="14" max="1025" width="21.6640625" customWidth="1"/>
+    <col min="14" max="1025" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="24" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="24" customFormat="1" ht="63.75">
       <c r="A1" s="21" t="s">
         <v>13</v>
       </c>
@@ -1892,7 +2052,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="32" customFormat="1" ht="91" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="32" customFormat="1" ht="89.25">
       <c r="A2" s="25" t="s">
         <v>26</v>
       </c>
@@ -1933,7 +2093,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="35" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" s="35" customFormat="1" ht="21.95" customHeight="1">
       <c r="A3" s="47" t="s">
         <v>54</v>
       </c>
@@ -1974,7 +2134,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="35" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="35" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="47"/>
       <c r="B4" s="33" t="s">
         <v>56</v>
@@ -2013,7 +2173,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="35" customFormat="1" ht="182" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="35" customFormat="1" ht="178.5">
       <c r="A5" s="47"/>
       <c r="B5" s="38" t="s">
         <v>57</v>
@@ -2052,7 +2212,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="35" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="35" customFormat="1" ht="63.75">
       <c r="A6" s="28" t="s">
         <v>61</v>
       </c>
@@ -2093,7 +2253,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="35" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="35" customFormat="1" ht="51">
       <c r="A7" s="28" t="s">
         <v>71</v>
       </c>
@@ -2134,7 +2294,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="35" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="35" customFormat="1" ht="23.1" customHeight="1">
       <c r="A8" s="47" t="s">
         <v>41</v>
       </c>
@@ -2175,7 +2335,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="35" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" s="35" customFormat="1" ht="24" customHeight="1">
       <c r="A9" s="47"/>
       <c r="B9" s="33" t="s">
         <v>47</v>
@@ -2214,7 +2374,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="37" customFormat="1" ht="65" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" s="37" customFormat="1" ht="76.5">
       <c r="A10" s="28" t="s">
         <v>50</v>
       </c>
@@ -2270,35 +2430,35 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:N68"/>
+  <dimension ref="B1:N86"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="19" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="19" customWidth="1"/>
     <col min="3" max="3" width="33" style="19" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" style="40" customWidth="1"/>
-    <col min="5" max="6" width="20.33203125" style="18" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="18" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="18" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="18" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" style="40" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="18" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="18" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="18" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="18" customWidth="1"/>
     <col min="11" max="11" width="14" style="19" customWidth="1"/>
-    <col min="12" max="12" width="24.1640625" style="19" customWidth="1"/>
-    <col min="13" max="13" width="21.6640625" style="19" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" style="19" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" style="19" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="13" style="18" hidden="1" customWidth="1"/>
-    <col min="15" max="1026" width="21.6640625" customWidth="1"/>
+    <col min="15" max="1026" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" s="24" customFormat="1" ht="65" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:14" s="24" customFormat="1" ht="76.5">
       <c r="B1" s="41" t="s">
         <v>13</v>
       </c>
@@ -2339,14 +2499,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="48" t="s">
+    <row r="2" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B2" s="56" t="s">
         <v>94</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="27"/>
+      <c r="D2" s="27" t="s">
+        <v>30</v>
+      </c>
       <c r="E2" s="33" t="s">
         <v>30</v>
       </c>
@@ -2366,14 +2528,16 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="49"/>
+    <row r="3" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B3" s="57"/>
       <c r="C3" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="27"/>
+      <c r="D3" s="27" t="s">
+        <v>154</v>
+      </c>
       <c r="E3" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F3" s="28"/>
       <c r="G3" s="33" t="s">
@@ -2392,14 +2556,16 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="49"/>
+    <row r="4" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B4" s="57"/>
       <c r="C4" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="27"/>
+      <c r="D4" s="27" t="s">
+        <v>155</v>
+      </c>
       <c r="E4" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="33" t="s">
@@ -2417,12 +2583,14 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="49"/>
+    <row r="5" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B5" s="57"/>
       <c r="C5" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="D5" s="27"/>
+        <v>150</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>156</v>
+      </c>
       <c r="E5" s="33" t="s">
         <v>30</v>
       </c>
@@ -2436,14 +2604,16 @@
       <c r="K5" s="28"/>
       <c r="L5" s="28"/>
     </row>
-    <row r="6" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="49"/>
+    <row r="6" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B6" s="57"/>
       <c r="C6" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="27"/>
+      <c r="D6" s="27" t="s">
+        <v>30</v>
+      </c>
       <c r="E6" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F6" s="28"/>
       <c r="G6" s="33" t="s">
@@ -2455,14 +2625,16 @@
       <c r="K6" s="28"/>
       <c r="L6" s="28"/>
     </row>
-    <row r="7" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="49"/>
+    <row r="7" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B7" s="57"/>
       <c r="C7" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="27"/>
+      <c r="D7" s="27" t="s">
+        <v>30</v>
+      </c>
       <c r="E7" s="33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="33" t="s">
@@ -2474,12 +2646,14 @@
       <c r="K7" s="28"/>
       <c r="L7" s="28"/>
     </row>
-    <row r="8" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="49"/>
+    <row r="8" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B8" s="57"/>
       <c r="C8" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="27"/>
+      <c r="D8" s="27" t="s">
+        <v>30</v>
+      </c>
       <c r="E8" s="33"/>
       <c r="F8" s="28"/>
       <c r="G8" s="33" t="s">
@@ -2491,400 +2665,428 @@
       <c r="K8" s="28"/>
       <c r="L8" s="28"/>
     </row>
-    <row r="9" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="50"/>
-      <c r="C9" s="34" t="s">
+    <row r="9" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B9" s="57"/>
+      <c r="C9" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="33" t="s">
+      <c r="D9" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="33"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+    </row>
+    <row r="10" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B10" s="61" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10" s="33"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+    </row>
+    <row r="11" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B11" s="62"/>
+      <c r="C11" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="33"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+    </row>
+    <row r="12" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B12" s="62"/>
+      <c r="C12" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="E12" s="33"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46"/>
+    </row>
+    <row r="13" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B13" s="62"/>
+      <c r="C13" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="E13" s="33"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
+    </row>
+    <row r="14" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B14" s="62"/>
+      <c r="C14" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14" s="33"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="46"/>
+    </row>
+    <row r="15" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B15" s="62"/>
+      <c r="C15" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="E15" s="33"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+    </row>
+    <row r="16" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B16" s="62"/>
+      <c r="C16" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="E16" s="33"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="46"/>
+    </row>
+    <row r="17" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B17" s="62"/>
+      <c r="C17" s="64" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="E17" s="33"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+    </row>
+    <row r="18" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B18" s="62"/>
+      <c r="C18" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="33"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+    </row>
+    <row r="19" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B19" s="62"/>
+      <c r="C19" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="E19" s="33"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+    </row>
+    <row r="20" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B20" s="62"/>
+      <c r="C20" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="E20" s="33"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+    </row>
+    <row r="21" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B21" s="62"/>
+      <c r="C21" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="E21" s="33"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+    </row>
+    <row r="22" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B22" s="62"/>
+      <c r="C22" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="E22" s="33"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+    </row>
+    <row r="23" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B23" s="62"/>
+      <c r="C23" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="E23" s="33"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+    </row>
+    <row r="24" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B24" s="62"/>
+      <c r="C24" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="E24" s="33"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+    </row>
+    <row r="25" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B25" s="62"/>
+      <c r="C25" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="33" t="s">
+      <c r="E25" s="33"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+    </row>
+    <row r="26" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B26" s="62"/>
+      <c r="C26" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="E26" s="33"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+    </row>
+    <row r="27" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B27" s="63"/>
+      <c r="C27" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="E27" s="33"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="N9" s="35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="48" t="s">
-        <v>106</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-    </row>
-    <row r="11" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="49"/>
-      <c r="C11" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-    </row>
-    <row r="12" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="49"/>
-      <c r="C12" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="18"/>
-    </row>
-    <row r="13" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="49"/>
-      <c r="C13" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="18"/>
-    </row>
-    <row r="14" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="49"/>
-      <c r="C14" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="18"/>
-    </row>
-    <row r="15" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="49"/>
-      <c r="C15" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="18"/>
-    </row>
-    <row r="16" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="49"/>
-      <c r="C16" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="D16" s="43"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="18"/>
-    </row>
-    <row r="17" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="49"/>
-      <c r="C17" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="D17" s="43"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="18"/>
-    </row>
-    <row r="18" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="50"/>
-      <c r="C18" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="D18" s="43"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="18"/>
-    </row>
-    <row r="19" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="51" t="s">
-        <v>107</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="D19" s="43"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="18"/>
-    </row>
-    <row r="20" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="52"/>
-      <c r="C20" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="43"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="18"/>
-    </row>
-    <row r="21" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="52"/>
-      <c r="C21" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="D21" s="43"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="18"/>
-    </row>
-    <row r="22" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="52"/>
-      <c r="C22" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" s="43"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="18"/>
-    </row>
-    <row r="23" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="52"/>
-      <c r="C23" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="D23" s="43"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="18"/>
-    </row>
-    <row r="24" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="53"/>
-      <c r="C24" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="D24" s="43"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="18"/>
-    </row>
-    <row r="25" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="54" t="s">
-        <v>113</v>
-      </c>
-      <c r="C25" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="D25" s="43"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="18"/>
-    </row>
-    <row r="26" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="55"/>
-      <c r="C26" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="43"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="18"/>
-    </row>
-    <row r="27" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="55"/>
-      <c r="C27" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="D27" s="43"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
       <c r="H27" s="28"/>
       <c r="I27" s="28"/>
       <c r="J27" s="28"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="18"/>
-    </row>
-    <row r="28" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="55"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="N27" s="35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B28" s="56" t="s">
+        <v>106</v>
+      </c>
       <c r="C28" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="43"/>
-      <c r="E28" s="28"/>
+        <v>96</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="33"/>
       <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
+      <c r="G28" s="33" t="s">
+        <v>93</v>
+      </c>
       <c r="H28" s="28"/>
       <c r="I28" s="28"/>
       <c r="J28" s="28"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="18"/>
-    </row>
-    <row r="29" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="55"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+    </row>
+    <row r="29" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B29" s="57"/>
       <c r="C29" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="D29" s="43"/>
-      <c r="E29" s="28"/>
+        <v>97</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="33"/>
       <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
+      <c r="G29" s="33" t="s">
+        <v>102</v>
+      </c>
       <c r="H29" s="28"/>
       <c r="I29" s="28"/>
       <c r="J29" s="28"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="34"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="18"/>
-    </row>
-    <row r="30" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="55"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+    </row>
+    <row r="30" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B30" s="57"/>
       <c r="C30" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="D30" s="43"/>
+        <v>80</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>30</v>
+      </c>
       <c r="E30" s="28"/>
       <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
+      <c r="G30" s="28" t="s">
+        <v>30</v>
+      </c>
       <c r="H30" s="28"/>
       <c r="I30" s="28"/>
       <c r="J30" s="28"/>
@@ -2893,15 +3095,19 @@
       <c r="M30" s="19"/>
       <c r="N30" s="18"/>
     </row>
-    <row r="31" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="55"/>
+    <row r="31" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B31" s="57"/>
       <c r="C31" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="D31" s="43"/>
+        <v>78</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>30</v>
+      </c>
       <c r="E31" s="28"/>
       <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
+      <c r="G31" s="28" t="s">
+        <v>30</v>
+      </c>
       <c r="H31" s="28"/>
       <c r="I31" s="28"/>
       <c r="J31" s="28"/>
@@ -2910,15 +3116,19 @@
       <c r="M31" s="19"/>
       <c r="N31" s="18"/>
     </row>
-    <row r="32" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="56"/>
+    <row r="32" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B32" s="57"/>
       <c r="C32" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="D32" s="43"/>
+        <v>98</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>30</v>
+      </c>
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
-      <c r="G32" s="33"/>
+      <c r="G32" s="28" t="s">
+        <v>30</v>
+      </c>
       <c r="H32" s="28"/>
       <c r="I32" s="28"/>
       <c r="J32" s="28"/>
@@ -2927,18 +3137,18 @@
       <c r="M32" s="19"/>
       <c r="N32" s="18"/>
     </row>
-    <row r="33" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="51" t="s">
-        <v>118</v>
-      </c>
+    <row r="33" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B33" s="57"/>
       <c r="C33" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="D33" s="43"/>
+        <v>79</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>30</v>
+      </c>
       <c r="E33" s="28"/>
       <c r="F33" s="28"/>
-      <c r="G33" s="33" t="s">
-        <v>120</v>
+      <c r="G33" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="H33" s="28"/>
       <c r="I33" s="28"/>
@@ -2948,16 +3158,18 @@
       <c r="M33" s="19"/>
       <c r="N33" s="18"/>
     </row>
-    <row r="34" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="B34" s="57"/>
       <c r="C34" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="D34" s="43"/>
+        <v>99</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>30</v>
+      </c>
       <c r="E34" s="28"/>
       <c r="F34" s="28"/>
-      <c r="G34" s="33" t="s">
-        <v>120</v>
+      <c r="G34" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="H34" s="28"/>
       <c r="I34" s="28"/>
@@ -2967,16 +3179,18 @@
       <c r="M34" s="19"/>
       <c r="N34" s="18"/>
     </row>
-    <row r="35" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
       <c r="B35" s="57"/>
       <c r="C35" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="D35" s="43"/>
+        <v>101</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>30</v>
+      </c>
       <c r="E35" s="28"/>
       <c r="F35" s="28"/>
-      <c r="G35" s="33" t="s">
-        <v>44</v>
+      <c r="G35" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="H35" s="28"/>
       <c r="I35" s="28"/>
@@ -2986,18 +3200,18 @@
       <c r="M35" s="19"/>
       <c r="N35" s="18"/>
     </row>
-    <row r="36" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="51" t="s">
-        <v>117</v>
-      </c>
-      <c r="C36" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="D36" s="43"/>
+    <row r="36" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B36" s="58"/>
+      <c r="C36" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="27" t="s">
+        <v>30</v>
+      </c>
       <c r="E36" s="28"/>
       <c r="F36" s="28"/>
-      <c r="G36" s="33" t="s">
-        <v>120</v>
+      <c r="G36" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="H36" s="28"/>
       <c r="I36" s="28"/>
@@ -3007,17 +3221,17 @@
       <c r="M36" s="19"/>
       <c r="N36" s="18"/>
     </row>
-    <row r="37" spans="2:14" s="35" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="53"/>
-      <c r="C37" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="D37" s="43"/>
+    <row r="37" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B37" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="27"/>
       <c r="E37" s="28"/>
       <c r="F37" s="28"/>
-      <c r="G37" s="33" t="s">
-        <v>44</v>
-      </c>
+      <c r="G37" s="46"/>
       <c r="H37" s="28"/>
       <c r="I37" s="28"/>
       <c r="J37" s="28"/>
@@ -3026,554 +3240,965 @@
       <c r="M37" s="19"/>
       <c r="N37" s="18"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B38" s="54" t="s">
-        <v>121</v>
-      </c>
+    <row r="38" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B38" s="59"/>
       <c r="C38" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="D38" s="43"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="H38" s="44"/>
-      <c r="I38" s="44"/>
-      <c r="J38" s="44"/>
+        <v>103</v>
+      </c>
+      <c r="D38" s="27"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
       <c r="K38" s="34"/>
       <c r="L38" s="34"/>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B39" s="55"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="18"/>
+    </row>
+    <row r="39" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B39" s="59"/>
       <c r="C39" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="D39" s="43"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="H39" s="44"/>
-      <c r="I39" s="44"/>
-      <c r="J39" s="44"/>
+        <v>98</v>
+      </c>
+      <c r="D39" s="27"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="28"/>
+      <c r="J39" s="28"/>
       <c r="K39" s="34"/>
       <c r="L39" s="34"/>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B40" s="54" t="s">
-        <v>123</v>
-      </c>
-      <c r="C40" s="46" t="s">
-        <v>124</v>
-      </c>
-      <c r="D40" s="43"/>
-      <c r="E40" s="44"/>
-      <c r="F40" s="44"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="18"/>
+    </row>
+    <row r="40" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B40" s="59"/>
+      <c r="C40" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="27"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="28"/>
+      <c r="J40" s="28"/>
       <c r="K40" s="34"/>
       <c r="L40" s="34"/>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B41" s="55"/>
-      <c r="C41" s="46" t="s">
-        <v>125</v>
-      </c>
-      <c r="D41" s="43"/>
-      <c r="E41" s="44"/>
-      <c r="F41" s="44"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="44"/>
-      <c r="I41" s="44"/>
-      <c r="J41" s="44"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="18"/>
+    </row>
+    <row r="41" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B41" s="59"/>
+      <c r="C41" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="D41" s="27"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="28"/>
       <c r="K41" s="34"/>
       <c r="L41" s="34"/>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B42" s="55"/>
-      <c r="C42" s="46" t="s">
-        <v>126</v>
-      </c>
-      <c r="D42" s="43"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="18"/>
+    </row>
+    <row r="42" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B42" s="52"/>
+      <c r="C42" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="D42" s="27"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="28"/>
+      <c r="J42" s="28"/>
       <c r="K42" s="34"/>
       <c r="L42" s="34"/>
-    </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B43" s="55"/>
-      <c r="C43" s="46" t="s">
-        <v>127</v>
-      </c>
-      <c r="D43" s="43"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="18"/>
+    </row>
+    <row r="43" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B43" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="28"/>
+      <c r="J43" s="28"/>
       <c r="K43" s="34"/>
       <c r="L43" s="34"/>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B44" s="56"/>
-      <c r="C44" s="46" t="s">
-        <v>128</v>
-      </c>
-      <c r="D44" s="43"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="33"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="44"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="18"/>
+    </row>
+    <row r="44" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B44" s="54"/>
+      <c r="C44" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="28"/>
       <c r="K44" s="34"/>
       <c r="L44" s="34"/>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B45" s="58" t="s">
-        <v>129</v>
-      </c>
+      <c r="M44" s="19"/>
+      <c r="N44" s="18"/>
+    </row>
+    <row r="45" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B45" s="54"/>
       <c r="C45" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="D45" s="43"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="44"/>
+        <v>108</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
       <c r="K45" s="34"/>
       <c r="L45" s="34"/>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B46" s="59"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="18"/>
+    </row>
+    <row r="46" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B46" s="54"/>
       <c r="C46" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="D46" s="43"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="H46" s="44"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+        <v>84</v>
+      </c>
+      <c r="D46" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="28"/>
+      <c r="I46" s="28"/>
+      <c r="J46" s="28"/>
       <c r="K46" s="34"/>
       <c r="L46" s="34"/>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B47" s="59"/>
+      <c r="M46" s="19"/>
+      <c r="N46" s="18"/>
+    </row>
+    <row r="47" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B47" s="54"/>
       <c r="C47" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="D47" s="43"/>
-      <c r="E47" s="44"/>
-      <c r="F47" s="44"/>
-      <c r="G47" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="H47" s="44"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+        <v>109</v>
+      </c>
+      <c r="D47" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="28"/>
+      <c r="I47" s="28"/>
+      <c r="J47" s="28"/>
       <c r="K47" s="34"/>
       <c r="L47" s="34"/>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B48" s="59"/>
+      <c r="M47" s="19"/>
+      <c r="N47" s="18"/>
+    </row>
+    <row r="48" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B48" s="54"/>
       <c r="C48" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="D48" s="43"/>
-      <c r="E48" s="44"/>
-      <c r="F48" s="44"/>
-      <c r="G48" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="H48" s="44"/>
-      <c r="I48" s="44"/>
-      <c r="J48" s="44"/>
+        <v>111</v>
+      </c>
+      <c r="D48" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="28"/>
+      <c r="H48" s="28"/>
+      <c r="I48" s="28"/>
+      <c r="J48" s="28"/>
       <c r="K48" s="34"/>
       <c r="L48" s="34"/>
-    </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B49" s="59"/>
+      <c r="M48" s="19"/>
+      <c r="N48" s="18"/>
+    </row>
+    <row r="49" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B49" s="54"/>
       <c r="C49" s="34" t="s">
-        <v>141</v>
-      </c>
-      <c r="D49" s="43"/>
-      <c r="E49" s="44"/>
-      <c r="F49" s="44"/>
-      <c r="G49" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="H49" s="44"/>
-      <c r="I49" s="44"/>
-      <c r="J49" s="44"/>
+        <v>112</v>
+      </c>
+      <c r="D49" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="28"/>
+      <c r="I49" s="28"/>
+      <c r="J49" s="28"/>
       <c r="K49" s="34"/>
       <c r="L49" s="34"/>
-      <c r="M49"/>
-      <c r="N49"/>
-    </row>
-    <row r="50" spans="2:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="58" t="s">
-        <v>134</v>
-      </c>
+      <c r="M49" s="19"/>
+      <c r="N49" s="18"/>
+    </row>
+    <row r="50" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B50" s="55"/>
       <c r="C50" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="D50" s="43"/>
-      <c r="E50" s="44"/>
-      <c r="F50" s="44"/>
-      <c r="G50" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="H50" s="44"/>
-      <c r="I50" s="44"/>
-      <c r="J50" s="44"/>
+        <v>110</v>
+      </c>
+      <c r="D50" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="28"/>
+      <c r="J50" s="28"/>
       <c r="K50" s="34"/>
       <c r="L50" s="34"/>
-    </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B51" s="59"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="18"/>
+    </row>
+    <row r="51" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B51" s="51" t="s">
+        <v>118</v>
+      </c>
       <c r="C51" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="D51" s="43"/>
-      <c r="E51" s="44"/>
-      <c r="F51" s="44"/>
+        <v>114</v>
+      </c>
+      <c r="D51" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
       <c r="G51" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="H51" s="44"/>
-      <c r="I51" s="44"/>
-      <c r="J51" s="44"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="28"/>
+      <c r="J51" s="28"/>
       <c r="K51" s="34"/>
       <c r="L51" s="34"/>
-    </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B52" s="59"/>
+      <c r="M51" s="19"/>
+      <c r="N51" s="18"/>
+    </row>
+    <row r="52" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B52" s="60"/>
       <c r="C52" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D52" s="43"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="44"/>
+        <v>115</v>
+      </c>
+      <c r="D52" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
       <c r="G52" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="H52" s="44"/>
-      <c r="I52" s="44"/>
-      <c r="J52" s="44"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="28"/>
+      <c r="J52" s="28"/>
       <c r="K52" s="34"/>
       <c r="L52" s="34"/>
-    </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B53" s="59"/>
+      <c r="M52" s="19"/>
+      <c r="N52" s="18"/>
+    </row>
+    <row r="53" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B53" s="60"/>
       <c r="C53" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="D53" s="43"/>
-      <c r="E53" s="44"/>
-      <c r="F53" s="44"/>
+        <v>116</v>
+      </c>
+      <c r="D53" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="E53" s="28"/>
+      <c r="F53" s="28"/>
       <c r="G53" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="H53" s="44"/>
-      <c r="I53" s="44"/>
-      <c r="J53" s="44"/>
+      <c r="H53" s="28"/>
+      <c r="I53" s="28"/>
+      <c r="J53" s="28"/>
       <c r="K53" s="34"/>
       <c r="L53" s="34"/>
-    </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B54" s="60"/>
-      <c r="C54" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="D54" s="43"/>
-      <c r="E54" s="44"/>
-      <c r="F54" s="44"/>
+      <c r="M53" s="19"/>
+      <c r="N53" s="18"/>
+    </row>
+    <row r="54" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B54" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="C54" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="D54" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28"/>
       <c r="G54" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="H54" s="44"/>
-      <c r="I54" s="44"/>
-      <c r="J54" s="44"/>
+        <v>120</v>
+      </c>
+      <c r="H54" s="28"/>
+      <c r="I54" s="28"/>
+      <c r="J54" s="28"/>
       <c r="K54" s="34"/>
       <c r="L54" s="34"/>
-    </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B55" s="58" t="s">
-        <v>139</v>
-      </c>
-      <c r="C55" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="D55" s="43"/>
-      <c r="E55" s="44"/>
-      <c r="F55" s="44"/>
+      <c r="M54" s="19"/>
+      <c r="N54" s="18"/>
+    </row>
+    <row r="55" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B55" s="52"/>
+      <c r="C55" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="D55" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28"/>
       <c r="G55" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="H55" s="44"/>
-      <c r="I55" s="44"/>
-      <c r="J55" s="44"/>
+        <v>44</v>
+      </c>
+      <c r="H55" s="28"/>
+      <c r="I55" s="28"/>
+      <c r="J55" s="28"/>
       <c r="K55" s="34"/>
       <c r="L55" s="34"/>
-    </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B56" s="59"/>
+      <c r="M55" s="19"/>
+      <c r="N55" s="18"/>
+    </row>
+    <row r="56" spans="2:14">
+      <c r="B56" s="53" t="s">
+        <v>121</v>
+      </c>
       <c r="C56" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="D56" s="43"/>
-      <c r="E56" s="44"/>
-      <c r="F56" s="44"/>
+        <v>122</v>
+      </c>
+      <c r="D56" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="E56" s="43"/>
+      <c r="F56" s="43"/>
       <c r="G56" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="H56" s="44"/>
-      <c r="I56" s="44"/>
-      <c r="J56" s="44"/>
+      <c r="H56" s="43"/>
+      <c r="I56" s="43"/>
+      <c r="J56" s="43"/>
       <c r="K56" s="34"/>
       <c r="L56" s="34"/>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B57" s="59"/>
+    <row r="57" spans="2:14">
+      <c r="B57" s="54"/>
       <c r="C57" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="D57" s="43"/>
-      <c r="E57" s="44"/>
-      <c r="F57" s="44"/>
+        <v>116</v>
+      </c>
+      <c r="D57" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
       <c r="G57" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="H57" s="44"/>
-      <c r="I57" s="44"/>
-      <c r="J57" s="44"/>
+        <v>44</v>
+      </c>
+      <c r="H57" s="43"/>
+      <c r="I57" s="43"/>
+      <c r="J57" s="43"/>
       <c r="K57" s="34"/>
       <c r="L57" s="34"/>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B58" s="59"/>
-      <c r="C58" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="D58" s="43"/>
-      <c r="E58" s="44"/>
-      <c r="F58" s="44"/>
-      <c r="G58" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="H58" s="44"/>
-      <c r="I58" s="44"/>
-      <c r="J58" s="44"/>
+    <row r="58" spans="2:14">
+      <c r="B58" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="D58" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E58" s="43"/>
+      <c r="F58" s="43"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="43"/>
+      <c r="I58" s="43"/>
+      <c r="J58" s="43"/>
       <c r="K58" s="34"/>
       <c r="L58" s="34"/>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B59" s="60"/>
-      <c r="C59" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="D59" s="43"/>
-      <c r="E59" s="44"/>
-      <c r="F59" s="44"/>
-      <c r="G59" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="H59" s="44"/>
-      <c r="I59" s="44"/>
-      <c r="J59" s="44"/>
+    <row r="59" spans="2:14">
+      <c r="B59" s="54"/>
+      <c r="C59" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="D59" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E59" s="43"/>
+      <c r="F59" s="43"/>
+      <c r="G59" s="33"/>
+      <c r="H59" s="43"/>
+      <c r="I59" s="43"/>
+      <c r="J59" s="43"/>
       <c r="K59" s="34"/>
       <c r="L59" s="34"/>
     </row>
-    <row r="60" spans="2:14" ht="26" x14ac:dyDescent="0.2">
-      <c r="B60" s="58" t="s">
-        <v>127</v>
-      </c>
-      <c r="C60" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="D60" s="43"/>
-      <c r="E60" s="44"/>
-      <c r="F60" s="44"/>
-      <c r="G60" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="H60" s="44"/>
-      <c r="I60" s="44"/>
-      <c r="J60" s="44"/>
+    <row r="60" spans="2:14">
+      <c r="B60" s="54"/>
+      <c r="C60" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="D60" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E60" s="43"/>
+      <c r="F60" s="43"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="43"/>
+      <c r="I60" s="43"/>
+      <c r="J60" s="43"/>
       <c r="K60" s="34"/>
       <c r="L60" s="34"/>
     </row>
-    <row r="61" spans="2:14" ht="26" x14ac:dyDescent="0.2">
-      <c r="B61" s="59"/>
-      <c r="C61" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="D61" s="43"/>
-      <c r="E61" s="44"/>
-      <c r="F61" s="44"/>
-      <c r="G61" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="H61" s="44"/>
-      <c r="I61" s="44"/>
-      <c r="J61" s="44"/>
+    <row r="61" spans="2:14">
+      <c r="B61" s="54"/>
+      <c r="C61" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="D61" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E61" s="43"/>
+      <c r="F61" s="43"/>
+      <c r="G61" s="33"/>
+      <c r="H61" s="43"/>
+      <c r="I61" s="43"/>
+      <c r="J61" s="43"/>
       <c r="K61" s="34"/>
       <c r="L61" s="34"/>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B62" s="59"/>
-      <c r="C62" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="D62" s="43"/>
-      <c r="E62" s="44"/>
-      <c r="F62" s="44"/>
-      <c r="G62" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="H62" s="44"/>
-      <c r="I62" s="44"/>
-      <c r="J62" s="44"/>
+    <row r="62" spans="2:14">
+      <c r="B62" s="55"/>
+      <c r="C62" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="D62" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E62" s="43"/>
+      <c r="F62" s="43"/>
+      <c r="G62" s="33"/>
+      <c r="H62" s="43"/>
+      <c r="I62" s="43"/>
+      <c r="J62" s="43"/>
       <c r="K62" s="34"/>
       <c r="L62" s="34"/>
     </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B63" s="60"/>
+    <row r="63" spans="2:14">
+      <c r="B63" s="48" t="s">
+        <v>129</v>
+      </c>
       <c r="C63" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="D63" s="43"/>
-      <c r="E63" s="44"/>
-      <c r="F63" s="44"/>
+        <v>122</v>
+      </c>
+      <c r="D63" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="E63" s="43"/>
+      <c r="F63" s="43"/>
       <c r="G63" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="H63" s="44"/>
-      <c r="I63" s="44"/>
-      <c r="J63" s="44"/>
+        <v>120</v>
+      </c>
+      <c r="H63" s="43"/>
+      <c r="I63" s="43"/>
+      <c r="J63" s="43"/>
       <c r="K63" s="34"/>
       <c r="L63" s="34"/>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B64" s="58" t="s">
-        <v>128</v>
-      </c>
+    <row r="64" spans="2:14">
+      <c r="B64" s="49"/>
       <c r="C64" s="34" t="s">
-        <v>128</v>
-      </c>
-      <c r="D64" s="43"/>
-      <c r="E64" s="44"/>
-      <c r="F64" s="44"/>
+        <v>130</v>
+      </c>
+      <c r="D64" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="E64" s="43"/>
+      <c r="F64" s="43"/>
       <c r="G64" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="H64" s="44"/>
-      <c r="I64" s="44"/>
-      <c r="J64" s="44"/>
+        <v>120</v>
+      </c>
+      <c r="H64" s="43"/>
+      <c r="I64" s="43"/>
+      <c r="J64" s="43"/>
       <c r="K64" s="34"/>
       <c r="L64" s="34"/>
     </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B65" s="59"/>
+    <row r="65" spans="2:14">
+      <c r="B65" s="49"/>
       <c r="C65" s="34" t="s">
-        <v>148</v>
-      </c>
-      <c r="D65" s="43"/>
-      <c r="E65" s="44"/>
-      <c r="F65" s="44"/>
+        <v>173</v>
+      </c>
+      <c r="D65" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="E65" s="43"/>
+      <c r="F65" s="43"/>
       <c r="G65" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="H65" s="44"/>
-      <c r="I65" s="44"/>
-      <c r="J65" s="44"/>
+        <v>120</v>
+      </c>
+      <c r="H65" s="43"/>
+      <c r="I65" s="43"/>
+      <c r="J65" s="43"/>
       <c r="K65" s="34"/>
       <c r="L65" s="34"/>
     </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B66" s="59"/>
+    <row r="66" spans="2:14">
+      <c r="B66" s="49"/>
       <c r="C66" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="D66" s="43"/>
-      <c r="E66" s="44"/>
-      <c r="F66" s="44"/>
+        <v>131</v>
+      </c>
+      <c r="D66" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="E66" s="43"/>
+      <c r="F66" s="43"/>
       <c r="G66" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="H66" s="44"/>
-      <c r="I66" s="44"/>
-      <c r="J66" s="44"/>
+        <v>120</v>
+      </c>
+      <c r="H66" s="43"/>
+      <c r="I66" s="43"/>
+      <c r="J66" s="43"/>
       <c r="K66" s="34"/>
       <c r="L66" s="34"/>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B67" s="59"/>
+    <row r="67" spans="2:14" ht="25.5">
+      <c r="B67" s="49"/>
       <c r="C67" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="D67" s="43"/>
-      <c r="E67" s="44"/>
-      <c r="F67" s="44"/>
+        <v>140</v>
+      </c>
+      <c r="D67" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="E67" s="43"/>
+      <c r="F67" s="43"/>
       <c r="G67" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="H67" s="44"/>
-      <c r="I67" s="44"/>
-      <c r="J67" s="44"/>
+        <v>132</v>
+      </c>
+      <c r="H67" s="43"/>
+      <c r="I67" s="43"/>
+      <c r="J67" s="43"/>
       <c r="K67" s="34"/>
       <c r="L67" s="34"/>
-    </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B68" s="60"/>
+      <c r="M67"/>
+      <c r="N67"/>
+    </row>
+    <row r="68" spans="2:14" ht="25.5" customHeight="1">
+      <c r="B68" s="48" t="s">
+        <v>133</v>
+      </c>
       <c r="C68" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="D68" s="43"/>
-      <c r="E68" s="44"/>
-      <c r="F68" s="44"/>
+        <v>114</v>
+      </c>
+      <c r="D68" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="E68" s="43"/>
+      <c r="F68" s="43"/>
       <c r="G68" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="H68" s="44"/>
-      <c r="I68" s="44"/>
-      <c r="J68" s="44"/>
+        <v>120</v>
+      </c>
+      <c r="H68" s="43"/>
+      <c r="I68" s="43"/>
+      <c r="J68" s="43"/>
       <c r="K68" s="34"/>
       <c r="L68" s="34"/>
     </row>
+    <row r="69" spans="2:14">
+      <c r="B69" s="49"/>
+      <c r="C69" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="D69" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="E69" s="43"/>
+      <c r="F69" s="43"/>
+      <c r="G69" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="H69" s="43"/>
+      <c r="I69" s="43"/>
+      <c r="J69" s="43"/>
+      <c r="K69" s="34"/>
+      <c r="L69" s="34"/>
+    </row>
+    <row r="70" spans="2:14">
+      <c r="B70" s="49"/>
+      <c r="C70" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="D70" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="E70" s="43"/>
+      <c r="F70" s="43"/>
+      <c r="G70" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="H70" s="43"/>
+      <c r="I70" s="43"/>
+      <c r="J70" s="43"/>
+      <c r="K70" s="34"/>
+      <c r="L70" s="34"/>
+    </row>
+    <row r="71" spans="2:14">
+      <c r="B71" s="49"/>
+      <c r="C71" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="D71" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E71" s="43"/>
+      <c r="F71" s="43"/>
+      <c r="G71" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H71" s="43"/>
+      <c r="I71" s="43"/>
+      <c r="J71" s="43"/>
+      <c r="K71" s="34"/>
+      <c r="L71" s="34"/>
+    </row>
+    <row r="72" spans="2:14">
+      <c r="B72" s="50"/>
+      <c r="C72" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="D72" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E72" s="43"/>
+      <c r="F72" s="43"/>
+      <c r="G72" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H72" s="43"/>
+      <c r="I72" s="43"/>
+      <c r="J72" s="43"/>
+      <c r="K72" s="34"/>
+      <c r="L72" s="34"/>
+    </row>
+    <row r="73" spans="2:14">
+      <c r="B73" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="C73" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D73" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="E73" s="43"/>
+      <c r="F73" s="43"/>
+      <c r="G73" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="H73" s="43"/>
+      <c r="I73" s="43"/>
+      <c r="J73" s="43"/>
+      <c r="K73" s="34"/>
+      <c r="L73" s="34"/>
+    </row>
+    <row r="74" spans="2:14">
+      <c r="B74" s="49"/>
+      <c r="C74" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="D74" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="E74" s="43"/>
+      <c r="F74" s="43"/>
+      <c r="G74" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="H74" s="43"/>
+      <c r="I74" s="43"/>
+      <c r="J74" s="43"/>
+      <c r="K74" s="34"/>
+      <c r="L74" s="34"/>
+    </row>
+    <row r="75" spans="2:14">
+      <c r="B75" s="49"/>
+      <c r="C75" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="D75" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="E75" s="43"/>
+      <c r="F75" s="43"/>
+      <c r="G75" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="H75" s="43"/>
+      <c r="I75" s="43"/>
+      <c r="J75" s="43"/>
+      <c r="K75" s="34"/>
+      <c r="L75" s="34"/>
+    </row>
+    <row r="76" spans="2:14">
+      <c r="B76" s="49"/>
+      <c r="C76" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="D76" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E76" s="43"/>
+      <c r="F76" s="43"/>
+      <c r="G76" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H76" s="43"/>
+      <c r="I76" s="43"/>
+      <c r="J76" s="43"/>
+      <c r="K76" s="34"/>
+      <c r="L76" s="34"/>
+    </row>
+    <row r="77" spans="2:14">
+      <c r="B77" s="50"/>
+      <c r="C77" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="D77" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E77" s="43"/>
+      <c r="F77" s="43"/>
+      <c r="G77" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H77" s="43"/>
+      <c r="I77" s="43"/>
+      <c r="J77" s="43"/>
+      <c r="K77" s="34"/>
+      <c r="L77" s="34"/>
+    </row>
+    <row r="78" spans="2:14" ht="25.5">
+      <c r="B78" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="C78" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="D78" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="E78" s="43"/>
+      <c r="F78" s="43"/>
+      <c r="G78" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H78" s="43"/>
+      <c r="I78" s="43"/>
+      <c r="J78" s="43"/>
+      <c r="K78" s="34"/>
+      <c r="L78" s="34"/>
+    </row>
+    <row r="79" spans="2:14" ht="25.5">
+      <c r="B79" s="49"/>
+      <c r="C79" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="D79" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="E79" s="43"/>
+      <c r="F79" s="43"/>
+      <c r="G79" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="H79" s="43"/>
+      <c r="I79" s="43"/>
+      <c r="J79" s="43"/>
+      <c r="K79" s="34"/>
+      <c r="L79" s="34"/>
+    </row>
+    <row r="80" spans="2:14">
+      <c r="B80" s="49"/>
+      <c r="C80" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="D80" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E80" s="43"/>
+      <c r="F80" s="43"/>
+      <c r="G80" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="H80" s="43"/>
+      <c r="I80" s="43"/>
+      <c r="J80" s="43"/>
+      <c r="K80" s="34"/>
+      <c r="L80" s="34"/>
+    </row>
+    <row r="81" spans="2:12">
+      <c r="B81" s="50"/>
+      <c r="C81" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="D81" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E81" s="43"/>
+      <c r="F81" s="43"/>
+      <c r="G81" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H81" s="43"/>
+      <c r="I81" s="43"/>
+      <c r="J81" s="43"/>
+      <c r="K81" s="34"/>
+      <c r="L81" s="34"/>
+    </row>
+    <row r="82" spans="2:12">
+      <c r="B82" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="C82" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="D82" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="E82" s="43"/>
+      <c r="F82" s="43"/>
+      <c r="G82" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="H82" s="43"/>
+      <c r="I82" s="43"/>
+      <c r="J82" s="43"/>
+      <c r="K82" s="34"/>
+      <c r="L82" s="34"/>
+    </row>
+    <row r="83" spans="2:12">
+      <c r="B83" s="49"/>
+      <c r="C83" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="D83" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="E83" s="43"/>
+      <c r="F83" s="43"/>
+      <c r="G83" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="H83" s="43"/>
+      <c r="I83" s="43"/>
+      <c r="J83" s="43"/>
+      <c r="K83" s="34"/>
+      <c r="L83" s="34"/>
+    </row>
+    <row r="84" spans="2:12">
+      <c r="B84" s="49"/>
+      <c r="C84" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="D84" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="E84" s="43"/>
+      <c r="F84" s="43"/>
+      <c r="G84" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="H84" s="43"/>
+      <c r="I84" s="43"/>
+      <c r="J84" s="43"/>
+      <c r="K84" s="34"/>
+      <c r="L84" s="34"/>
+    </row>
+    <row r="85" spans="2:12">
+      <c r="B85" s="49"/>
+      <c r="C85" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="D85" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="E85" s="43"/>
+      <c r="F85" s="43"/>
+      <c r="G85" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="H85" s="43"/>
+      <c r="I85" s="43"/>
+      <c r="J85" s="43"/>
+      <c r="K85" s="34"/>
+      <c r="L85" s="34"/>
+    </row>
+    <row r="86" spans="2:12">
+      <c r="B86" s="50"/>
+      <c r="C86" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="D86" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="E86" s="43"/>
+      <c r="F86" s="43"/>
+      <c r="G86" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H86" s="43"/>
+      <c r="I86" s="43"/>
+      <c r="J86" s="43"/>
+      <c r="K86" s="34"/>
+      <c r="L86" s="34"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B55:B59"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="B64:B68"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B44"/>
-    <mergeCell ref="B45:B49"/>
-    <mergeCell ref="B50:B54"/>
+  <mergeCells count="14">
+    <mergeCell ref="B28:B36"/>
+    <mergeCell ref="B37:B42"/>
+    <mergeCell ref="B43:B50"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="B10:B27"/>
     <mergeCell ref="B2:B9"/>
-    <mergeCell ref="B10:B18"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="B25:B32"/>
-    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B73:B77"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B58:B62"/>
+    <mergeCell ref="B63:B67"/>
+    <mergeCell ref="B68:B72"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="1" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Field names and response added, and some other changes
</commit_message>
<xml_diff>
--- a/Form SpecificationsV0.1_DRAFT.xlsx
+++ b/Form SpecificationsV0.1_DRAFT.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="274">
   <si>
     <t xml:space="preserve"> Specifications Author:</t>
   </si>
@@ -381,9 +381,6 @@
     <t>Link</t>
   </si>
   <si>
-    <t>Login page</t>
-  </si>
-  <si>
     <t>Forgot password?</t>
   </si>
   <si>
@@ -411,9 +408,6 @@
     <t>Surname</t>
   </si>
   <si>
-    <t>Birth of date</t>
-  </si>
-  <si>
     <t>Photo</t>
   </si>
   <si>
@@ -660,9 +654,6 @@
     <t>aboutus_spread_way</t>
   </si>
   <si>
-    <t>Signup page</t>
-  </si>
-  <si>
     <t>School</t>
   </si>
   <si>
@@ -696,9 +687,6 @@
     <t>settlement</t>
   </si>
   <si>
-    <t>education-level</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -712,6 +700,225 @@
   </si>
   <si>
     <t>signup</t>
+  </si>
+  <si>
+    <t>Employer Login page</t>
+  </si>
+  <si>
+    <t>link to Google addin Code</t>
+  </si>
+  <si>
+    <t>Open employee signup page</t>
+  </si>
+  <si>
+    <t>Employee Login page</t>
+  </si>
+  <si>
+    <t>Employee Signup page</t>
+  </si>
+  <si>
+    <t>Employer Signup page</t>
+  </si>
+  <si>
+    <t>Open employer signup page</t>
+  </si>
+  <si>
+    <t>Signup Tab</t>
+  </si>
+  <si>
+    <t>Your Company</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>fill in first name</t>
+  </si>
+  <si>
+    <t>fill in last name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sex </t>
+  </si>
+  <si>
+    <t>Sex (Male, Female)</t>
+  </si>
+  <si>
+    <t>sex selected (Male or Female)</t>
+  </si>
+  <si>
+    <t>Date of birth(Year, Month, Day)</t>
+  </si>
+  <si>
+    <t>date of Birth (Year, Month, Day)</t>
+  </si>
+  <si>
+    <t>Date of birth</t>
+  </si>
+  <si>
+    <t>Date of birth selected (Year, Month and Day)</t>
+  </si>
+  <si>
+    <t>Education level selected (Primary, Secondary, High school, Certificate, Ordinary Diploma, Advanced Diploma, Bachelor Degree, Masters, Doctorial, or Professional)</t>
+  </si>
+  <si>
+    <t>education-_evel</t>
+  </si>
+  <si>
+    <t>fill in course taken</t>
+  </si>
+  <si>
+    <t>fill in phone number</t>
+  </si>
+  <si>
+    <t>fill in address</t>
+  </si>
+  <si>
+    <t>fill in post office box</t>
+  </si>
+  <si>
+    <t>fill in password</t>
+  </si>
+  <si>
+    <t>fill in password again</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graduation year selected </t>
+  </si>
+  <si>
+    <t>surname</t>
+  </si>
+  <si>
+    <t>fill in surname</t>
+  </si>
+  <si>
+    <t>File (pdf format)</t>
+  </si>
+  <si>
+    <t>fill in name of school</t>
+  </si>
+  <si>
+    <t>Award selected (First class, Upper second class, Lower second class, Pass or Fail)</t>
+  </si>
+  <si>
+    <t>fill in skills</t>
+  </si>
+  <si>
+    <t>fill in work experince</t>
+  </si>
+  <si>
+    <t>Uploading a resume</t>
+  </si>
+  <si>
+    <t>fill in job title</t>
+  </si>
+  <si>
+    <t>fill in job location</t>
+  </si>
+  <si>
+    <t>fill in company name or job title</t>
+  </si>
+  <si>
+    <t>Display job search results</t>
+  </si>
+  <si>
+    <t>Display salary search results</t>
+  </si>
+  <si>
+    <t>fill in company name</t>
+  </si>
+  <si>
+    <t>Display company search results</t>
+  </si>
+  <si>
+    <t>fill in pssword</t>
+  </si>
+  <si>
+    <t>Open Job description page</t>
+  </si>
+  <si>
+    <t>Open Application settings page</t>
+  </si>
+  <si>
+    <t>Open Job details page</t>
+  </si>
+  <si>
+    <t>Open Getting started page</t>
+  </si>
+  <si>
+    <t>Application settings page</t>
+  </si>
+  <si>
+    <t>Job description page</t>
+  </si>
+  <si>
+    <t>Company size selected (1-49, 50-149, 150-249, 250-499, 500-749, 750-999, 1000+)</t>
+  </si>
+  <si>
+    <t>fill in person full name</t>
+  </si>
+  <si>
+    <t>Spread way selected (Radio, TV, Newspaper, Social media, Online video, Streaming audio, Search engine, Mail, Words of mouth or Others)</t>
+  </si>
+  <si>
+    <t>fill in Job titl</t>
+  </si>
+  <si>
+    <t>fill in location</t>
+  </si>
+  <si>
+    <t>Back to Account information page</t>
+  </si>
+  <si>
+    <t>Type of job selected (Full time, Part time, Temporary, Contract, Internship, Permanent)</t>
+  </si>
+  <si>
+    <t>fill in job salary</t>
+  </si>
+  <si>
+    <t>salary timre range selected (Per hour, Per day, Per week, Per month, Per year)</t>
+  </si>
+  <si>
+    <t>Back to Getting started page</t>
+  </si>
+  <si>
+    <t>Application media selected (Email or in-person)</t>
+  </si>
+  <si>
+    <t>fill in email</t>
+  </si>
+  <si>
+    <t>Back to Job details page</t>
+  </si>
+  <si>
+    <t>fill in job description</t>
+  </si>
+  <si>
+    <t>fill in required education</t>
+  </si>
+  <si>
+    <t>fill in required skills</t>
+  </si>
+  <si>
+    <t>fill in required experience</t>
+  </si>
+  <si>
+    <t>fill in settlement</t>
+  </si>
+  <si>
+    <t>fill in  nationality</t>
+  </si>
+  <si>
+    <t>fill in nationality</t>
+  </si>
+  <si>
+    <t>fill in position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subpage </t>
   </si>
 </sst>
 </file>
@@ -957,7 +1164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1090,18 +1297,27 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1112,18 +1328,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1136,8 +1340,14 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1477,7 +1687,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1850,7 +2060,7 @@
       <c r="M3" s="31"/>
     </row>
     <row r="4" spans="1:13" s="35" customFormat="1" ht="23.1" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="49" t="s">
         <v>41</v>
       </c>
       <c r="B4" s="33" t="s">
@@ -1891,7 +2101,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" s="35" customFormat="1" ht="24" customHeight="1">
-      <c r="A5" s="47"/>
+      <c r="A5" s="49"/>
       <c r="B5" s="33" t="s">
         <v>47</v>
       </c>
@@ -2094,7 +2304,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" s="35" customFormat="1" ht="21.95" customHeight="1">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="49" t="s">
         <v>54</v>
       </c>
       <c r="B3" s="38" t="s">
@@ -2135,7 +2345,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" s="35" customFormat="1" ht="30" customHeight="1">
-      <c r="A4" s="47"/>
+      <c r="A4" s="49"/>
       <c r="B4" s="33" t="s">
         <v>56</v>
       </c>
@@ -2174,7 +2384,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" s="35" customFormat="1" ht="178.5">
-      <c r="A5" s="47"/>
+      <c r="A5" s="49"/>
       <c r="B5" s="38" t="s">
         <v>57</v>
       </c>
@@ -2295,7 +2505,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" s="35" customFormat="1" ht="23.1" customHeight="1">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="49" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="33" t="s">
@@ -2336,7 +2546,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" s="35" customFormat="1" ht="24" customHeight="1">
-      <c r="A9" s="47"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="33" t="s">
         <v>47</v>
       </c>
@@ -2434,10 +2644,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:N86"/>
+  <dimension ref="A1:N109"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="G86" sqref="G86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2500,8 +2710,8 @@
       </c>
     </row>
     <row r="2" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B2" s="56" t="s">
-        <v>94</v>
+      <c r="B2" s="50" t="s">
+        <v>204</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>85</v>
@@ -2529,15 +2739,15 @@
       </c>
     </row>
     <row r="3" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B3" s="57"/>
+      <c r="B3" s="51"/>
       <c r="C3" s="34" t="s">
         <v>86</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F3" s="28"/>
       <c r="G3" s="33" t="s">
@@ -2557,15 +2767,15 @@
       </c>
     </row>
     <row r="4" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B4" s="57"/>
+      <c r="B4" s="51"/>
       <c r="C4" s="34" t="s">
         <v>87</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="33" t="s">
@@ -2584,12 +2794,12 @@
       </c>
     </row>
     <row r="5" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B5" s="57"/>
+      <c r="B5" s="51"/>
       <c r="C5" s="34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E5" s="33" t="s">
         <v>30</v>
@@ -2605,15 +2815,15 @@
       <c r="L5" s="28"/>
     </row>
     <row r="6" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B6" s="57"/>
+      <c r="B6" s="51"/>
       <c r="C6" s="34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D6" s="27" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F6" s="28"/>
       <c r="G6" s="33" t="s">
@@ -2626,7 +2836,7 @@
       <c r="L6" s="28"/>
     </row>
     <row r="7" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B7" s="57"/>
+      <c r="B7" s="51"/>
       <c r="C7" s="34" t="s">
         <v>88</v>
       </c>
@@ -2634,7 +2844,7 @@
         <v>30</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="33" t="s">
@@ -2647,14 +2857,16 @@
       <c r="L7" s="28"/>
     </row>
     <row r="8" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B8" s="57"/>
+      <c r="B8" s="51"/>
       <c r="C8" s="34" t="s">
         <v>89</v>
       </c>
       <c r="D8" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="33"/>
+      <c r="E8" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="F8" s="28"/>
       <c r="G8" s="33" t="s">
         <v>93</v>
@@ -2666,14 +2878,16 @@
       <c r="L8" s="28"/>
     </row>
     <row r="9" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B9" s="57"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="45" t="s">
         <v>90</v>
       </c>
       <c r="D9" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="33"/>
+      <c r="E9" s="33" t="s">
+        <v>203</v>
+      </c>
       <c r="F9" s="46"/>
       <c r="G9" s="33" t="s">
         <v>44</v>
@@ -2685,19 +2899,21 @@
       <c r="L9" s="46"/>
     </row>
     <row r="10" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B10" s="61" t="s">
-        <v>187</v>
+      <c r="B10" s="60" t="s">
+        <v>205</v>
       </c>
       <c r="C10" s="34" t="s">
         <v>80</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="E10" s="33"/>
+        <v>190</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>212</v>
+      </c>
       <c r="F10" s="46"/>
       <c r="G10" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H10" s="46"/>
       <c r="I10" s="46"/>
@@ -2706,17 +2922,19 @@
       <c r="L10" s="46"/>
     </row>
     <row r="11" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B11" s="62"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="34" t="s">
         <v>78</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="E11" s="33"/>
+        <v>191</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>213</v>
+      </c>
       <c r="F11" s="46"/>
       <c r="G11" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H11" s="46"/>
       <c r="I11" s="46"/>
@@ -2725,14 +2943,16 @@
       <c r="L11" s="46"/>
     </row>
     <row r="12" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B12" s="62"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="34" t="s">
-        <v>98</v>
+        <v>215</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="E12" s="33"/>
+        <v>214</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>216</v>
+      </c>
       <c r="F12" s="46"/>
       <c r="G12" s="33" t="s">
         <v>38</v>
@@ -2744,17 +2964,19 @@
       <c r="L12" s="46"/>
     </row>
     <row r="13" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B13" s="62"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="34" t="s">
-        <v>104</v>
+        <v>217</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>196</v>
-      </c>
-      <c r="E13" s="33"/>
+        <v>193</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>220</v>
+      </c>
       <c r="F13" s="46"/>
       <c r="G13" s="33" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H13" s="46"/>
       <c r="I13" s="46"/>
@@ -2763,17 +2985,19 @@
       <c r="L13" s="46"/>
     </row>
     <row r="14" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B14" s="62"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="E14" s="33"/>
+        <v>194</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>271</v>
+      </c>
       <c r="F14" s="46"/>
       <c r="G14" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H14" s="46"/>
       <c r="I14" s="46"/>
@@ -2782,17 +3006,19 @@
       <c r="L14" s="46"/>
     </row>
     <row r="15" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B15" s="62"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="34" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>198</v>
-      </c>
-      <c r="E15" s="33"/>
+        <v>195</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>269</v>
+      </c>
       <c r="F15" s="46"/>
       <c r="G15" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H15" s="46"/>
       <c r="I15" s="46"/>
@@ -2800,18 +3026,20 @@
       <c r="K15" s="46"/>
       <c r="L15" s="46"/>
     </row>
-    <row r="16" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B16" s="62"/>
+    <row r="16" spans="2:14" s="35" customFormat="1" ht="117.75" customHeight="1">
+      <c r="B16" s="61"/>
       <c r="C16" s="34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>199</v>
-      </c>
-      <c r="E16" s="33"/>
+        <v>222</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>221</v>
+      </c>
       <c r="F16" s="46"/>
       <c r="G16" s="33" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H16" s="46"/>
       <c r="I16" s="46"/>
@@ -2820,17 +3048,19 @@
       <c r="L16" s="46"/>
     </row>
     <row r="17" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B17" s="62"/>
-      <c r="C17" s="64" t="s">
+      <c r="B17" s="61"/>
+      <c r="C17" s="48" t="s">
         <v>83</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="E17" s="33"/>
+        <v>155</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>223</v>
+      </c>
       <c r="F17" s="46"/>
       <c r="G17" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H17" s="46"/>
       <c r="I17" s="46"/>
@@ -2839,17 +3069,19 @@
       <c r="L17" s="46"/>
     </row>
     <row r="18" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B18" s="62"/>
+      <c r="B18" s="61"/>
       <c r="C18" s="34" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>158</v>
-      </c>
-      <c r="E18" s="33"/>
+        <v>156</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>233</v>
+      </c>
       <c r="F18" s="46"/>
       <c r="G18" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H18" s="46"/>
       <c r="I18" s="46"/>
@@ -2858,17 +3090,19 @@
       <c r="L18" s="46"/>
     </row>
     <row r="19" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B19" s="62"/>
+      <c r="B19" s="61"/>
       <c r="C19" s="34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="E19" s="33"/>
+        <v>157</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>229</v>
+      </c>
       <c r="F19" s="46"/>
       <c r="G19" s="33" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H19" s="46"/>
       <c r="I19" s="46"/>
@@ -2877,17 +3111,19 @@
       <c r="L19" s="46"/>
     </row>
     <row r="20" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B20" s="62"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="E20" s="33"/>
+        <v>173</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>224</v>
+      </c>
       <c r="F20" s="46"/>
       <c r="G20" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H20" s="46"/>
       <c r="I20" s="46"/>
@@ -2896,17 +3132,19 @@
       <c r="L20" s="46"/>
     </row>
     <row r="21" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B21" s="62"/>
+      <c r="B21" s="61"/>
       <c r="C21" s="34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>200</v>
-      </c>
-      <c r="E21" s="33"/>
+        <v>196</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>263</v>
+      </c>
       <c r="F21" s="46"/>
       <c r="G21" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H21" s="46"/>
       <c r="I21" s="46"/>
@@ -2915,17 +3153,19 @@
       <c r="L21" s="46"/>
     </row>
     <row r="22" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B22" s="62"/>
+      <c r="B22" s="61"/>
       <c r="C22" s="19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>201</v>
-      </c>
-      <c r="E22" s="33"/>
+        <v>197</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>225</v>
+      </c>
       <c r="F22" s="46"/>
       <c r="G22" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H22" s="46"/>
       <c r="I22" s="46"/>
@@ -2934,17 +3174,19 @@
       <c r="L22" s="46"/>
     </row>
     <row r="23" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B23" s="62"/>
+      <c r="B23" s="61"/>
       <c r="C23" s="19" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>202</v>
-      </c>
-      <c r="E23" s="33"/>
+        <v>198</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>226</v>
+      </c>
       <c r="F23" s="46"/>
       <c r="G23" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H23" s="46"/>
       <c r="I23" s="46"/>
@@ -2953,17 +3195,19 @@
       <c r="L23" s="46"/>
     </row>
     <row r="24" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B24" s="62"/>
+      <c r="B24" s="61"/>
       <c r="C24" s="35" t="s">
         <v>86</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>154</v>
-      </c>
-      <c r="E24" s="33"/>
+        <v>152</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>150</v>
+      </c>
       <c r="F24" s="46"/>
       <c r="G24" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H24" s="46"/>
       <c r="I24" s="46"/>
@@ -2972,17 +3216,19 @@
       <c r="L24" s="46"/>
     </row>
     <row r="25" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B25" s="62"/>
+      <c r="B25" s="61"/>
       <c r="C25" s="34" t="s">
         <v>87</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>155</v>
-      </c>
-      <c r="E25" s="33"/>
+        <v>153</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>227</v>
+      </c>
       <c r="F25" s="46"/>
       <c r="G25" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H25" s="46"/>
       <c r="I25" s="46"/>
@@ -2991,17 +3237,19 @@
       <c r="L25" s="46"/>
     </row>
     <row r="26" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B26" s="62"/>
-      <c r="C26" s="64" t="s">
-        <v>189</v>
+      <c r="B26" s="61"/>
+      <c r="C26" s="48" t="s">
+        <v>186</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>203</v>
-      </c>
-      <c r="E26" s="33"/>
+        <v>199</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>228</v>
+      </c>
       <c r="F26" s="46"/>
       <c r="G26" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H26" s="46"/>
       <c r="I26" s="46"/>
@@ -3010,14 +3258,16 @@
       <c r="L26" s="46"/>
     </row>
     <row r="27" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B27" s="63"/>
-      <c r="C27" s="64" t="s">
+      <c r="B27" s="62"/>
+      <c r="C27" s="48" t="s">
         <v>90</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>204</v>
-      </c>
-      <c r="E27" s="33"/>
+        <v>200</v>
+      </c>
+      <c r="E27" s="33" t="s">
+        <v>203</v>
+      </c>
       <c r="F27" s="28"/>
       <c r="G27" s="33" t="s">
         <v>93</v>
@@ -3035,16 +3285,18 @@
       </c>
     </row>
     <row r="28" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B28" s="56" t="s">
-        <v>106</v>
+      <c r="B28" s="50" t="s">
+        <v>104</v>
       </c>
       <c r="C28" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="D28" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="33"/>
+        <v>95</v>
+      </c>
+      <c r="D28" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="47" t="s">
+        <v>30</v>
+      </c>
       <c r="F28" s="28"/>
       <c r="G28" s="33" t="s">
         <v>93</v>
@@ -3056,17 +3308,19 @@
       <c r="L28" s="28"/>
     </row>
     <row r="29" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B29" s="57"/>
+      <c r="B29" s="51"/>
       <c r="C29" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="D29" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" s="33"/>
+        <v>96</v>
+      </c>
+      <c r="D29" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="47" t="s">
+        <v>30</v>
+      </c>
       <c r="F29" s="28"/>
       <c r="G29" s="33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H29" s="28"/>
       <c r="I29" s="28"/>
@@ -3075,14 +3329,16 @@
       <c r="L29" s="28"/>
     </row>
     <row r="30" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B30" s="57"/>
+      <c r="B30" s="51"/>
       <c r="C30" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="28"/>
+      <c r="D30" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="47" t="s">
+        <v>30</v>
+      </c>
       <c r="F30" s="28"/>
       <c r="G30" s="28" t="s">
         <v>30</v>
@@ -3096,14 +3352,16 @@
       <c r="N30" s="18"/>
     </row>
     <row r="31" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B31" s="57"/>
+      <c r="B31" s="51"/>
       <c r="C31" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" s="28"/>
+      <c r="D31" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="47" t="s">
+        <v>30</v>
+      </c>
       <c r="F31" s="28"/>
       <c r="G31" s="28" t="s">
         <v>30</v>
@@ -3117,14 +3375,16 @@
       <c r="N31" s="18"/>
     </row>
     <row r="32" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B32" s="57"/>
+      <c r="B32" s="51"/>
       <c r="C32" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" s="28"/>
+        <v>97</v>
+      </c>
+      <c r="D32" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="47" t="s">
+        <v>30</v>
+      </c>
       <c r="F32" s="28"/>
       <c r="G32" s="28" t="s">
         <v>30</v>
@@ -3138,14 +3398,16 @@
       <c r="N32" s="18"/>
     </row>
     <row r="33" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B33" s="57"/>
+      <c r="B33" s="51"/>
       <c r="C33" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" s="28"/>
+      <c r="D33" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="47" t="s">
+        <v>30</v>
+      </c>
       <c r="F33" s="28"/>
       <c r="G33" s="28" t="s">
         <v>30</v>
@@ -3159,14 +3421,16 @@
       <c r="N33" s="18"/>
     </row>
     <row r="34" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B34" s="57"/>
+      <c r="B34" s="51"/>
       <c r="C34" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E34" s="28"/>
+        <v>98</v>
+      </c>
+      <c r="D34" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" s="47" t="s">
+        <v>30</v>
+      </c>
       <c r="F34" s="28"/>
       <c r="G34" s="28" t="s">
         <v>30</v>
@@ -3180,14 +3444,16 @@
       <c r="N34" s="18"/>
     </row>
     <row r="35" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B35" s="57"/>
+      <c r="B35" s="51"/>
       <c r="C35" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="D35" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E35" s="28"/>
+        <v>100</v>
+      </c>
+      <c r="D35" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" s="47" t="s">
+        <v>30</v>
+      </c>
       <c r="F35" s="28"/>
       <c r="G35" s="28" t="s">
         <v>30</v>
@@ -3201,14 +3467,16 @@
       <c r="N35" s="18"/>
     </row>
     <row r="36" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B36" s="58"/>
+      <c r="B36" s="52"/>
       <c r="C36" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="D36" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E36" s="28"/>
+        <v>99</v>
+      </c>
+      <c r="D36" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" s="47" t="s">
+        <v>30</v>
+      </c>
       <c r="F36" s="28"/>
       <c r="G36" s="28" t="s">
         <v>30</v>
@@ -3222,16 +3490,22 @@
       <c r="N36" s="18"/>
     </row>
     <row r="37" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B37" s="51" t="s">
-        <v>107</v>
+      <c r="B37" s="53" t="s">
+        <v>105</v>
       </c>
       <c r="C37" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="D37" s="27"/>
-      <c r="E37" s="28"/>
+      <c r="D37" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="E37" s="33" t="s">
+        <v>212</v>
+      </c>
       <c r="F37" s="28"/>
-      <c r="G37" s="46"/>
+      <c r="G37" s="33" t="s">
+        <v>118</v>
+      </c>
       <c r="H37" s="28"/>
       <c r="I37" s="28"/>
       <c r="J37" s="28"/>
@@ -3241,14 +3515,20 @@
       <c r="N37" s="18"/>
     </row>
     <row r="38" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B38" s="59"/>
+      <c r="B38" s="54"/>
       <c r="C38" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="D38" s="27"/>
-      <c r="E38" s="28"/>
+        <v>102</v>
+      </c>
+      <c r="D38" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="E38" s="33" t="s">
+        <v>231</v>
+      </c>
       <c r="F38" s="28"/>
-      <c r="G38" s="46"/>
+      <c r="G38" s="33" t="s">
+        <v>118</v>
+      </c>
       <c r="H38" s="28"/>
       <c r="I38" s="28"/>
       <c r="J38" s="28"/>
@@ -3258,14 +3538,20 @@
       <c r="N38" s="18"/>
     </row>
     <row r="39" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B39" s="59"/>
+      <c r="B39" s="54"/>
       <c r="C39" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="D39" s="27"/>
-      <c r="E39" s="28"/>
+        <v>97</v>
+      </c>
+      <c r="D39" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="E39" s="33" t="s">
+        <v>216</v>
+      </c>
       <c r="F39" s="28"/>
-      <c r="G39" s="46"/>
+      <c r="G39" s="33" t="s">
+        <v>38</v>
+      </c>
       <c r="H39" s="28"/>
       <c r="I39" s="28"/>
       <c r="J39" s="28"/>
@@ -3275,14 +3561,20 @@
       <c r="N39" s="18"/>
     </row>
     <row r="40" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B40" s="59"/>
+      <c r="B40" s="54"/>
       <c r="C40" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="D40" s="27"/>
-      <c r="E40" s="28"/>
+      <c r="D40" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="E40" s="33" t="s">
+        <v>225</v>
+      </c>
       <c r="F40" s="28"/>
-      <c r="G40" s="46"/>
+      <c r="G40" s="33" t="s">
+        <v>118</v>
+      </c>
       <c r="H40" s="28"/>
       <c r="I40" s="28"/>
       <c r="J40" s="28"/>
@@ -3292,14 +3584,20 @@
       <c r="N40" s="18"/>
     </row>
     <row r="41" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B41" s="59"/>
+      <c r="B41" s="54"/>
       <c r="C41" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="D41" s="27"/>
-      <c r="E41" s="28"/>
+        <v>219</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="E41" s="33" t="s">
+        <v>220</v>
+      </c>
       <c r="F41" s="28"/>
-      <c r="G41" s="46"/>
+      <c r="G41" s="33" t="s">
+        <v>130</v>
+      </c>
       <c r="H41" s="28"/>
       <c r="I41" s="28"/>
       <c r="J41" s="28"/>
@@ -3309,14 +3607,20 @@
       <c r="N41" s="18"/>
     </row>
     <row r="42" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B42" s="52"/>
+      <c r="B42" s="55"/>
       <c r="C42" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="D42" s="27"/>
-      <c r="E42" s="28"/>
+        <v>103</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" s="33" t="s">
+        <v>30</v>
+      </c>
       <c r="F42" s="28"/>
-      <c r="G42" s="46"/>
+      <c r="G42" s="33" t="s">
+        <v>30</v>
+      </c>
       <c r="H42" s="28"/>
       <c r="I42" s="28"/>
       <c r="J42" s="28"/>
@@ -3326,18 +3630,22 @@
       <c r="N42" s="18"/>
     </row>
     <row r="43" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B43" s="53" t="s">
-        <v>113</v>
+      <c r="B43" s="56" t="s">
+        <v>111</v>
       </c>
       <c r="C43" s="34" t="s">
         <v>83</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="E43" s="28"/>
+        <v>155</v>
+      </c>
+      <c r="E43" s="33" t="s">
+        <v>223</v>
+      </c>
       <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
+      <c r="G43" s="33" t="s">
+        <v>118</v>
+      </c>
       <c r="H43" s="28"/>
       <c r="I43" s="28"/>
       <c r="J43" s="28"/>
@@ -3347,16 +3655,20 @@
       <c r="N43" s="18"/>
     </row>
     <row r="44" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B44" s="54"/>
+      <c r="B44" s="57"/>
       <c r="C44" s="34" t="s">
         <v>82</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>158</v>
-      </c>
-      <c r="E44" s="28"/>
+        <v>156</v>
+      </c>
+      <c r="E44" s="33" t="s">
+        <v>233</v>
+      </c>
       <c r="F44" s="28"/>
-      <c r="G44" s="28"/>
+      <c r="G44" s="33" t="s">
+        <v>118</v>
+      </c>
       <c r="H44" s="28"/>
       <c r="I44" s="28"/>
       <c r="J44" s="28"/>
@@ -3366,16 +3678,20 @@
       <c r="N44" s="18"/>
     </row>
     <row r="45" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B45" s="54"/>
+      <c r="B45" s="57"/>
       <c r="C45" s="34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="E45" s="28"/>
+        <v>157</v>
+      </c>
+      <c r="E45" s="47" t="s">
+        <v>229</v>
+      </c>
       <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
+      <c r="G45" s="33" t="s">
+        <v>130</v>
+      </c>
       <c r="H45" s="28"/>
       <c r="I45" s="28"/>
       <c r="J45" s="28"/>
@@ -3384,17 +3700,21 @@
       <c r="M45" s="19"/>
       <c r="N45" s="18"/>
     </row>
-    <row r="46" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B46" s="54"/>
+    <row r="46" spans="2:14" s="35" customFormat="1" ht="50.25" customHeight="1">
+      <c r="B46" s="57"/>
       <c r="C46" s="34" t="s">
         <v>84</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="E46" s="28"/>
+        <v>158</v>
+      </c>
+      <c r="E46" s="33" t="s">
+        <v>234</v>
+      </c>
       <c r="F46" s="28"/>
-      <c r="G46" s="28"/>
+      <c r="G46" s="33" t="s">
+        <v>130</v>
+      </c>
       <c r="H46" s="28"/>
       <c r="I46" s="28"/>
       <c r="J46" s="28"/>
@@ -3403,17 +3723,21 @@
       <c r="M46" s="19"/>
       <c r="N46" s="18"/>
     </row>
-    <row r="47" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B47" s="54"/>
+    <row r="47" spans="2:14" s="35" customFormat="1" ht="101.25" customHeight="1">
+      <c r="B47" s="57"/>
       <c r="C47" s="34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="E47" s="28"/>
+        <v>159</v>
+      </c>
+      <c r="E47" s="33" t="s">
+        <v>221</v>
+      </c>
       <c r="F47" s="28"/>
-      <c r="G47" s="28"/>
+      <c r="G47" s="33" t="s">
+        <v>130</v>
+      </c>
       <c r="H47" s="28"/>
       <c r="I47" s="28"/>
       <c r="J47" s="28"/>
@@ -3423,16 +3747,20 @@
       <c r="N47" s="18"/>
     </row>
     <row r="48" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B48" s="54"/>
+      <c r="B48" s="57"/>
       <c r="C48" s="34" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D48" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="E48" s="28"/>
+        <v>160</v>
+      </c>
+      <c r="E48" s="33" t="s">
+        <v>235</v>
+      </c>
       <c r="F48" s="28"/>
-      <c r="G48" s="28"/>
+      <c r="G48" s="33" t="s">
+        <v>147</v>
+      </c>
       <c r="H48" s="28"/>
       <c r="I48" s="28"/>
       <c r="J48" s="28"/>
@@ -3441,17 +3769,21 @@
       <c r="M48" s="19"/>
       <c r="N48" s="18"/>
     </row>
-    <row r="49" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B49" s="54"/>
+    <row r="49" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B49" s="57"/>
       <c r="C49" s="34" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="E49" s="28"/>
+        <v>161</v>
+      </c>
+      <c r="E49" s="33" t="s">
+        <v>236</v>
+      </c>
       <c r="F49" s="28"/>
-      <c r="G49" s="28"/>
+      <c r="G49" s="33" t="s">
+        <v>147</v>
+      </c>
       <c r="H49" s="28"/>
       <c r="I49" s="28"/>
       <c r="J49" s="28"/>
@@ -3460,17 +3792,21 @@
       <c r="M49" s="19"/>
       <c r="N49" s="18"/>
     </row>
-    <row r="50" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B50" s="55"/>
+    <row r="50" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B50" s="58"/>
       <c r="C50" s="34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>164</v>
-      </c>
-      <c r="E50" s="28"/>
+        <v>162</v>
+      </c>
+      <c r="E50" s="33" t="s">
+        <v>237</v>
+      </c>
       <c r="F50" s="28"/>
-      <c r="G50" s="33"/>
+      <c r="G50" s="33" t="s">
+        <v>232</v>
+      </c>
       <c r="H50" s="28"/>
       <c r="I50" s="28"/>
       <c r="J50" s="28"/>
@@ -3479,20 +3815,22 @@
       <c r="M50" s="19"/>
       <c r="N50" s="18"/>
     </row>
-    <row r="51" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B51" s="51" t="s">
-        <v>118</v>
+    <row r="51" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B51" s="53" t="s">
+        <v>116</v>
       </c>
       <c r="C51" s="34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="E51" s="28"/>
+        <v>163</v>
+      </c>
+      <c r="E51" s="33" t="s">
+        <v>238</v>
+      </c>
       <c r="F51" s="28"/>
       <c r="G51" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H51" s="28"/>
       <c r="I51" s="28"/>
@@ -3502,18 +3840,20 @@
       <c r="M51" s="19"/>
       <c r="N51" s="18"/>
     </row>
-    <row r="52" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B52" s="60"/>
+    <row r="52" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B52" s="59"/>
       <c r="C52" s="34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="E52" s="28"/>
+        <v>164</v>
+      </c>
+      <c r="E52" s="33" t="s">
+        <v>239</v>
+      </c>
       <c r="F52" s="28"/>
       <c r="G52" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H52" s="28"/>
       <c r="I52" s="28"/>
@@ -3523,15 +3863,17 @@
       <c r="M52" s="19"/>
       <c r="N52" s="18"/>
     </row>
-    <row r="53" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B53" s="60"/>
+    <row r="53" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B53" s="59"/>
       <c r="C53" s="34" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>167</v>
-      </c>
-      <c r="E53" s="28"/>
+        <v>165</v>
+      </c>
+      <c r="E53" s="33" t="s">
+        <v>241</v>
+      </c>
       <c r="F53" s="28"/>
       <c r="G53" s="33" t="s">
         <v>44</v>
@@ -3544,20 +3886,22 @@
       <c r="M53" s="19"/>
       <c r="N53" s="18"/>
     </row>
-    <row r="54" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B54" s="51" t="s">
+    <row r="54" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B54" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="C54" s="44" t="s">
-        <v>119</v>
-      </c>
       <c r="D54" s="27" t="s">
-        <v>168</v>
-      </c>
-      <c r="E54" s="28"/>
+        <v>166</v>
+      </c>
+      <c r="E54" s="33" t="s">
+        <v>240</v>
+      </c>
       <c r="F54" s="28"/>
       <c r="G54" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H54" s="28"/>
       <c r="I54" s="28"/>
@@ -3567,15 +3911,17 @@
       <c r="M54" s="19"/>
       <c r="N54" s="18"/>
     </row>
-    <row r="55" spans="2:14" s="35" customFormat="1" ht="26.1" customHeight="1">
-      <c r="B55" s="52"/>
+    <row r="55" spans="1:14" s="35" customFormat="1" ht="26.1" customHeight="1">
+      <c r="B55" s="55"/>
       <c r="C55" s="44" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="E55" s="28"/>
+        <v>167</v>
+      </c>
+      <c r="E55" s="33" t="s">
+        <v>242</v>
+      </c>
       <c r="F55" s="28"/>
       <c r="G55" s="33" t="s">
         <v>44</v>
@@ -3588,20 +3934,22 @@
       <c r="M55" s="19"/>
       <c r="N55" s="18"/>
     </row>
-    <row r="56" spans="2:14">
-      <c r="B56" s="53" t="s">
-        <v>121</v>
+    <row r="56" spans="1:14">
+      <c r="B56" s="56" t="s">
+        <v>119</v>
       </c>
       <c r="C56" s="34" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="E56" s="43"/>
+        <v>168</v>
+      </c>
+      <c r="E56" s="33" t="s">
+        <v>243</v>
+      </c>
       <c r="F56" s="43"/>
       <c r="G56" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H56" s="43"/>
       <c r="I56" s="43"/>
@@ -3609,15 +3957,17 @@
       <c r="K56" s="34"/>
       <c r="L56" s="34"/>
     </row>
-    <row r="57" spans="2:14">
-      <c r="B57" s="54"/>
+    <row r="57" spans="1:14" ht="25.5">
+      <c r="B57" s="57"/>
       <c r="C57" s="34" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D57" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="E57" s="43"/>
+        <v>169</v>
+      </c>
+      <c r="E57" s="33" t="s">
+        <v>244</v>
+      </c>
       <c r="F57" s="43"/>
       <c r="G57" s="33" t="s">
         <v>44</v>
@@ -3628,438 +3978,512 @@
       <c r="K57" s="34"/>
       <c r="L57" s="34"/>
     </row>
-    <row r="58" spans="2:14">
-      <c r="B58" s="53" t="s">
-        <v>123</v>
-      </c>
-      <c r="C58" s="45" t="s">
-        <v>124</v>
+    <row r="58" spans="1:14" ht="15" customHeight="1">
+      <c r="A58" s="35"/>
+      <c r="B58" s="50" t="s">
+        <v>201</v>
+      </c>
+      <c r="C58" s="34" t="s">
+        <v>85</v>
       </c>
       <c r="D58" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E58" s="43"/>
-      <c r="F58" s="43"/>
-      <c r="G58" s="33"/>
-      <c r="H58" s="43"/>
-      <c r="I58" s="43"/>
-      <c r="J58" s="43"/>
-      <c r="K58" s="34"/>
-      <c r="L58" s="34"/>
-    </row>
-    <row r="59" spans="2:14">
-      <c r="B59" s="54"/>
-      <c r="C59" s="45" t="s">
-        <v>125</v>
+      <c r="E58" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F58" s="47"/>
+      <c r="G58" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="H58" s="47"/>
+      <c r="I58" s="47"/>
+      <c r="J58" s="47"/>
+      <c r="K58" s="47"/>
+      <c r="L58" s="47"/>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59" s="35"/>
+      <c r="B59" s="51"/>
+      <c r="C59" s="34" t="s">
+        <v>86</v>
       </c>
       <c r="D59" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E59" s="43"/>
-      <c r="F59" s="43"/>
-      <c r="G59" s="33"/>
-      <c r="H59" s="43"/>
-      <c r="I59" s="43"/>
-      <c r="J59" s="43"/>
-      <c r="K59" s="34"/>
-      <c r="L59" s="34"/>
-    </row>
-    <row r="60" spans="2:14">
-      <c r="B60" s="54"/>
-      <c r="C60" s="45" t="s">
-        <v>126</v>
+        <v>152</v>
+      </c>
+      <c r="E59" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="F59" s="47"/>
+      <c r="G59" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="H59" s="47"/>
+      <c r="I59" s="47"/>
+      <c r="J59" s="47"/>
+      <c r="K59" s="47"/>
+      <c r="L59" s="47"/>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60" s="35"/>
+      <c r="B60" s="51"/>
+      <c r="C60" s="34" t="s">
+        <v>87</v>
       </c>
       <c r="D60" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E60" s="43"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="33"/>
-      <c r="H60" s="43"/>
-      <c r="I60" s="43"/>
-      <c r="J60" s="43"/>
-      <c r="K60" s="34"/>
-      <c r="L60" s="34"/>
-    </row>
-    <row r="61" spans="2:14">
-      <c r="B61" s="54"/>
-      <c r="C61" s="45" t="s">
-        <v>127</v>
+        <v>153</v>
+      </c>
+      <c r="E60" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="F60" s="47"/>
+      <c r="G60" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="H60" s="47"/>
+      <c r="I60" s="47"/>
+      <c r="J60" s="47"/>
+      <c r="K60" s="47"/>
+      <c r="L60" s="47"/>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61" s="35"/>
+      <c r="B61" s="51"/>
+      <c r="C61" s="34" t="s">
+        <v>148</v>
       </c>
       <c r="D61" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E61" s="43"/>
-      <c r="F61" s="43"/>
-      <c r="G61" s="33"/>
-      <c r="H61" s="43"/>
-      <c r="I61" s="43"/>
-      <c r="J61" s="43"/>
-      <c r="K61" s="34"/>
-      <c r="L61" s="34"/>
-    </row>
-    <row r="62" spans="2:14">
-      <c r="B62" s="55"/>
-      <c r="C62" s="45" t="s">
-        <v>128</v>
+        <v>154</v>
+      </c>
+      <c r="E61" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F61" s="47"/>
+      <c r="G61" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H61" s="47"/>
+      <c r="I61" s="47"/>
+      <c r="J61" s="47"/>
+      <c r="K61" s="47"/>
+      <c r="L61" s="47"/>
+    </row>
+    <row r="62" spans="1:14" ht="25.5">
+      <c r="A62" s="35"/>
+      <c r="B62" s="51"/>
+      <c r="C62" s="34" t="s">
+        <v>94</v>
       </c>
       <c r="D62" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E62" s="43"/>
-      <c r="F62" s="43"/>
-      <c r="G62" s="33"/>
-      <c r="H62" s="43"/>
-      <c r="I62" s="43"/>
-      <c r="J62" s="43"/>
-      <c r="K62" s="34"/>
-      <c r="L62" s="34"/>
-    </row>
-    <row r="63" spans="2:14">
-      <c r="B63" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="C63" s="34" t="s">
+      <c r="E62" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="F62" s="47"/>
+      <c r="G62" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="H62" s="47"/>
+      <c r="I62" s="47"/>
+      <c r="J62" s="47"/>
+      <c r="K62" s="47"/>
+      <c r="L62" s="47"/>
+    </row>
+    <row r="63" spans="1:14" ht="25.5">
+      <c r="A63" s="35"/>
+      <c r="B63" s="51"/>
+      <c r="C63" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="D63" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E63" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="F63" s="47"/>
+      <c r="G63" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H63" s="47"/>
+      <c r="I63" s="47"/>
+      <c r="J63" s="47"/>
+      <c r="K63" s="47"/>
+      <c r="L63" s="47"/>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="A64" s="35"/>
+      <c r="B64" s="60" t="s">
+        <v>206</v>
+      </c>
+      <c r="C64" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="D64" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="E64" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="F64" s="47"/>
+      <c r="G64" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H64" s="47"/>
+      <c r="I64" s="47"/>
+      <c r="J64" s="47"/>
+      <c r="K64" s="47"/>
+      <c r="L64" s="47"/>
+    </row>
+    <row r="65" spans="1:14">
+      <c r="A65" s="35"/>
+      <c r="B65" s="61"/>
+      <c r="C65" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D65" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="E65" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="F65" s="47"/>
+      <c r="G65" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H65" s="47"/>
+      <c r="I65" s="47"/>
+      <c r="J65" s="47"/>
+      <c r="K65" s="47"/>
+      <c r="L65" s="47"/>
+      <c r="M65"/>
+      <c r="N65"/>
+    </row>
+    <row r="66" spans="1:14" ht="25.5" customHeight="1">
+      <c r="A66" s="35"/>
+      <c r="B66" s="61"/>
+      <c r="C66" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="D66" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="E66" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="F66" s="47"/>
+      <c r="G66" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H66" s="47"/>
+      <c r="I66" s="47"/>
+      <c r="J66" s="47"/>
+      <c r="K66" s="47"/>
+      <c r="L66" s="47"/>
+    </row>
+    <row r="67" spans="1:14" ht="25.5">
+      <c r="A67" s="35"/>
+      <c r="B67" s="61"/>
+      <c r="C67" s="34" t="s">
+        <v>218</v>
+      </c>
+      <c r="D67" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="E67" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="F67" s="47"/>
+      <c r="G67" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="H67" s="47"/>
+      <c r="I67" s="47"/>
+      <c r="J67" s="47"/>
+      <c r="K67" s="47"/>
+      <c r="L67" s="47"/>
+    </row>
+    <row r="68" spans="1:14">
+      <c r="A68" s="35"/>
+      <c r="B68" s="61"/>
+      <c r="C68" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="D68" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="E68" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="F68" s="47"/>
+      <c r="G68" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H68" s="47"/>
+      <c r="I68" s="47"/>
+      <c r="J68" s="47"/>
+      <c r="K68" s="47"/>
+      <c r="L68" s="47"/>
+    </row>
+    <row r="69" spans="1:14">
+      <c r="A69" s="35"/>
+      <c r="B69" s="61"/>
+      <c r="C69" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="D69" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="E69" s="33" t="s">
+        <v>269</v>
+      </c>
+      <c r="F69" s="47"/>
+      <c r="G69" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H69" s="47"/>
+      <c r="I69" s="47"/>
+      <c r="J69" s="47"/>
+      <c r="K69" s="47"/>
+      <c r="L69" s="47"/>
+    </row>
+    <row r="70" spans="1:14">
+      <c r="A70" s="35"/>
+      <c r="B70" s="61"/>
+      <c r="C70" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="D70" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="E70" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="F70" s="47"/>
+      <c r="G70" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H70" s="47"/>
+      <c r="I70" s="47"/>
+      <c r="J70" s="47"/>
+      <c r="K70" s="47"/>
+      <c r="L70" s="47"/>
+    </row>
+    <row r="71" spans="1:14">
+      <c r="A71" s="35"/>
+      <c r="B71" s="61"/>
+      <c r="C71" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="D71" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="E71" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="F71" s="47"/>
+      <c r="G71" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H71" s="47"/>
+      <c r="I71" s="47"/>
+      <c r="J71" s="47"/>
+      <c r="K71" s="47"/>
+      <c r="L71" s="47"/>
+    </row>
+    <row r="72" spans="1:14">
+      <c r="A72" s="35"/>
+      <c r="B72" s="61"/>
+      <c r="C72" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D72" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="E72" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="F72" s="47"/>
+      <c r="G72" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H72" s="47"/>
+      <c r="I72" s="47"/>
+      <c r="J72" s="47"/>
+      <c r="K72" s="47"/>
+      <c r="L72" s="47"/>
+    </row>
+    <row r="73" spans="1:14">
+      <c r="A73" s="35"/>
+      <c r="B73" s="61"/>
+      <c r="C73" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="D73" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="E73" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="F73" s="47"/>
+      <c r="G73" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H73" s="47"/>
+      <c r="I73" s="47"/>
+      <c r="J73" s="47"/>
+      <c r="K73" s="47"/>
+      <c r="L73" s="47"/>
+    </row>
+    <row r="74" spans="1:14">
+      <c r="A74" s="35"/>
+      <c r="B74" s="61"/>
+      <c r="C74" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="D74" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="E74" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="F74" s="47"/>
+      <c r="G74" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H74" s="47"/>
+      <c r="I74" s="47"/>
+      <c r="J74" s="47"/>
+      <c r="K74" s="47"/>
+      <c r="L74" s="47"/>
+    </row>
+    <row r="75" spans="1:14">
+      <c r="A75" s="35"/>
+      <c r="B75" s="61"/>
+      <c r="C75" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="D75" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="E75" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="F75" s="47"/>
+      <c r="G75" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H75" s="47"/>
+      <c r="I75" s="47"/>
+      <c r="J75" s="47"/>
+      <c r="K75" s="47"/>
+      <c r="L75" s="47"/>
+    </row>
+    <row r="76" spans="1:14">
+      <c r="A76" s="35"/>
+      <c r="B76" s="61"/>
+      <c r="C76" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D76" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="E76" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="F76" s="47"/>
+      <c r="G76" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H76" s="47"/>
+      <c r="I76" s="47"/>
+      <c r="J76" s="47"/>
+      <c r="K76" s="47"/>
+      <c r="L76" s="47"/>
+    </row>
+    <row r="77" spans="1:14">
+      <c r="A77" s="35"/>
+      <c r="B77" s="61"/>
+      <c r="C77" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D77" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="E77" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="F77" s="47"/>
+      <c r="G77" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H77" s="47"/>
+      <c r="I77" s="47"/>
+      <c r="J77" s="47"/>
+      <c r="K77" s="47"/>
+      <c r="L77" s="47"/>
+    </row>
+    <row r="78" spans="1:14">
+      <c r="A78" s="35"/>
+      <c r="B78" s="61"/>
+      <c r="C78" s="48" t="s">
+        <v>186</v>
+      </c>
+      <c r="D78" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="E78" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="F78" s="47"/>
+      <c r="G78" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H78" s="47"/>
+      <c r="I78" s="47"/>
+      <c r="J78" s="47"/>
+      <c r="K78" s="47"/>
+      <c r="L78" s="47"/>
+    </row>
+    <row r="79" spans="1:14" ht="25.5">
+      <c r="A79" s="35"/>
+      <c r="B79" s="62"/>
+      <c r="C79" s="48" t="s">
+        <v>208</v>
+      </c>
+      <c r="D79" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="E79" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="F79" s="47"/>
+      <c r="G79" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H79" s="47"/>
+      <c r="I79" s="47"/>
+      <c r="J79" s="47"/>
+      <c r="K79" s="47"/>
+      <c r="L79" s="47"/>
+    </row>
+    <row r="80" spans="1:14">
+      <c r="B80" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="C80" s="45" t="s">
         <v>122</v>
       </c>
-      <c r="D63" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="E63" s="43"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="H63" s="43"/>
-      <c r="I63" s="43"/>
-      <c r="J63" s="43"/>
-      <c r="K63" s="34"/>
-      <c r="L63" s="34"/>
-    </row>
-    <row r="64" spans="2:14">
-      <c r="B64" s="49"/>
-      <c r="C64" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="D64" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="E64" s="43"/>
-      <c r="F64" s="43"/>
-      <c r="G64" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="H64" s="43"/>
-      <c r="I64" s="43"/>
-      <c r="J64" s="43"/>
-      <c r="K64" s="34"/>
-      <c r="L64" s="34"/>
-    </row>
-    <row r="65" spans="2:14">
-      <c r="B65" s="49"/>
-      <c r="C65" s="34" t="s">
-        <v>173</v>
-      </c>
-      <c r="D65" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="E65" s="43"/>
-      <c r="F65" s="43"/>
-      <c r="G65" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="H65" s="43"/>
-      <c r="I65" s="43"/>
-      <c r="J65" s="43"/>
-      <c r="K65" s="34"/>
-      <c r="L65" s="34"/>
-    </row>
-    <row r="66" spans="2:14">
-      <c r="B66" s="49"/>
-      <c r="C66" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="D66" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="H66" s="43"/>
-      <c r="I66" s="43"/>
-      <c r="J66" s="43"/>
-      <c r="K66" s="34"/>
-      <c r="L66" s="34"/>
-    </row>
-    <row r="67" spans="2:14" ht="25.5">
-      <c r="B67" s="49"/>
-      <c r="C67" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="D67" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="E67" s="43"/>
-      <c r="F67" s="43"/>
-      <c r="G67" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="H67" s="43"/>
-      <c r="I67" s="43"/>
-      <c r="J67" s="43"/>
-      <c r="K67" s="34"/>
-      <c r="L67" s="34"/>
-      <c r="M67"/>
-      <c r="N67"/>
-    </row>
-    <row r="68" spans="2:14" ht="25.5" customHeight="1">
-      <c r="B68" s="48" t="s">
-        <v>133</v>
-      </c>
-      <c r="C68" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="D68" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="E68" s="43"/>
-      <c r="F68" s="43"/>
-      <c r="G68" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="H68" s="43"/>
-      <c r="I68" s="43"/>
-      <c r="J68" s="43"/>
-      <c r="K68" s="34"/>
-      <c r="L68" s="34"/>
-    </row>
-    <row r="69" spans="2:14">
-      <c r="B69" s="49"/>
-      <c r="C69" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="D69" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="E69" s="43"/>
-      <c r="F69" s="43"/>
-      <c r="G69" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="H69" s="43"/>
-      <c r="I69" s="43"/>
-      <c r="J69" s="43"/>
-      <c r="K69" s="34"/>
-      <c r="L69" s="34"/>
-    </row>
-    <row r="70" spans="2:14">
-      <c r="B70" s="49"/>
-      <c r="C70" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="D70" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="E70" s="43"/>
-      <c r="F70" s="43"/>
-      <c r="G70" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="H70" s="43"/>
-      <c r="I70" s="43"/>
-      <c r="J70" s="43"/>
-      <c r="K70" s="34"/>
-      <c r="L70" s="34"/>
-    </row>
-    <row r="71" spans="2:14">
-      <c r="B71" s="49"/>
-      <c r="C71" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D71" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E71" s="43"/>
-      <c r="F71" s="43"/>
-      <c r="G71" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="H71" s="43"/>
-      <c r="I71" s="43"/>
-      <c r="J71" s="43"/>
-      <c r="K71" s="34"/>
-      <c r="L71" s="34"/>
-    </row>
-    <row r="72" spans="2:14">
-      <c r="B72" s="50"/>
-      <c r="C72" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="D72" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E72" s="43"/>
-      <c r="F72" s="43"/>
-      <c r="G72" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="H72" s="43"/>
-      <c r="I72" s="43"/>
-      <c r="J72" s="43"/>
-      <c r="K72" s="34"/>
-      <c r="L72" s="34"/>
-    </row>
-    <row r="73" spans="2:14">
-      <c r="B73" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="C73" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="D73" s="27" t="s">
-        <v>177</v>
-      </c>
-      <c r="E73" s="43"/>
-      <c r="F73" s="43"/>
-      <c r="G73" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="H73" s="43"/>
-      <c r="I73" s="43"/>
-      <c r="J73" s="43"/>
-      <c r="K73" s="34"/>
-      <c r="L73" s="34"/>
-    </row>
-    <row r="74" spans="2:14">
-      <c r="B74" s="49"/>
-      <c r="C74" s="34" t="s">
-        <v>141</v>
-      </c>
-      <c r="D74" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="E74" s="43"/>
-      <c r="F74" s="43"/>
-      <c r="G74" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="H74" s="43"/>
-      <c r="I74" s="43"/>
-      <c r="J74" s="43"/>
-      <c r="K74" s="34"/>
-      <c r="L74" s="34"/>
-    </row>
-    <row r="75" spans="2:14">
-      <c r="B75" s="49"/>
-      <c r="C75" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="D75" s="27" t="s">
-        <v>179</v>
-      </c>
-      <c r="E75" s="43"/>
-      <c r="F75" s="43"/>
-      <c r="G75" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="H75" s="43"/>
-      <c r="I75" s="43"/>
-      <c r="J75" s="43"/>
-      <c r="K75" s="34"/>
-      <c r="L75" s="34"/>
-    </row>
-    <row r="76" spans="2:14">
-      <c r="B76" s="49"/>
-      <c r="C76" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D76" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E76" s="43"/>
-      <c r="F76" s="43"/>
-      <c r="G76" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="H76" s="43"/>
-      <c r="I76" s="43"/>
-      <c r="J76" s="43"/>
-      <c r="K76" s="34"/>
-      <c r="L76" s="34"/>
-    </row>
-    <row r="77" spans="2:14">
-      <c r="B77" s="50"/>
-      <c r="C77" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="D77" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E77" s="43"/>
-      <c r="F77" s="43"/>
-      <c r="G77" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="H77" s="43"/>
-      <c r="I77" s="43"/>
-      <c r="J77" s="43"/>
-      <c r="K77" s="34"/>
-      <c r="L77" s="34"/>
-    </row>
-    <row r="78" spans="2:14" ht="25.5">
-      <c r="B78" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="C78" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="D78" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="E78" s="43"/>
-      <c r="F78" s="43"/>
-      <c r="G78" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="H78" s="43"/>
-      <c r="I78" s="43"/>
-      <c r="J78" s="43"/>
-      <c r="K78" s="34"/>
-      <c r="L78" s="34"/>
-    </row>
-    <row r="79" spans="2:14" ht="25.5">
-      <c r="B79" s="49"/>
-      <c r="C79" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="D79" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="E79" s="43"/>
-      <c r="F79" s="43"/>
-      <c r="G79" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="H79" s="43"/>
-      <c r="I79" s="43"/>
-      <c r="J79" s="43"/>
-      <c r="K79" s="34"/>
-      <c r="L79" s="34"/>
-    </row>
-    <row r="80" spans="2:14">
-      <c r="B80" s="49"/>
-      <c r="C80" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D80" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E80" s="43"/>
+      <c r="D80" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E80" s="47" t="s">
+        <v>30</v>
+      </c>
       <c r="F80" s="43"/>
-      <c r="G80" s="34" t="s">
-        <v>44</v>
+      <c r="G80" s="33" t="s">
+        <v>273</v>
       </c>
       <c r="H80" s="43"/>
       <c r="I80" s="43"/>
@@ -4068,17 +4492,19 @@
       <c r="L80" s="34"/>
     </row>
     <row r="81" spans="2:12">
-      <c r="B81" s="50"/>
-      <c r="C81" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="D81" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E81" s="43"/>
+      <c r="B81" s="57"/>
+      <c r="C81" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="D81" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E81" s="47" t="s">
+        <v>30</v>
+      </c>
       <c r="F81" s="43"/>
       <c r="G81" s="33" t="s">
-        <v>44</v>
+        <v>273</v>
       </c>
       <c r="H81" s="43"/>
       <c r="I81" s="43"/>
@@ -4087,19 +4513,19 @@
       <c r="L81" s="34"/>
     </row>
     <row r="82" spans="2:12">
-      <c r="B82" s="48" t="s">
-        <v>128</v>
-      </c>
-      <c r="C82" s="34" t="s">
-        <v>128</v>
-      </c>
-      <c r="D82" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="E82" s="43"/>
+      <c r="B82" s="57"/>
+      <c r="C82" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="D82" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E82" s="47" t="s">
+        <v>30</v>
+      </c>
       <c r="F82" s="43"/>
       <c r="G82" s="33" t="s">
-        <v>149</v>
+        <v>273</v>
       </c>
       <c r="H82" s="43"/>
       <c r="I82" s="43"/>
@@ -4108,17 +4534,19 @@
       <c r="L82" s="34"/>
     </row>
     <row r="83" spans="2:12">
-      <c r="B83" s="49"/>
-      <c r="C83" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="D83" s="27" t="s">
-        <v>183</v>
-      </c>
-      <c r="E83" s="43"/>
+      <c r="B83" s="57"/>
+      <c r="C83" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="D83" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E83" s="47" t="s">
+        <v>30</v>
+      </c>
       <c r="F83" s="43"/>
       <c r="G83" s="33" t="s">
-        <v>149</v>
+        <v>273</v>
       </c>
       <c r="H83" s="43"/>
       <c r="I83" s="43"/>
@@ -4127,17 +4555,19 @@
       <c r="L83" s="34"/>
     </row>
     <row r="84" spans="2:12">
-      <c r="B84" s="49"/>
-      <c r="C84" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="D84" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="E84" s="43"/>
+      <c r="B84" s="58"/>
+      <c r="C84" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="D84" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E84" s="47" t="s">
+        <v>30</v>
+      </c>
       <c r="F84" s="43"/>
       <c r="G84" s="33" t="s">
-        <v>149</v>
+        <v>273</v>
       </c>
       <c r="H84" s="43"/>
       <c r="I84" s="43"/>
@@ -4146,17 +4576,21 @@
       <c r="L84" s="34"/>
     </row>
     <row r="85" spans="2:12">
-      <c r="B85" s="49"/>
+      <c r="B85" s="63" t="s">
+        <v>127</v>
+      </c>
       <c r="C85" s="34" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="D85" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="E85" s="43"/>
+        <v>168</v>
+      </c>
+      <c r="E85" s="33" t="s">
+        <v>243</v>
+      </c>
       <c r="F85" s="43"/>
       <c r="G85" s="33" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="H85" s="43"/>
       <c r="I85" s="43"/>
@@ -4164,18 +4598,20 @@
       <c r="K85" s="34"/>
       <c r="L85" s="34"/>
     </row>
-    <row r="86" spans="2:12">
-      <c r="B86" s="50"/>
+    <row r="86" spans="2:12" ht="51">
+      <c r="B86" s="64"/>
       <c r="C86" s="34" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="D86" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="E86" s="43"/>
+        <v>170</v>
+      </c>
+      <c r="E86" s="33" t="s">
+        <v>252</v>
+      </c>
       <c r="F86" s="43"/>
       <c r="G86" s="33" t="s">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="H86" s="43"/>
       <c r="I86" s="43"/>
@@ -4183,22 +4619,515 @@
       <c r="K86" s="34"/>
       <c r="L86" s="34"/>
     </row>
+    <row r="87" spans="2:12">
+      <c r="B87" s="64"/>
+      <c r="C87" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="D87" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="E87" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="F87" s="43"/>
+      <c r="G87" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H87" s="43"/>
+      <c r="I87" s="43"/>
+      <c r="J87" s="43"/>
+      <c r="K87" s="34"/>
+      <c r="L87" s="34"/>
+    </row>
+    <row r="88" spans="2:12">
+      <c r="B88" s="64"/>
+      <c r="C88" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="D88" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="E88" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="F88" s="43"/>
+      <c r="G88" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H88" s="43"/>
+      <c r="I88" s="43"/>
+      <c r="J88" s="43"/>
+      <c r="K88" s="34"/>
+      <c r="L88" s="34"/>
+    </row>
+    <row r="89" spans="2:12" ht="89.25">
+      <c r="B89" s="64"/>
+      <c r="C89" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D89" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="E89" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="F89" s="47"/>
+      <c r="G89" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="H89" s="47"/>
+      <c r="I89" s="47"/>
+      <c r="J89" s="47"/>
+      <c r="K89" s="34"/>
+      <c r="L89" s="34"/>
+    </row>
+    <row r="90" spans="2:12" ht="25.5">
+      <c r="B90" s="64"/>
+      <c r="C90" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="D90" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E90" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="F90" s="43"/>
+      <c r="G90" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H90" s="43"/>
+      <c r="I90" s="43"/>
+      <c r="J90" s="43"/>
+      <c r="K90" s="34"/>
+      <c r="L90" s="34"/>
+    </row>
+    <row r="91" spans="2:12">
+      <c r="B91" s="63" t="s">
+        <v>131</v>
+      </c>
+      <c r="C91" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D91" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="E91" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="F91" s="43"/>
+      <c r="G91" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H91" s="43"/>
+      <c r="I91" s="43"/>
+      <c r="J91" s="43"/>
+      <c r="K91" s="34"/>
+      <c r="L91" s="34"/>
+    </row>
+    <row r="92" spans="2:12">
+      <c r="B92" s="64"/>
+      <c r="C92" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="D92" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="E92" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="F92" s="43"/>
+      <c r="G92" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H92" s="43"/>
+      <c r="I92" s="43"/>
+      <c r="J92" s="43"/>
+      <c r="K92" s="34"/>
+      <c r="L92" s="34"/>
+    </row>
+    <row r="93" spans="2:12">
+      <c r="B93" s="64"/>
+      <c r="C93" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="D93" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="E93" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="F93" s="43"/>
+      <c r="G93" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H93" s="43"/>
+      <c r="I93" s="43"/>
+      <c r="J93" s="43"/>
+      <c r="K93" s="34"/>
+      <c r="L93" s="34"/>
+    </row>
+    <row r="94" spans="2:12" ht="25.5">
+      <c r="B94" s="64"/>
+      <c r="C94" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="D94" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E94" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="F94" s="43"/>
+      <c r="G94" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H94" s="43"/>
+      <c r="I94" s="43"/>
+      <c r="J94" s="43"/>
+      <c r="K94" s="34"/>
+      <c r="L94" s="34"/>
+    </row>
+    <row r="95" spans="2:12">
+      <c r="B95" s="65"/>
+      <c r="C95" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="D95" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E95" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="F95" s="43"/>
+      <c r="G95" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H95" s="43"/>
+      <c r="I95" s="43"/>
+      <c r="J95" s="43"/>
+      <c r="K95" s="34"/>
+      <c r="L95" s="34"/>
+    </row>
+    <row r="96" spans="2:12" ht="51">
+      <c r="B96" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="C96" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="D96" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="E96" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="F96" s="43"/>
+      <c r="G96" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="H96" s="43"/>
+      <c r="I96" s="43"/>
+      <c r="J96" s="43"/>
+      <c r="K96" s="34"/>
+      <c r="L96" s="34"/>
+    </row>
+    <row r="97" spans="2:12">
+      <c r="B97" s="64"/>
+      <c r="C97" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D97" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="E97" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="F97" s="43"/>
+      <c r="G97" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H97" s="43"/>
+      <c r="I97" s="43"/>
+      <c r="J97" s="43"/>
+      <c r="K97" s="34"/>
+      <c r="L97" s="34"/>
+    </row>
+    <row r="98" spans="2:12" ht="51">
+      <c r="B98" s="64"/>
+      <c r="C98" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="D98" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="E98" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="F98" s="43"/>
+      <c r="G98" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="H98" s="43"/>
+      <c r="I98" s="43"/>
+      <c r="J98" s="43"/>
+      <c r="K98" s="34"/>
+      <c r="L98" s="34"/>
+    </row>
+    <row r="99" spans="2:12" ht="25.5">
+      <c r="B99" s="64"/>
+      <c r="C99" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="D99" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E99" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="F99" s="43"/>
+      <c r="G99" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H99" s="43"/>
+      <c r="I99" s="43"/>
+      <c r="J99" s="43"/>
+      <c r="K99" s="34"/>
+      <c r="L99" s="34"/>
+    </row>
+    <row r="100" spans="2:12" ht="25.5">
+      <c r="B100" s="65"/>
+      <c r="C100" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="D100" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E100" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="F100" s="43"/>
+      <c r="G100" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H100" s="43"/>
+      <c r="I100" s="43"/>
+      <c r="J100" s="43"/>
+      <c r="K100" s="34"/>
+      <c r="L100" s="34"/>
+    </row>
+    <row r="101" spans="2:12" ht="38.25">
+      <c r="B101" s="63" t="s">
+        <v>250</v>
+      </c>
+      <c r="C101" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="D101" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="E101" s="47" t="s">
+        <v>262</v>
+      </c>
+      <c r="F101" s="43"/>
+      <c r="G101" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H101" s="43"/>
+      <c r="I101" s="43"/>
+      <c r="J101" s="43"/>
+      <c r="K101" s="34"/>
+      <c r="L101" s="34"/>
+    </row>
+    <row r="102" spans="2:12" ht="25.5">
+      <c r="B102" s="64"/>
+      <c r="C102" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="D102" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="E102" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="F102" s="43"/>
+      <c r="G102" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="H102" s="43"/>
+      <c r="I102" s="43"/>
+      <c r="J102" s="43"/>
+      <c r="K102" s="34"/>
+      <c r="L102" s="34"/>
+    </row>
+    <row r="103" spans="2:12">
+      <c r="B103" s="64"/>
+      <c r="C103" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="D103" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E103" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="F103" s="43"/>
+      <c r="G103" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="H103" s="43"/>
+      <c r="I103" s="43"/>
+      <c r="J103" s="43"/>
+      <c r="K103" s="34"/>
+      <c r="L103" s="34"/>
+    </row>
+    <row r="104" spans="2:12" ht="25.5">
+      <c r="B104" s="65"/>
+      <c r="C104" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="D104" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E104" s="34" t="s">
+        <v>246</v>
+      </c>
+      <c r="F104" s="43"/>
+      <c r="G104" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H104" s="43"/>
+      <c r="I104" s="43"/>
+      <c r="J104" s="43"/>
+      <c r="K104" s="34"/>
+      <c r="L104" s="34"/>
+    </row>
+    <row r="105" spans="2:12">
+      <c r="B105" s="63" t="s">
+        <v>251</v>
+      </c>
+      <c r="C105" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D105" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="E105" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="F105" s="43"/>
+      <c r="G105" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="H105" s="43"/>
+      <c r="I105" s="43"/>
+      <c r="J105" s="43"/>
+      <c r="K105" s="34"/>
+      <c r="L105" s="34"/>
+    </row>
+    <row r="106" spans="2:12">
+      <c r="B106" s="64"/>
+      <c r="C106" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="D106" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="E106" s="33" t="s">
+        <v>266</v>
+      </c>
+      <c r="F106" s="43"/>
+      <c r="G106" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="H106" s="43"/>
+      <c r="I106" s="43"/>
+      <c r="J106" s="43"/>
+      <c r="K106" s="34"/>
+      <c r="L106" s="34"/>
+    </row>
+    <row r="107" spans="2:12">
+      <c r="B107" s="64"/>
+      <c r="C107" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="D107" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="E107" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="F107" s="43"/>
+      <c r="G107" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="H107" s="43"/>
+      <c r="I107" s="43"/>
+      <c r="J107" s="43"/>
+      <c r="K107" s="34"/>
+      <c r="L107" s="34"/>
+    </row>
+    <row r="108" spans="2:12">
+      <c r="B108" s="64"/>
+      <c r="C108" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="D108" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="E108" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="F108" s="43"/>
+      <c r="G108" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="H108" s="43"/>
+      <c r="I108" s="43"/>
+      <c r="J108" s="43"/>
+      <c r="K108" s="34"/>
+      <c r="L108" s="34"/>
+    </row>
+    <row r="109" spans="2:12">
+      <c r="B109" s="65"/>
+      <c r="C109" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="D109" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="E109" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F109" s="43"/>
+      <c r="G109" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H109" s="43"/>
+      <c r="I109" s="43"/>
+      <c r="J109" s="43"/>
+      <c r="K109" s="34"/>
+      <c r="L109" s="34"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="16">
+    <mergeCell ref="B58:B63"/>
+    <mergeCell ref="B64:B79"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="B96:B100"/>
+    <mergeCell ref="B101:B104"/>
+    <mergeCell ref="B105:B109"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B80:B84"/>
+    <mergeCell ref="B85:B90"/>
+    <mergeCell ref="B91:B95"/>
     <mergeCell ref="B28:B36"/>
     <mergeCell ref="B37:B42"/>
     <mergeCell ref="B43:B50"/>
     <mergeCell ref="B51:B53"/>
     <mergeCell ref="B10:B27"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="B73:B77"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B58:B62"/>
-    <mergeCell ref="B63:B67"/>
-    <mergeCell ref="B68:B72"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="1" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
analytics metrics sheet added2
</commit_message>
<xml_diff>
--- a/Form SpecificationsV0.1_DRAFT.xlsx
+++ b/Form SpecificationsV0.1_DRAFT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Approval" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="265">
   <si>
     <t xml:space="preserve"> Specifications Author:</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Facebook login</t>
   </si>
   <si>
-    <t>Google login</t>
-  </si>
-  <si>
     <t>Signup</t>
   </si>
   <si>
@@ -520,9 +517,6 @@
   </si>
   <si>
     <t>Employer Login page</t>
-  </si>
-  <si>
-    <t>link to Google addin Code</t>
   </si>
   <si>
     <t>Open employee signup page</t>
@@ -1000,6 +994,27 @@
   </si>
   <si>
     <t>External Data Source (Yes, NO)</t>
+  </si>
+  <si>
+    <t>LinkedIn login</t>
+  </si>
+  <si>
+    <t>link to LinkedIn addin Code</t>
+  </si>
+  <si>
+    <t>Primary= 0, Secondary= 1, High school= 2, Certificate= 3, Ordinary Diploma= 4, Advanced Diploma= 5, Bachelor Degree= 6, Masters= 7, Doctorial or Professional= 8)</t>
+  </si>
+  <si>
+    <t>LEVEL_EDU</t>
+  </si>
+  <si>
+    <t>USER_NAME</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>LOGO</t>
   </si>
 </sst>
 </file>
@@ -1334,61 +1349,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1405,6 +1365,61 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1759,14 +1774,14 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.19921875" customWidth="1"/>
-    <col min="2" max="2" width="24.796875" customWidth="1"/>
-    <col min="3" max="3" width="38.59765625" customWidth="1"/>
-    <col min="4" max="4" width="26.3984375" customWidth="1"/>
-    <col min="5" max="5" width="26.796875" customWidth="1"/>
-    <col min="6" max="1025" width="8.796875" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" customWidth="1"/>
+    <col min="6" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23" x14ac:dyDescent="0.25">
@@ -1977,33 +1992,33 @@
   </sheetPr>
   <dimension ref="A1:P109"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C36" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.796875" style="17" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="17" customWidth="1"/>
     <col min="3" max="3" width="33" style="17" customWidth="1"/>
-    <col min="4" max="4" width="23.59765625" style="26" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="26" customWidth="1"/>
     <col min="5" max="5" width="27" style="16" customWidth="1"/>
-    <col min="6" max="8" width="20.3984375" style="58" customWidth="1"/>
-    <col min="9" max="9" width="13.3984375" style="16" customWidth="1"/>
-    <col min="10" max="10" width="10.19921875" style="16" customWidth="1"/>
-    <col min="11" max="11" width="15.3984375" style="16" customWidth="1"/>
-    <col min="12" max="12" width="12.59765625" style="16" customWidth="1"/>
+    <col min="6" max="8" width="20.33203125" style="39" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="16" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" style="16" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" style="16" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" style="16" customWidth="1"/>
     <col min="13" max="13" width="14" style="17" customWidth="1"/>
-    <col min="14" max="14" width="24.19921875" style="17" customWidth="1"/>
-    <col min="15" max="15" width="21.59765625" style="17" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="24.1640625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="21.6640625" style="17" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="13" style="16" hidden="1" customWidth="1"/>
-    <col min="17" max="1028" width="21.59765625" customWidth="1"/>
+    <col min="17" max="1028" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" s="20" customFormat="1" ht="91" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:16" s="20" customFormat="1" ht="65" x14ac:dyDescent="0.2">
       <c r="B1" s="18" t="s">
         <v>13</v>
       </c>
@@ -2011,19 +2026,19 @@
         <v>14</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>31</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G1" s="18" t="s">
         <v>15</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>16</v>
@@ -2051,8 +2066,8 @@
       </c>
     </row>
     <row r="2" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="42" t="s">
-        <v>158</v>
+      <c r="B2" s="40" t="s">
+        <v>156</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>39</v>
@@ -2063,11 +2078,13 @@
       <c r="E2" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="56"/>
+      <c r="F2" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="G2" s="36"/>
+      <c r="H2" s="37"/>
       <c r="I2" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>
@@ -2082,21 +2099,23 @@
       </c>
     </row>
     <row r="3" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="43"/>
+      <c r="B3" s="41"/>
       <c r="C3" s="24" t="s">
         <v>40</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="56"/>
+        <v>103</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>262</v>
+      </c>
+      <c r="G3" s="36"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J3" s="22"/>
       <c r="K3" s="22"/>
@@ -2112,21 +2131,23 @@
       </c>
     </row>
     <row r="4" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="43"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="24" t="s">
         <v>41</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>227</v>
-      </c>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="56"/>
+        <v>225</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>263</v>
+      </c>
+      <c r="G4" s="36"/>
+      <c r="H4" s="37"/>
       <c r="I4" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
@@ -2141,19 +2162,19 @@
       </c>
     </row>
     <row r="5" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="43"/>
+      <c r="B5" s="41"/>
       <c r="C5" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="56"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="37"/>
       <c r="I5" s="23" t="s">
         <v>27</v>
       </c>
@@ -2164,21 +2185,21 @@
       <c r="N5" s="22"/>
     </row>
     <row r="6" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="43"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="56"/>
+        <v>102</v>
+      </c>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="37"/>
       <c r="I6" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
@@ -2187,7 +2208,7 @@
       <c r="N6" s="22"/>
     </row>
     <row r="7" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="43"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="24" t="s">
         <v>42</v>
       </c>
@@ -2195,13 +2216,13 @@
         <v>24</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="56"/>
+        <v>104</v>
+      </c>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="37"/>
       <c r="I7" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
@@ -2210,21 +2231,21 @@
       <c r="N7" s="22"/>
     </row>
     <row r="8" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="43"/>
+      <c r="B8" s="41"/>
       <c r="C8" s="24" t="s">
-        <v>43</v>
+        <v>258</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="56"/>
+        <v>259</v>
+      </c>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
       <c r="I8" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
@@ -2233,19 +2254,19 @@
       <c r="N8" s="22"/>
     </row>
     <row r="9" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="43"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="56"/>
+        <v>155</v>
+      </c>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="37"/>
       <c r="I9" s="23" t="s">
         <v>27</v>
       </c>
@@ -2256,23 +2277,23 @@
       <c r="N9" s="31"/>
     </row>
     <row r="10" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="44" t="s">
-        <v>159</v>
+      <c r="B10" s="53" t="s">
+        <v>157</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="56"/>
+        <v>164</v>
+      </c>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
       <c r="I10" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J10" s="31"/>
       <c r="K10" s="31"/>
@@ -2281,21 +2302,21 @@
       <c r="N10" s="31"/>
     </row>
     <row r="11" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="45"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="24" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="56"/>
+        <v>165</v>
+      </c>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="37"/>
       <c r="I11" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
@@ -2304,19 +2325,19 @@
       <c r="N11" s="31"/>
     </row>
     <row r="12" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="45"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D12" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="E12" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="E12" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="56"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="37"/>
       <c r="I12" s="23" t="s">
         <v>26</v>
       </c>
@@ -2327,21 +2348,21 @@
       <c r="N12" s="31"/>
     </row>
     <row r="13" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="45"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="24" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="56"/>
+        <v>172</v>
+      </c>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="37"/>
       <c r="I13" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J13" s="31"/>
       <c r="K13" s="31"/>
@@ -2350,21 +2371,21 @@
       <c r="N13" s="31"/>
     </row>
     <row r="14" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="45"/>
+      <c r="B14" s="54"/>
       <c r="C14" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>224</v>
-      </c>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="56"/>
+        <v>222</v>
+      </c>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="37"/>
       <c r="I14" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J14" s="31"/>
       <c r="K14" s="31"/>
@@ -2373,21 +2394,21 @@
       <c r="N14" s="31"/>
     </row>
     <row r="15" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="45"/>
+      <c r="B15" s="54"/>
       <c r="C15" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>222</v>
-      </c>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="56"/>
+        <v>220</v>
+      </c>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
       <c r="I15" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J15" s="31"/>
       <c r="K15" s="31"/>
@@ -2395,22 +2416,28 @@
       <c r="M15" s="31"/>
       <c r="N15" s="31"/>
     </row>
-    <row r="16" spans="2:16" s="25" customFormat="1" ht="78" x14ac:dyDescent="0.2">
-      <c r="B16" s="45"/>
+    <row r="16" spans="2:16" s="25" customFormat="1" ht="91" x14ac:dyDescent="0.2">
+      <c r="B16" s="54"/>
       <c r="C16" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="56"/>
+        <v>173</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>261</v>
+      </c>
+      <c r="G16" s="36" t="s">
+        <v>260</v>
+      </c>
+      <c r="H16" s="37">
+        <v>1</v>
+      </c>
       <c r="I16" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J16" s="31"/>
       <c r="K16" s="31"/>
@@ -2419,21 +2446,21 @@
       <c r="N16" s="31"/>
     </row>
     <row r="17" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="45"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="33" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="37"/>
       <c r="I17" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J17" s="31"/>
       <c r="K17" s="31"/>
@@ -2442,21 +2469,21 @@
       <c r="N17" s="31"/>
     </row>
     <row r="18" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="45"/>
+      <c r="B18" s="54"/>
       <c r="C18" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="56"/>
+        <v>184</v>
+      </c>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
       <c r="I18" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J18" s="31"/>
       <c r="K18" s="31"/>
@@ -2465,21 +2492,21 @@
       <c r="N18" s="31"/>
     </row>
     <row r="19" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="45"/>
+      <c r="B19" s="54"/>
       <c r="C19" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="56"/>
+        <v>180</v>
+      </c>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
       <c r="I19" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J19" s="31"/>
       <c r="K19" s="31"/>
@@ -2488,21 +2515,21 @@
       <c r="N19" s="31"/>
     </row>
     <row r="20" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="45"/>
+      <c r="B20" s="54"/>
       <c r="C20" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="56"/>
+        <v>175</v>
+      </c>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="37"/>
       <c r="I20" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J20" s="31"/>
       <c r="K20" s="31"/>
@@ -2511,21 +2538,21 @@
       <c r="N20" s="31"/>
     </row>
     <row r="21" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="45"/>
+      <c r="B21" s="54"/>
       <c r="C21" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="56"/>
+        <v>214</v>
+      </c>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="37"/>
       <c r="I21" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J21" s="31"/>
       <c r="K21" s="31"/>
@@ -2534,21 +2561,21 @@
       <c r="N21" s="31"/>
     </row>
     <row r="22" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="45"/>
+      <c r="B22" s="54"/>
       <c r="C22" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="56"/>
+        <v>176</v>
+      </c>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="37"/>
       <c r="I22" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J22" s="31"/>
       <c r="K22" s="31"/>
@@ -2557,21 +2584,21 @@
       <c r="N22" s="31"/>
     </row>
     <row r="23" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="45"/>
+      <c r="B23" s="54"/>
       <c r="C23" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="56"/>
+        <v>177</v>
+      </c>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="37"/>
       <c r="I23" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J23" s="31"/>
       <c r="K23" s="31"/>
@@ -2580,21 +2607,21 @@
       <c r="N23" s="31"/>
     </row>
     <row r="24" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="45"/>
+      <c r="B24" s="54"/>
       <c r="C24" s="25" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="56"/>
+        <v>103</v>
+      </c>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="37"/>
       <c r="I24" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J24" s="31"/>
       <c r="K24" s="31"/>
@@ -2603,21 +2630,21 @@
       <c r="N24" s="31"/>
     </row>
     <row r="25" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="45"/>
+      <c r="B25" s="54"/>
       <c r="C25" s="24" t="s">
         <v>41</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="56"/>
+        <v>178</v>
+      </c>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="37"/>
       <c r="I25" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J25" s="31"/>
       <c r="K25" s="31"/>
@@ -2626,21 +2653,21 @@
       <c r="N25" s="31"/>
     </row>
     <row r="26" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="45"/>
+      <c r="B26" s="54"/>
       <c r="C26" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="56"/>
+        <v>179</v>
+      </c>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="37"/>
       <c r="I26" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J26" s="31"/>
       <c r="K26" s="31"/>
@@ -2649,21 +2676,21 @@
       <c r="N26" s="31"/>
     </row>
     <row r="27" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="46"/>
+      <c r="B27" s="55"/>
       <c r="C27" s="33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="56"/>
+        <v>155</v>
+      </c>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="37"/>
       <c r="I27" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J27" s="22"/>
       <c r="K27" s="22"/>
@@ -2678,11 +2705,11 @@
       </c>
     </row>
     <row r="28" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="42" t="s">
-        <v>58</v>
+      <c r="B28" s="40" t="s">
+        <v>57</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D28" s="32" t="s">
         <v>24</v>
@@ -2690,11 +2717,11 @@
       <c r="E28" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
       <c r="I28" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J28" s="22"/>
       <c r="K28" s="22"/>
@@ -2703,9 +2730,9 @@
       <c r="N28" s="22"/>
     </row>
     <row r="29" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="43"/>
+      <c r="B29" s="41"/>
       <c r="C29" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D29" s="32" t="s">
         <v>24</v>
@@ -2713,11 +2740,11 @@
       <c r="E29" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
       <c r="I29" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J29" s="22"/>
       <c r="K29" s="22"/>
@@ -2726,7 +2753,7 @@
       <c r="N29" s="22"/>
     </row>
     <row r="30" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="43"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="24" t="s">
         <v>34</v>
       </c>
@@ -2736,9 +2763,9 @@
       <c r="E30" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
       <c r="I30" s="22" t="s">
         <v>24</v>
       </c>
@@ -2751,7 +2778,7 @@
       <c r="P30" s="16"/>
     </row>
     <row r="31" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="43"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="24" t="s">
         <v>32</v>
       </c>
@@ -2761,9 +2788,9 @@
       <c r="E31" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
       <c r="I31" s="22" t="s">
         <v>24</v>
       </c>
@@ -2776,9 +2803,9 @@
       <c r="P31" s="16"/>
     </row>
     <row r="32" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="43"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D32" s="32" t="s">
         <v>24</v>
@@ -2786,9 +2813,9 @@
       <c r="E32" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="56"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
       <c r="I32" s="22" t="s">
         <v>24</v>
       </c>
@@ -2801,7 +2828,7 @@
       <c r="P32" s="16"/>
     </row>
     <row r="33" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="43"/>
+      <c r="B33" s="41"/>
       <c r="C33" s="24" t="s">
         <v>33</v>
       </c>
@@ -2811,9 +2838,9 @@
       <c r="E33" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="56"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
       <c r="I33" s="22" t="s">
         <v>24</v>
       </c>
@@ -2826,9 +2853,9 @@
       <c r="P33" s="16"/>
     </row>
     <row r="34" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="43"/>
+      <c r="B34" s="41"/>
       <c r="C34" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D34" s="32" t="s">
         <v>24</v>
@@ -2836,9 +2863,9 @@
       <c r="E34" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F34" s="56"/>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
       <c r="I34" s="22" t="s">
         <v>24</v>
       </c>
@@ -2851,9 +2878,9 @@
       <c r="P34" s="16"/>
     </row>
     <row r="35" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="43"/>
+      <c r="B35" s="41"/>
       <c r="C35" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D35" s="32" t="s">
         <v>24</v>
@@ -2861,9 +2888,9 @@
       <c r="E35" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
       <c r="I35" s="22" t="s">
         <v>24</v>
       </c>
@@ -2876,9 +2903,9 @@
       <c r="P35" s="16"/>
     </row>
     <row r="36" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="47"/>
+      <c r="B36" s="45"/>
       <c r="C36" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D36" s="32" t="s">
         <v>24</v>
@@ -2886,9 +2913,9 @@
       <c r="E36" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F36" s="56"/>
-      <c r="G36" s="56"/>
-      <c r="H36" s="56"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37"/>
       <c r="I36" s="22" t="s">
         <v>24</v>
       </c>
@@ -2901,23 +2928,23 @@
       <c r="P36" s="16"/>
     </row>
     <row r="37" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="37" t="s">
-        <v>59</v>
+      <c r="B37" s="46" t="s">
+        <v>58</v>
       </c>
       <c r="C37" s="24" t="s">
         <v>34</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="F37" s="55"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="56"/>
+        <v>164</v>
+      </c>
+      <c r="F37" s="36"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="37"/>
       <c r="I37" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J37" s="22"/>
       <c r="K37" s="22"/>
@@ -2928,21 +2955,21 @@
       <c r="P37" s="16"/>
     </row>
     <row r="38" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="48"/>
+      <c r="B38" s="47"/>
       <c r="C38" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="56"/>
+        <v>182</v>
+      </c>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="37"/>
       <c r="I38" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J38" s="22"/>
       <c r="K38" s="22"/>
@@ -2953,19 +2980,19 @@
       <c r="P38" s="16"/>
     </row>
     <row r="39" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="48"/>
+      <c r="B39" s="47"/>
       <c r="C39" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="F39" s="55"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="56"/>
+        <v>168</v>
+      </c>
+      <c r="F39" s="36"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="37"/>
       <c r="I39" s="23" t="s">
         <v>26</v>
       </c>
@@ -2978,7 +3005,7 @@
       <c r="P39" s="16"/>
     </row>
     <row r="40" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="48"/>
+      <c r="B40" s="47"/>
       <c r="C40" s="24" t="s">
         <v>35</v>
       </c>
@@ -2986,13 +3013,13 @@
         <v>35</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="F40" s="55"/>
-      <c r="G40" s="55"/>
-      <c r="H40" s="56"/>
+        <v>176</v>
+      </c>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="37"/>
       <c r="I40" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J40" s="22"/>
       <c r="K40" s="22"/>
@@ -3003,21 +3030,21 @@
       <c r="P40" s="16"/>
     </row>
     <row r="41" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="48"/>
+      <c r="B41" s="47"/>
       <c r="C41" s="24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="F41" s="55"/>
-      <c r="G41" s="55"/>
-      <c r="H41" s="56"/>
+        <v>172</v>
+      </c>
+      <c r="F41" s="36"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="37"/>
       <c r="I41" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J41" s="22"/>
       <c r="K41" s="22"/>
@@ -3028,9 +3055,9 @@
       <c r="P41" s="16"/>
     </row>
     <row r="42" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="38"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D42" s="21" t="s">
         <v>24</v>
@@ -3038,9 +3065,9 @@
       <c r="E42" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F42" s="55"/>
-      <c r="G42" s="55"/>
-      <c r="H42" s="56"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="37"/>
       <c r="I42" s="23" t="s">
         <v>24</v>
       </c>
@@ -3053,23 +3080,23 @@
       <c r="P42" s="16"/>
     </row>
     <row r="43" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="39" t="s">
-        <v>65</v>
+      <c r="B43" s="49" t="s">
+        <v>64</v>
       </c>
       <c r="C43" s="24" t="s">
         <v>37</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="F43" s="55"/>
-      <c r="G43" s="55"/>
-      <c r="H43" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="37"/>
       <c r="I43" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J43" s="22"/>
       <c r="K43" s="22"/>
@@ -3080,21 +3107,21 @@
       <c r="P43" s="16"/>
     </row>
     <row r="44" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="40"/>
+      <c r="B44" s="50"/>
       <c r="C44" s="24" t="s">
         <v>36</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="F44" s="55"/>
-      <c r="G44" s="55"/>
-      <c r="H44" s="56"/>
+        <v>184</v>
+      </c>
+      <c r="F44" s="36"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="37"/>
       <c r="I44" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J44" s="22"/>
       <c r="K44" s="22"/>
@@ -3105,21 +3132,21 @@
       <c r="P44" s="16"/>
     </row>
     <row r="45" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="40"/>
+      <c r="B45" s="50"/>
       <c r="C45" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>182</v>
-      </c>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="56"/>
+        <v>180</v>
+      </c>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
       <c r="I45" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J45" s="22"/>
       <c r="K45" s="22"/>
@@ -3130,21 +3157,21 @@
       <c r="P45" s="16"/>
     </row>
     <row r="46" spans="2:16" s="25" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="40"/>
+      <c r="B46" s="50"/>
       <c r="C46" s="24" t="s">
         <v>38</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="F46" s="55"/>
-      <c r="G46" s="55"/>
-      <c r="H46" s="56"/>
+        <v>185</v>
+      </c>
+      <c r="F46" s="36"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="37"/>
       <c r="I46" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J46" s="22"/>
       <c r="K46" s="22"/>
@@ -3154,22 +3181,22 @@
       <c r="O46" s="17"/>
       <c r="P46" s="16"/>
     </row>
-    <row r="47" spans="2:16" s="25" customFormat="1" ht="78" x14ac:dyDescent="0.2">
-      <c r="B47" s="40"/>
+    <row r="47" spans="2:16" s="25" customFormat="1" ht="65" x14ac:dyDescent="0.2">
+      <c r="B47" s="50"/>
       <c r="C47" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="F47" s="55"/>
-      <c r="G47" s="55"/>
-      <c r="H47" s="56"/>
+        <v>173</v>
+      </c>
+      <c r="F47" s="36"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="37"/>
       <c r="I47" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J47" s="22"/>
       <c r="K47" s="22"/>
@@ -3180,21 +3207,21 @@
       <c r="P47" s="16"/>
     </row>
     <row r="48" spans="2:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="40"/>
+      <c r="B48" s="50"/>
       <c r="C48" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="F48" s="55"/>
-      <c r="G48" s="55"/>
-      <c r="H48" s="56"/>
+        <v>186</v>
+      </c>
+      <c r="F48" s="36"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="37"/>
       <c r="I48" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J48" s="22"/>
       <c r="K48" s="22"/>
@@ -3205,21 +3232,21 @@
       <c r="P48" s="16"/>
     </row>
     <row r="49" spans="1:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="40"/>
+      <c r="B49" s="50"/>
       <c r="C49" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E49" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="F49" s="55"/>
-      <c r="G49" s="55"/>
-      <c r="H49" s="56"/>
+        <v>187</v>
+      </c>
+      <c r="F49" s="36"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="37"/>
       <c r="I49" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J49" s="22"/>
       <c r="K49" s="22"/>
@@ -3230,21 +3257,21 @@
       <c r="P49" s="16"/>
     </row>
     <row r="50" spans="1:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="41"/>
+      <c r="B50" s="51"/>
       <c r="C50" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="F50" s="55"/>
-      <c r="G50" s="55"/>
-      <c r="H50" s="56"/>
+        <v>188</v>
+      </c>
+      <c r="F50" s="36"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="37"/>
       <c r="I50" s="23" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J50" s="22"/>
       <c r="K50" s="22"/>
@@ -3255,23 +3282,23 @@
       <c r="P50" s="16"/>
     </row>
     <row r="51" spans="1:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="37" t="s">
-        <v>70</v>
+      <c r="B51" s="46" t="s">
+        <v>69</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="F51" s="55"/>
-      <c r="G51" s="55"/>
-      <c r="H51" s="56"/>
+        <v>189</v>
+      </c>
+      <c r="F51" s="36"/>
+      <c r="G51" s="36"/>
+      <c r="H51" s="37"/>
       <c r="I51" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J51" s="22"/>
       <c r="K51" s="22"/>
@@ -3282,21 +3309,21 @@
       <c r="P51" s="16"/>
     </row>
     <row r="52" spans="1:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="49"/>
+      <c r="B52" s="52"/>
       <c r="C52" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>192</v>
-      </c>
-      <c r="F52" s="55"/>
-      <c r="G52" s="55"/>
-      <c r="H52" s="56"/>
+        <v>190</v>
+      </c>
+      <c r="F52" s="36"/>
+      <c r="G52" s="36"/>
+      <c r="H52" s="37"/>
       <c r="I52" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J52" s="22"/>
       <c r="K52" s="22"/>
@@ -3307,19 +3334,19 @@
       <c r="P52" s="16"/>
     </row>
     <row r="53" spans="1:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="49"/>
+      <c r="B53" s="52"/>
       <c r="C53" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D53" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="F53" s="55"/>
-      <c r="G53" s="55"/>
-      <c r="H53" s="56"/>
+        <v>192</v>
+      </c>
+      <c r="F53" s="36"/>
+      <c r="G53" s="36"/>
+      <c r="H53" s="37"/>
       <c r="I53" s="23" t="s">
         <v>27</v>
       </c>
@@ -3332,23 +3359,23 @@
       <c r="P53" s="16"/>
     </row>
     <row r="54" spans="1:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="37" t="s">
-        <v>69</v>
+      <c r="B54" s="46" t="s">
+        <v>68</v>
       </c>
       <c r="C54" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="F54" s="36"/>
+      <c r="G54" s="36"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="23" t="s">
         <v>71</v>
-      </c>
-      <c r="D54" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="E54" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="F54" s="55"/>
-      <c r="G54" s="55"/>
-      <c r="H54" s="56"/>
-      <c r="I54" s="23" t="s">
-        <v>72</v>
       </c>
       <c r="J54" s="22"/>
       <c r="K54" s="22"/>
@@ -3359,19 +3386,19 @@
       <c r="P54" s="16"/>
     </row>
     <row r="55" spans="1:16" s="25" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="38"/>
+      <c r="B55" s="48"/>
       <c r="C55" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="F55" s="55"/>
-      <c r="G55" s="55"/>
-      <c r="H55" s="56"/>
+        <v>193</v>
+      </c>
+      <c r="F55" s="36"/>
+      <c r="G55" s="36"/>
+      <c r="H55" s="37"/>
       <c r="I55" s="23" t="s">
         <v>27</v>
       </c>
@@ -3384,23 +3411,23 @@
       <c r="P55" s="16"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B56" s="39" t="s">
+      <c r="B56" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C56" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C56" s="24" t="s">
-        <v>74</v>
-      </c>
       <c r="D56" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="F56" s="55"/>
-      <c r="G56" s="55"/>
-      <c r="H56" s="56"/>
+        <v>194</v>
+      </c>
+      <c r="F56" s="36"/>
+      <c r="G56" s="36"/>
+      <c r="H56" s="37"/>
       <c r="I56" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J56" s="28"/>
       <c r="K56" s="28"/>
@@ -3408,20 +3435,20 @@
       <c r="M56" s="24"/>
       <c r="N56" s="24"/>
     </row>
-    <row r="57" spans="1:16" ht="26" x14ac:dyDescent="0.2">
-      <c r="B57" s="40"/>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B57" s="50"/>
       <c r="C57" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="F57" s="55"/>
-      <c r="G57" s="55"/>
-      <c r="H57" s="56"/>
+        <v>195</v>
+      </c>
+      <c r="F57" s="36"/>
+      <c r="G57" s="36"/>
+      <c r="H57" s="37"/>
       <c r="I57" s="23" t="s">
         <v>27</v>
       </c>
@@ -3433,8 +3460,8 @@
     </row>
     <row r="58" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="25"/>
-      <c r="B58" s="42" t="s">
-        <v>155</v>
+      <c r="B58" s="40" t="s">
+        <v>154</v>
       </c>
       <c r="C58" s="24" t="s">
         <v>39</v>
@@ -3445,11 +3472,11 @@
       <c r="E58" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F58" s="55"/>
-      <c r="G58" s="55"/>
-      <c r="H58" s="56"/>
+      <c r="F58" s="36"/>
+      <c r="G58" s="36"/>
+      <c r="H58" s="37"/>
       <c r="I58" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J58" s="32"/>
       <c r="K58" s="32"/>
@@ -3459,21 +3486,21 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="25"/>
-      <c r="B59" s="43"/>
+      <c r="B59" s="41"/>
       <c r="C59" s="24" t="s">
         <v>40</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="F59" s="55"/>
-      <c r="G59" s="55"/>
-      <c r="H59" s="56"/>
+        <v>103</v>
+      </c>
+      <c r="F59" s="36"/>
+      <c r="G59" s="36"/>
+      <c r="H59" s="37"/>
       <c r="I59" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J59" s="32"/>
       <c r="K59" s="32"/>
@@ -3483,21 +3510,21 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="25"/>
-      <c r="B60" s="43"/>
+      <c r="B60" s="41"/>
       <c r="C60" s="24" t="s">
         <v>41</v>
       </c>
       <c r="D60" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E60" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="F60" s="55"/>
-      <c r="G60" s="55"/>
-      <c r="H60" s="56"/>
+        <v>196</v>
+      </c>
+      <c r="F60" s="36"/>
+      <c r="G60" s="36"/>
+      <c r="H60" s="37"/>
       <c r="I60" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J60" s="32"/>
       <c r="K60" s="32"/>
@@ -3507,19 +3534,19 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="25"/>
-      <c r="B61" s="43"/>
+      <c r="B61" s="41"/>
       <c r="C61" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D61" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E61" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F61" s="55"/>
-      <c r="G61" s="55"/>
-      <c r="H61" s="56"/>
+      <c r="F61" s="36"/>
+      <c r="G61" s="36"/>
+      <c r="H61" s="37"/>
       <c r="I61" s="23" t="s">
         <v>27</v>
       </c>
@@ -3529,23 +3556,23 @@
       <c r="M61" s="32"/>
       <c r="N61" s="32"/>
     </row>
-    <row r="62" spans="1:16" ht="26" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="25"/>
-      <c r="B62" s="43"/>
+      <c r="B62" s="41"/>
       <c r="C62" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D62" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E62" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="F62" s="55"/>
-      <c r="G62" s="55"/>
-      <c r="H62" s="56"/>
+        <v>102</v>
+      </c>
+      <c r="F62" s="36"/>
+      <c r="G62" s="36"/>
+      <c r="H62" s="37"/>
       <c r="I62" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J62" s="32"/>
       <c r="K62" s="32"/>
@@ -3553,21 +3580,21 @@
       <c r="M62" s="32"/>
       <c r="N62" s="32"/>
     </row>
-    <row r="63" spans="1:16" ht="26" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="25"/>
-      <c r="B63" s="43"/>
+      <c r="B63" s="41"/>
       <c r="C63" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D63" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E63" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="F63" s="55"/>
-      <c r="G63" s="55"/>
-      <c r="H63" s="56"/>
+        <v>159</v>
+      </c>
+      <c r="F63" s="36"/>
+      <c r="G63" s="36"/>
+      <c r="H63" s="37"/>
       <c r="I63" s="23" t="s">
         <v>27</v>
       </c>
@@ -3579,23 +3606,23 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="25"/>
-      <c r="B64" s="44" t="s">
-        <v>160</v>
+      <c r="B64" s="53" t="s">
+        <v>158</v>
       </c>
       <c r="C64" s="24" t="s">
         <v>34</v>
       </c>
       <c r="D64" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E64" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="F64" s="55"/>
-      <c r="G64" s="55"/>
-      <c r="H64" s="56"/>
+        <v>164</v>
+      </c>
+      <c r="F64" s="36"/>
+      <c r="G64" s="36"/>
+      <c r="H64" s="37"/>
       <c r="I64" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J64" s="32"/>
       <c r="K64" s="32"/>
@@ -3605,21 +3632,21 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" s="25"/>
-      <c r="B65" s="45"/>
+      <c r="B65" s="54"/>
       <c r="C65" s="24" t="s">
         <v>32</v>
       </c>
       <c r="D65" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E65" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="F65" s="55"/>
-      <c r="G65" s="55"/>
-      <c r="H65" s="56"/>
+        <v>165</v>
+      </c>
+      <c r="F65" s="36"/>
+      <c r="G65" s="36"/>
+      <c r="H65" s="37"/>
       <c r="I65" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J65" s="32"/>
       <c r="K65" s="32"/>
@@ -3631,19 +3658,19 @@
     </row>
     <row r="66" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="25"/>
-      <c r="B66" s="45"/>
+      <c r="B66" s="54"/>
       <c r="C66" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D66" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E66" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="F66" s="55"/>
-      <c r="G66" s="55"/>
-      <c r="H66" s="56"/>
+        <v>168</v>
+      </c>
+      <c r="F66" s="36"/>
+      <c r="G66" s="36"/>
+      <c r="H66" s="37"/>
       <c r="I66" s="23" t="s">
         <v>26</v>
       </c>
@@ -3655,21 +3682,21 @@
     </row>
     <row r="67" spans="1:16" ht="26" x14ac:dyDescent="0.2">
       <c r="A67" s="25"/>
-      <c r="B67" s="45"/>
+      <c r="B67" s="54"/>
       <c r="C67" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="D67" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E67" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="D67" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="E67" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="F67" s="55"/>
-      <c r="G67" s="55"/>
-      <c r="H67" s="56"/>
+      <c r="F67" s="36"/>
+      <c r="G67" s="36"/>
+      <c r="H67" s="37"/>
       <c r="I67" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J67" s="32"/>
       <c r="K67" s="32"/>
@@ -3679,21 +3706,21 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" s="25"/>
-      <c r="B68" s="45"/>
+      <c r="B68" s="54"/>
       <c r="C68" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E68" s="23" t="s">
-        <v>223</v>
-      </c>
-      <c r="F68" s="55"/>
-      <c r="G68" s="55"/>
-      <c r="H68" s="56"/>
+        <v>221</v>
+      </c>
+      <c r="F68" s="36"/>
+      <c r="G68" s="36"/>
+      <c r="H68" s="37"/>
       <c r="I68" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J68" s="32"/>
       <c r="K68" s="32"/>
@@ -3703,21 +3730,21 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" s="25"/>
-      <c r="B69" s="45"/>
+      <c r="B69" s="54"/>
       <c r="C69" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D69" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E69" s="23" t="s">
-        <v>222</v>
-      </c>
-      <c r="F69" s="55"/>
-      <c r="G69" s="55"/>
-      <c r="H69" s="56"/>
+        <v>220</v>
+      </c>
+      <c r="F69" s="36"/>
+      <c r="G69" s="36"/>
+      <c r="H69" s="37"/>
       <c r="I69" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J69" s="32"/>
       <c r="K69" s="32"/>
@@ -3727,21 +3754,21 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" s="25"/>
-      <c r="B70" s="45"/>
+      <c r="B70" s="54"/>
       <c r="C70" s="24" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E70" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="F70" s="55"/>
-      <c r="G70" s="55"/>
-      <c r="H70" s="56"/>
+        <v>194</v>
+      </c>
+      <c r="F70" s="36"/>
+      <c r="G70" s="36"/>
+      <c r="H70" s="37"/>
       <c r="I70" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J70" s="32"/>
       <c r="K70" s="32"/>
@@ -3751,21 +3778,21 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" s="25"/>
-      <c r="B71" s="45"/>
+      <c r="B71" s="54"/>
       <c r="C71" s="24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D71" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E71" s="23" t="s">
-        <v>225</v>
-      </c>
-      <c r="F71" s="55"/>
-      <c r="G71" s="55"/>
-      <c r="H71" s="56"/>
+        <v>223</v>
+      </c>
+      <c r="F71" s="36"/>
+      <c r="G71" s="36"/>
+      <c r="H71" s="37"/>
       <c r="I71" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J71" s="32"/>
       <c r="K71" s="32"/>
@@ -3775,21 +3802,21 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" s="25"/>
-      <c r="B72" s="45"/>
+      <c r="B72" s="54"/>
       <c r="C72" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D72" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E72" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="F72" s="55"/>
-      <c r="G72" s="55"/>
-      <c r="H72" s="56"/>
+        <v>175</v>
+      </c>
+      <c r="F72" s="36"/>
+      <c r="G72" s="36"/>
+      <c r="H72" s="37"/>
       <c r="I72" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J72" s="32"/>
       <c r="K72" s="32"/>
@@ -3799,21 +3826,21 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" s="25"/>
-      <c r="B73" s="45"/>
+      <c r="B73" s="54"/>
       <c r="C73" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D73" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E73" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F73" s="55"/>
-      <c r="G73" s="55"/>
-      <c r="H73" s="56"/>
+        <v>214</v>
+      </c>
+      <c r="F73" s="36"/>
+      <c r="G73" s="36"/>
+      <c r="H73" s="37"/>
       <c r="I73" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J73" s="32"/>
       <c r="K73" s="32"/>
@@ -3823,21 +3850,21 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" s="25"/>
-      <c r="B74" s="45"/>
+      <c r="B74" s="54"/>
       <c r="C74" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D74" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E74" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="F74" s="55"/>
-      <c r="G74" s="55"/>
-      <c r="H74" s="56"/>
+        <v>176</v>
+      </c>
+      <c r="F74" s="36"/>
+      <c r="G74" s="36"/>
+      <c r="H74" s="37"/>
       <c r="I74" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J74" s="32"/>
       <c r="K74" s="32"/>
@@ -3847,21 +3874,21 @@
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" s="25"/>
-      <c r="B75" s="45"/>
+      <c r="B75" s="54"/>
       <c r="C75" s="24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D75" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E75" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="F75" s="55"/>
-      <c r="G75" s="55"/>
-      <c r="H75" s="56"/>
+        <v>177</v>
+      </c>
+      <c r="F75" s="36"/>
+      <c r="G75" s="36"/>
+      <c r="H75" s="37"/>
       <c r="I75" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J75" s="32"/>
       <c r="K75" s="32"/>
@@ -3871,21 +3898,21 @@
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" s="25"/>
-      <c r="B76" s="45"/>
+      <c r="B76" s="54"/>
       <c r="C76" s="23" t="s">
         <v>40</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E76" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="F76" s="55"/>
-      <c r="G76" s="55"/>
-      <c r="H76" s="56"/>
+        <v>103</v>
+      </c>
+      <c r="F76" s="36"/>
+      <c r="G76" s="36"/>
+      <c r="H76" s="37"/>
       <c r="I76" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J76" s="32"/>
       <c r="K76" s="32"/>
@@ -3895,21 +3922,21 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" s="25"/>
-      <c r="B77" s="45"/>
+      <c r="B77" s="54"/>
       <c r="C77" s="24" t="s">
         <v>41</v>
       </c>
       <c r="D77" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E77" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="F77" s="55"/>
-      <c r="G77" s="55"/>
-      <c r="H77" s="56"/>
+        <v>178</v>
+      </c>
+      <c r="F77" s="36"/>
+      <c r="G77" s="36"/>
+      <c r="H77" s="37"/>
       <c r="I77" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J77" s="32"/>
       <c r="K77" s="32"/>
@@ -3919,21 +3946,21 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" s="25"/>
-      <c r="B78" s="45"/>
+      <c r="B78" s="54"/>
       <c r="C78" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D78" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E78" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="F78" s="55"/>
-      <c r="G78" s="55"/>
-      <c r="H78" s="56"/>
+        <v>179</v>
+      </c>
+      <c r="F78" s="36"/>
+      <c r="G78" s="36"/>
+      <c r="H78" s="37"/>
       <c r="I78" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J78" s="32"/>
       <c r="K78" s="32"/>
@@ -3941,21 +3968,21 @@
       <c r="M78" s="32"/>
       <c r="N78" s="32"/>
     </row>
-    <row r="79" spans="1:16" ht="26" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79" s="25"/>
-      <c r="B79" s="46"/>
+      <c r="B79" s="55"/>
       <c r="C79" s="33" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D79" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E79" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="F79" s="55"/>
-      <c r="G79" s="55"/>
-      <c r="H79" s="56"/>
+        <v>155</v>
+      </c>
+      <c r="F79" s="36"/>
+      <c r="G79" s="36"/>
+      <c r="H79" s="37"/>
       <c r="I79" s="23" t="s">
         <v>27</v>
       </c>
@@ -3966,23 +3993,23 @@
       <c r="N79" s="32"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B80" s="39" t="s">
+      <c r="B80" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="C80" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="C80" s="30" t="s">
-        <v>76</v>
-      </c>
       <c r="D80" s="32" t="s">
         <v>24</v>
       </c>
       <c r="E80" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F80" s="56"/>
-      <c r="G80" s="56"/>
-      <c r="H80" s="56"/>
+      <c r="F80" s="37"/>
+      <c r="G80" s="37"/>
+      <c r="H80" s="37"/>
       <c r="I80" s="23" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J80" s="28"/>
       <c r="K80" s="28"/>
@@ -3991,9 +4018,9 @@
       <c r="N80" s="24"/>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B81" s="40"/>
+      <c r="B81" s="50"/>
       <c r="C81" s="30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D81" s="32" t="s">
         <v>24</v>
@@ -4001,11 +4028,11 @@
       <c r="E81" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F81" s="56"/>
-      <c r="G81" s="56"/>
-      <c r="H81" s="56"/>
+      <c r="F81" s="37"/>
+      <c r="G81" s="37"/>
+      <c r="H81" s="37"/>
       <c r="I81" s="23" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J81" s="28"/>
       <c r="K81" s="28"/>
@@ -4014,9 +4041,9 @@
       <c r="N81" s="24"/>
     </row>
     <row r="82" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B82" s="40"/>
+      <c r="B82" s="50"/>
       <c r="C82" s="30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D82" s="32" t="s">
         <v>24</v>
@@ -4024,11 +4051,11 @@
       <c r="E82" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F82" s="56"/>
-      <c r="G82" s="56"/>
-      <c r="H82" s="56"/>
+      <c r="F82" s="37"/>
+      <c r="G82" s="37"/>
+      <c r="H82" s="37"/>
       <c r="I82" s="23" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J82" s="28"/>
       <c r="K82" s="28"/>
@@ -4037,9 +4064,9 @@
       <c r="N82" s="24"/>
     </row>
     <row r="83" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B83" s="40"/>
+      <c r="B83" s="50"/>
       <c r="C83" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D83" s="32" t="s">
         <v>24</v>
@@ -4047,11 +4074,11 @@
       <c r="E83" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F83" s="56"/>
-      <c r="G83" s="56"/>
-      <c r="H83" s="56"/>
+      <c r="F83" s="37"/>
+      <c r="G83" s="37"/>
+      <c r="H83" s="37"/>
       <c r="I83" s="23" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J83" s="28"/>
       <c r="K83" s="28"/>
@@ -4060,9 +4087,9 @@
       <c r="N83" s="24"/>
     </row>
     <row r="84" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B84" s="41"/>
+      <c r="B84" s="51"/>
       <c r="C84" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D84" s="32" t="s">
         <v>24</v>
@@ -4070,11 +4097,11 @@
       <c r="E84" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F84" s="56"/>
-      <c r="G84" s="56"/>
-      <c r="H84" s="56"/>
+      <c r="F84" s="37"/>
+      <c r="G84" s="37"/>
+      <c r="H84" s="37"/>
       <c r="I84" s="23" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J84" s="28"/>
       <c r="K84" s="28"/>
@@ -4083,23 +4110,23 @@
       <c r="N84" s="24"/>
     </row>
     <row r="85" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B85" s="34" t="s">
-        <v>81</v>
+      <c r="B85" s="42" t="s">
+        <v>80</v>
       </c>
       <c r="C85" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D85" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E85" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="F85" s="55"/>
-      <c r="G85" s="55"/>
-      <c r="H85" s="56"/>
+        <v>194</v>
+      </c>
+      <c r="F85" s="36"/>
+      <c r="G85" s="36"/>
+      <c r="H85" s="37"/>
       <c r="I85" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J85" s="28"/>
       <c r="K85" s="28"/>
@@ -4107,22 +4134,22 @@
       <c r="M85" s="24"/>
       <c r="N85" s="24"/>
     </row>
-    <row r="86" spans="2:14" ht="52" x14ac:dyDescent="0.2">
-      <c r="B86" s="35"/>
+    <row r="86" spans="2:14" ht="39" x14ac:dyDescent="0.2">
+      <c r="B86" s="43"/>
       <c r="C86" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D86" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E86" s="23" t="s">
-        <v>205</v>
-      </c>
-      <c r="F86" s="55"/>
-      <c r="G86" s="55"/>
-      <c r="H86" s="56"/>
+        <v>203</v>
+      </c>
+      <c r="F86" s="36"/>
+      <c r="G86" s="36"/>
+      <c r="H86" s="37"/>
       <c r="I86" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J86" s="28"/>
       <c r="K86" s="28"/>
@@ -4131,21 +4158,21 @@
       <c r="N86" s="24"/>
     </row>
     <row r="87" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B87" s="35"/>
+      <c r="B87" s="43"/>
       <c r="C87" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="D87" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="D87" s="21" t="s">
-        <v>126</v>
-      </c>
       <c r="E87" s="23" t="s">
-        <v>206</v>
-      </c>
-      <c r="F87" s="55"/>
-      <c r="G87" s="55"/>
-      <c r="H87" s="56"/>
+        <v>204</v>
+      </c>
+      <c r="F87" s="36"/>
+      <c r="G87" s="36"/>
+      <c r="H87" s="37"/>
       <c r="I87" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J87" s="28"/>
       <c r="K87" s="28"/>
@@ -4154,21 +4181,21 @@
       <c r="N87" s="24"/>
     </row>
     <row r="88" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B88" s="35"/>
+      <c r="B88" s="43"/>
       <c r="C88" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D88" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E88" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="F88" s="55"/>
-      <c r="G88" s="55"/>
-      <c r="H88" s="56"/>
+        <v>175</v>
+      </c>
+      <c r="F88" s="36"/>
+      <c r="G88" s="36"/>
+      <c r="H88" s="37"/>
       <c r="I88" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J88" s="28"/>
       <c r="K88" s="28"/>
@@ -4176,22 +4203,22 @@
       <c r="M88" s="24"/>
       <c r="N88" s="24"/>
     </row>
-    <row r="89" spans="2:14" ht="104" x14ac:dyDescent="0.2">
-      <c r="B89" s="35"/>
+    <row r="89" spans="2:14" ht="65" x14ac:dyDescent="0.2">
+      <c r="B89" s="43"/>
       <c r="C89" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D89" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E89" s="23" t="s">
-        <v>207</v>
-      </c>
-      <c r="F89" s="55"/>
-      <c r="G89" s="55"/>
-      <c r="H89" s="56"/>
+        <v>205</v>
+      </c>
+      <c r="F89" s="36"/>
+      <c r="G89" s="36"/>
+      <c r="H89" s="37"/>
       <c r="I89" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J89" s="32"/>
       <c r="K89" s="32"/>
@@ -4199,20 +4226,20 @@
       <c r="M89" s="24"/>
       <c r="N89" s="24"/>
     </row>
-    <row r="90" spans="2:14" ht="26" x14ac:dyDescent="0.2">
-      <c r="B90" s="35"/>
+    <row r="90" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B90" s="43"/>
       <c r="C90" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D90" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E90" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="F90" s="55"/>
-      <c r="G90" s="55"/>
-      <c r="H90" s="56"/>
+        <v>200</v>
+      </c>
+      <c r="F90" s="36"/>
+      <c r="G90" s="36"/>
+      <c r="H90" s="37"/>
       <c r="I90" s="23" t="s">
         <v>27</v>
       </c>
@@ -4223,23 +4250,23 @@
       <c r="N90" s="24"/>
     </row>
     <row r="91" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B91" s="34" t="s">
-        <v>85</v>
+      <c r="B91" s="42" t="s">
+        <v>84</v>
       </c>
       <c r="C91" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D91" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E91" s="23" t="s">
-        <v>208</v>
-      </c>
-      <c r="F91" s="55"/>
-      <c r="G91" s="55"/>
-      <c r="H91" s="56"/>
+        <v>206</v>
+      </c>
+      <c r="F91" s="36"/>
+      <c r="G91" s="36"/>
+      <c r="H91" s="37"/>
       <c r="I91" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J91" s="28"/>
       <c r="K91" s="28"/>
@@ -4248,21 +4275,21 @@
       <c r="N91" s="24"/>
     </row>
     <row r="92" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B92" s="35"/>
+      <c r="B92" s="43"/>
       <c r="C92" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D92" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E92" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="F92" s="55"/>
-      <c r="G92" s="55"/>
-      <c r="H92" s="56"/>
+        <v>194</v>
+      </c>
+      <c r="F92" s="36"/>
+      <c r="G92" s="36"/>
+      <c r="H92" s="37"/>
       <c r="I92" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J92" s="28"/>
       <c r="K92" s="28"/>
@@ -4271,21 +4298,21 @@
       <c r="N92" s="24"/>
     </row>
     <row r="93" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B93" s="35"/>
+      <c r="B93" s="43"/>
       <c r="C93" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D93" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E93" s="23" t="s">
-        <v>209</v>
-      </c>
-      <c r="F93" s="55"/>
-      <c r="G93" s="55"/>
-      <c r="H93" s="56"/>
+        <v>207</v>
+      </c>
+      <c r="F93" s="36"/>
+      <c r="G93" s="36"/>
+      <c r="H93" s="37"/>
       <c r="I93" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J93" s="28"/>
       <c r="K93" s="28"/>
@@ -4293,20 +4320,20 @@
       <c r="M93" s="24"/>
       <c r="N93" s="24"/>
     </row>
-    <row r="94" spans="2:14" ht="26" x14ac:dyDescent="0.2">
-      <c r="B94" s="35"/>
+    <row r="94" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B94" s="43"/>
       <c r="C94" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D94" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E94" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="F94" s="55"/>
-      <c r="G94" s="55"/>
-      <c r="H94" s="56"/>
+        <v>208</v>
+      </c>
+      <c r="F94" s="36"/>
+      <c r="G94" s="36"/>
+      <c r="H94" s="37"/>
       <c r="I94" s="23" t="s">
         <v>27</v>
       </c>
@@ -4317,19 +4344,19 @@
       <c r="N94" s="24"/>
     </row>
     <row r="95" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B95" s="36"/>
+      <c r="B95" s="44"/>
       <c r="C95" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D95" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E95" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="F95" s="55"/>
-      <c r="G95" s="55"/>
-      <c r="H95" s="56"/>
+        <v>199</v>
+      </c>
+      <c r="F95" s="36"/>
+      <c r="G95" s="36"/>
+      <c r="H95" s="37"/>
       <c r="I95" s="23" t="s">
         <v>27</v>
       </c>
@@ -4339,24 +4366,24 @@
       <c r="M95" s="24"/>
       <c r="N95" s="24"/>
     </row>
-    <row r="96" spans="2:14" ht="52" x14ac:dyDescent="0.2">
-      <c r="B96" s="34" t="s">
+    <row r="96" spans="2:14" ht="39" x14ac:dyDescent="0.2">
+      <c r="B96" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C96" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="C96" s="24" t="s">
-        <v>91</v>
-      </c>
       <c r="D96" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E96" s="24" t="s">
-        <v>211</v>
-      </c>
-      <c r="F96" s="57"/>
-      <c r="G96" s="57"/>
-      <c r="H96" s="56"/>
+        <v>209</v>
+      </c>
+      <c r="F96" s="38"/>
+      <c r="G96" s="38"/>
+      <c r="H96" s="37"/>
       <c r="I96" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J96" s="28"/>
       <c r="K96" s="28"/>
@@ -4365,21 +4392,21 @@
       <c r="N96" s="24"/>
     </row>
     <row r="97" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B97" s="35"/>
+      <c r="B97" s="43"/>
       <c r="C97" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D97" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E97" s="23" t="s">
-        <v>212</v>
-      </c>
-      <c r="F97" s="55"/>
-      <c r="G97" s="55"/>
-      <c r="H97" s="56"/>
+        <v>210</v>
+      </c>
+      <c r="F97" s="36"/>
+      <c r="G97" s="36"/>
+      <c r="H97" s="37"/>
       <c r="I97" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J97" s="28"/>
       <c r="K97" s="28"/>
@@ -4387,22 +4414,22 @@
       <c r="M97" s="24"/>
       <c r="N97" s="24"/>
     </row>
-    <row r="98" spans="2:14" ht="52" x14ac:dyDescent="0.2">
-      <c r="B98" s="35"/>
+    <row r="98" spans="2:14" ht="39" x14ac:dyDescent="0.2">
+      <c r="B98" s="43"/>
       <c r="C98" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D98" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E98" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="F98" s="55"/>
-      <c r="G98" s="55"/>
-      <c r="H98" s="56"/>
+        <v>211</v>
+      </c>
+      <c r="F98" s="36"/>
+      <c r="G98" s="36"/>
+      <c r="H98" s="37"/>
       <c r="I98" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J98" s="28"/>
       <c r="K98" s="28"/>
@@ -4410,20 +4437,20 @@
       <c r="M98" s="24"/>
       <c r="N98" s="24"/>
     </row>
-    <row r="99" spans="2:14" ht="26" x14ac:dyDescent="0.2">
-      <c r="B99" s="35"/>
+    <row r="99" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B99" s="43"/>
       <c r="C99" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D99" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E99" s="23" t="s">
-        <v>214</v>
-      </c>
-      <c r="F99" s="55"/>
-      <c r="G99" s="55"/>
-      <c r="H99" s="56"/>
+        <v>212</v>
+      </c>
+      <c r="F99" s="36"/>
+      <c r="G99" s="36"/>
+      <c r="H99" s="37"/>
       <c r="I99" s="23" t="s">
         <v>27</v>
       </c>
@@ -4433,20 +4460,20 @@
       <c r="M99" s="24"/>
       <c r="N99" s="24"/>
     </row>
-    <row r="100" spans="2:14" ht="26" x14ac:dyDescent="0.2">
-      <c r="B100" s="36"/>
+    <row r="100" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B100" s="44"/>
       <c r="C100" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D100" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E100" s="23" t="s">
-        <v>200</v>
-      </c>
-      <c r="F100" s="55"/>
-      <c r="G100" s="55"/>
-      <c r="H100" s="56"/>
+        <v>198</v>
+      </c>
+      <c r="F100" s="36"/>
+      <c r="G100" s="36"/>
+      <c r="H100" s="37"/>
       <c r="I100" s="23" t="s">
         <v>27</v>
       </c>
@@ -4456,22 +4483,22 @@
       <c r="M100" s="24"/>
       <c r="N100" s="24"/>
     </row>
-    <row r="101" spans="2:14" ht="39" x14ac:dyDescent="0.2">
-      <c r="B101" s="34" t="s">
-        <v>203</v>
+    <row r="101" spans="2:14" ht="26" x14ac:dyDescent="0.2">
+      <c r="B101" s="42" t="s">
+        <v>201</v>
       </c>
       <c r="C101" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D101" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E101" s="32" t="s">
-        <v>215</v>
-      </c>
-      <c r="F101" s="56"/>
-      <c r="G101" s="56"/>
-      <c r="H101" s="56"/>
+        <v>213</v>
+      </c>
+      <c r="F101" s="37"/>
+      <c r="G101" s="37"/>
+      <c r="H101" s="37"/>
       <c r="I101" s="24" t="s">
         <v>26</v>
       </c>
@@ -4482,21 +4509,21 @@
       <c r="N101" s="24"/>
     </row>
     <row r="102" spans="2:14" ht="26" x14ac:dyDescent="0.2">
-      <c r="B102" s="35"/>
+      <c r="B102" s="43"/>
       <c r="C102" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D102" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E102" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F102" s="55"/>
-      <c r="G102" s="55"/>
-      <c r="H102" s="56"/>
+        <v>214</v>
+      </c>
+      <c r="F102" s="36"/>
+      <c r="G102" s="36"/>
+      <c r="H102" s="37"/>
       <c r="I102" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J102" s="28"/>
       <c r="K102" s="28"/>
@@ -4504,20 +4531,20 @@
       <c r="M102" s="24"/>
       <c r="N102" s="24"/>
     </row>
-    <row r="103" spans="2:14" ht="26" x14ac:dyDescent="0.2">
-      <c r="B103" s="35"/>
+    <row r="103" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B103" s="43"/>
       <c r="C103" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D103" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E103" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F103" s="55"/>
-      <c r="G103" s="55"/>
-      <c r="H103" s="56"/>
+        <v>215</v>
+      </c>
+      <c r="F103" s="36"/>
+      <c r="G103" s="36"/>
+      <c r="H103" s="37"/>
       <c r="I103" s="24" t="s">
         <v>27</v>
       </c>
@@ -4527,20 +4554,20 @@
       <c r="M103" s="24"/>
       <c r="N103" s="24"/>
     </row>
-    <row r="104" spans="2:14" ht="26" x14ac:dyDescent="0.2">
-      <c r="B104" s="36"/>
+    <row r="104" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B104" s="44"/>
       <c r="C104" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D104" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E104" s="24" t="s">
-        <v>199</v>
-      </c>
-      <c r="F104" s="57"/>
-      <c r="G104" s="57"/>
-      <c r="H104" s="56"/>
+        <v>197</v>
+      </c>
+      <c r="F104" s="38"/>
+      <c r="G104" s="38"/>
+      <c r="H104" s="37"/>
       <c r="I104" s="23" t="s">
         <v>27</v>
       </c>
@@ -4551,23 +4578,23 @@
       <c r="N104" s="24"/>
     </row>
     <row r="105" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B105" s="34" t="s">
-        <v>204</v>
+      <c r="B105" s="42" t="s">
+        <v>202</v>
       </c>
       <c r="C105" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D105" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E105" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F105" s="55"/>
-      <c r="G105" s="55"/>
-      <c r="H105" s="56"/>
+        <v>216</v>
+      </c>
+      <c r="F105" s="36"/>
+      <c r="G105" s="36"/>
+      <c r="H105" s="37"/>
       <c r="I105" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J105" s="28"/>
       <c r="K105" s="28"/>
@@ -4575,22 +4602,22 @@
       <c r="M105" s="24"/>
       <c r="N105" s="24"/>
     </row>
-    <row r="106" spans="2:14" ht="26" x14ac:dyDescent="0.2">
-      <c r="B106" s="35"/>
+    <row r="106" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B106" s="43"/>
       <c r="C106" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D106" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E106" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F106" s="55"/>
-      <c r="G106" s="55"/>
-      <c r="H106" s="56"/>
+        <v>217</v>
+      </c>
+      <c r="F106" s="36"/>
+      <c r="G106" s="36"/>
+      <c r="H106" s="37"/>
       <c r="I106" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J106" s="28"/>
       <c r="K106" s="28"/>
@@ -4599,21 +4626,21 @@
       <c r="N106" s="24"/>
     </row>
     <row r="107" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B107" s="35"/>
+      <c r="B107" s="43"/>
       <c r="C107" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D107" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E107" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="F107" s="55"/>
-      <c r="G107" s="55"/>
-      <c r="H107" s="56"/>
+        <v>218</v>
+      </c>
+      <c r="F107" s="36"/>
+      <c r="G107" s="36"/>
+      <c r="H107" s="37"/>
       <c r="I107" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J107" s="28"/>
       <c r="K107" s="28"/>
@@ -4621,22 +4648,22 @@
       <c r="M107" s="24"/>
       <c r="N107" s="24"/>
     </row>
-    <row r="108" spans="2:14" ht="26" x14ac:dyDescent="0.2">
-      <c r="B108" s="35"/>
+    <row r="108" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B108" s="43"/>
       <c r="C108" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D108" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E108" s="23" t="s">
-        <v>221</v>
-      </c>
-      <c r="F108" s="55"/>
-      <c r="G108" s="55"/>
-      <c r="H108" s="56"/>
+        <v>219</v>
+      </c>
+      <c r="F108" s="36"/>
+      <c r="G108" s="36"/>
+      <c r="H108" s="37"/>
       <c r="I108" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J108" s="28"/>
       <c r="K108" s="28"/>
@@ -4645,19 +4672,19 @@
       <c r="N108" s="24"/>
     </row>
     <row r="109" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B109" s="36"/>
+      <c r="B109" s="44"/>
       <c r="C109" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D109" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E109" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F109" s="55"/>
-      <c r="G109" s="55"/>
-      <c r="H109" s="56"/>
+      <c r="F109" s="36"/>
+      <c r="G109" s="36"/>
+      <c r="H109" s="37"/>
       <c r="I109" s="23" t="s">
         <v>27</v>
       </c>
@@ -4669,6 +4696,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B105:B109"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B80:B84"/>
+    <mergeCell ref="B85:B90"/>
+    <mergeCell ref="B91:B95"/>
+    <mergeCell ref="B58:B63"/>
+    <mergeCell ref="B64:B79"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="B96:B100"/>
     <mergeCell ref="B101:B104"/>
@@ -4677,14 +4712,6 @@
     <mergeCell ref="B43:B50"/>
     <mergeCell ref="B51:B53"/>
     <mergeCell ref="B10:B27"/>
-    <mergeCell ref="B105:B109"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B80:B84"/>
-    <mergeCell ref="B85:B90"/>
-    <mergeCell ref="B91:B95"/>
-    <mergeCell ref="B58:B63"/>
-    <mergeCell ref="B64:B79"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="1" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4706,29 +4733,29 @@
   </sheetPr>
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.796875" style="17" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="17" customWidth="1"/>
     <col min="3" max="3" width="33" style="17" customWidth="1"/>
-    <col min="4" max="4" width="23.59765625" style="26" customWidth="1"/>
-    <col min="5" max="8" width="20.3984375" style="16" customWidth="1"/>
-    <col min="9" max="9" width="13.3984375" style="16" customWidth="1"/>
-    <col min="10" max="10" width="10.19921875" style="16" customWidth="1"/>
-    <col min="11" max="11" width="15.3984375" style="16" customWidth="1"/>
-    <col min="12" max="12" width="12.59765625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="26" customWidth="1"/>
+    <col min="5" max="8" width="20.33203125" style="16" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="16" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" style="16" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" style="16" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" style="16" customWidth="1"/>
     <col min="13" max="13" width="14" style="17" customWidth="1"/>
-    <col min="14" max="14" width="24.19921875" style="17" customWidth="1"/>
-    <col min="15" max="15" width="21.59765625" style="17" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="24.1640625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="21.6640625" style="17" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="13" style="16" hidden="1" customWidth="1"/>
-    <col min="17" max="1028" width="21.59765625" customWidth="1"/>
+    <col min="17" max="1028" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="20" customFormat="1" ht="39" x14ac:dyDescent="0.2">
@@ -4736,25 +4763,25 @@
         <v>13</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E1" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="H1" s="27" t="s">
         <v>234</v>
       </c>
-      <c r="F1" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>237</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>236</v>
-      </c>
       <c r="I1" s="18" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J1" s="18"/>
       <c r="K1" s="18"/>
@@ -4772,11 +4799,11 @@
     </row>
     <row r="2" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2"/>
-      <c r="B2" s="50" t="s">
-        <v>231</v>
-      </c>
-      <c r="C2" s="53" t="s">
-        <v>232</v>
+      <c r="B2" s="56" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>230</v>
       </c>
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
@@ -4793,9 +4820,9 @@
     </row>
     <row r="3" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3"/>
-      <c r="B3" s="51"/>
+      <c r="B3" s="57"/>
       <c r="C3" s="24" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
@@ -4812,9 +4839,9 @@
     </row>
     <row r="4" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4"/>
-      <c r="B4" s="51"/>
+      <c r="B4" s="57"/>
       <c r="C4" s="24" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
@@ -4831,9 +4858,9 @@
     </row>
     <row r="5" spans="1:16" s="17" customFormat="1" ht="26" x14ac:dyDescent="0.2">
       <c r="A5"/>
-      <c r="B5" s="51"/>
+      <c r="B5" s="57"/>
       <c r="C5" s="24" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D5" s="24"/>
       <c r="E5" s="24"/>
@@ -4850,9 +4877,9 @@
     </row>
     <row r="6" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6"/>
-      <c r="B6" s="51"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="24" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
@@ -4869,9 +4896,9 @@
     </row>
     <row r="7" spans="1:16" s="17" customFormat="1" ht="26" x14ac:dyDescent="0.2">
       <c r="A7"/>
-      <c r="B7" s="51"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="24" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
@@ -4888,9 +4915,9 @@
     </row>
     <row r="8" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8"/>
-      <c r="B8" s="51"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="24" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
@@ -4907,9 +4934,9 @@
     </row>
     <row r="9" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9"/>
-      <c r="B9" s="51"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="24" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
@@ -4926,9 +4953,9 @@
     </row>
     <row r="10" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10"/>
-      <c r="B10" s="51"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="24" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
@@ -4945,9 +4972,9 @@
     </row>
     <row r="11" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11"/>
-      <c r="B11" s="51"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="24" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
@@ -4964,9 +4991,9 @@
     </row>
     <row r="12" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12"/>
-      <c r="B12" s="51"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="24" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="24"/>
@@ -4983,9 +5010,9 @@
     </row>
     <row r="13" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="54" t="s">
-        <v>256</v>
+      <c r="B13" s="57"/>
+      <c r="C13" s="35" t="s">
+        <v>254</v>
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
@@ -5002,9 +5029,9 @@
     </row>
     <row r="14" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14"/>
-      <c r="B14" s="51"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="24" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="24"/>
@@ -5021,9 +5048,9 @@
     </row>
     <row r="15" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15"/>
-      <c r="B15" s="51"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
@@ -5038,11 +5065,11 @@
       <c r="N15" s="24"/>
       <c r="P15" s="16"/>
     </row>
-    <row r="16" spans="1:16" s="17" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16"/>
-      <c r="B16" s="51"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
@@ -5059,9 +5086,9 @@
     </row>
     <row r="17" spans="1:16" s="17" customFormat="1" ht="26" x14ac:dyDescent="0.2">
       <c r="A17"/>
-      <c r="B17" s="51"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="24" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="24"/>
@@ -5078,9 +5105,9 @@
     </row>
     <row r="18" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18"/>
-      <c r="B18" s="51"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
@@ -5097,9 +5124,9 @@
     </row>
     <row r="19" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19"/>
-      <c r="B19" s="51"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
@@ -5116,9 +5143,9 @@
     </row>
     <row r="20" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="54" t="s">
-        <v>257</v>
+      <c r="B20" s="57"/>
+      <c r="C20" s="35" t="s">
+        <v>255</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
@@ -5135,9 +5162,9 @@
     </row>
     <row r="21" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21"/>
-      <c r="B21" s="51"/>
+      <c r="B21" s="57"/>
       <c r="C21" s="24" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D21" s="24"/>
       <c r="E21" s="24"/>
@@ -5154,9 +5181,9 @@
     </row>
     <row r="22" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22"/>
-      <c r="B22" s="51"/>
+      <c r="B22" s="57"/>
       <c r="C22" s="24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D22" s="24"/>
       <c r="E22" s="24"/>
@@ -5173,9 +5200,9 @@
     </row>
     <row r="23" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23"/>
-      <c r="B23" s="51"/>
+      <c r="B23" s="57"/>
       <c r="C23" s="24" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
@@ -5192,7 +5219,7 @@
     </row>
     <row r="24" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24"/>
-      <c r="B24" s="51"/>
+      <c r="B24" s="57"/>
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
@@ -5209,7 +5236,7 @@
     </row>
     <row r="25" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25"/>
-      <c r="B25" s="51"/>
+      <c r="B25" s="57"/>
       <c r="C25" s="24"/>
       <c r="D25" s="24"/>
       <c r="E25" s="24"/>
@@ -5226,7 +5253,7 @@
     </row>
     <row r="26" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26"/>
-      <c r="B26" s="51"/>
+      <c r="B26" s="57"/>
       <c r="C26" s="24"/>
       <c r="D26" s="24"/>
       <c r="E26" s="24"/>
@@ -5243,7 +5270,7 @@
     </row>
     <row r="27" spans="1:16" s="17" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27"/>
-      <c r="B27" s="52"/>
+      <c r="B27" s="58"/>
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>

</xml_diff>